<commit_message>
fix roblox experience name normalization to ignore emojis
</commit_message>
<xml_diff>
--- a/data/total_roblox_experiences.xlsx
+++ b/data/total_roblox_experiences.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenwang/Desktop/Makers/HW_Roblox_Weekly_Update/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenwang/Desktop/Makers/Steam_Roblox_Streamlit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF8A792-F0F0-244E-A313-E19CBE18E32E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F3F3A5-ED45-D74D-A48B-9EB4C9F509F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5840" yWindow="1100" windowWidth="23460" windowHeight="18020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2024-07-09" sheetId="3" r:id="rId1"/>
-    <sheet name="2024-07-01" sheetId="1" r:id="rId2"/>
-    <sheet name="2024-06-20" sheetId="2" r:id="rId3"/>
+    <sheet name="2024-07-25" sheetId="4" r:id="rId1"/>
+    <sheet name="2024-07-09" sheetId="3" r:id="rId2"/>
+    <sheet name="2024-07-01" sheetId="1" r:id="rId3"/>
+    <sheet name="2024-06-20" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="654" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="265">
   <si>
     <t>#1</t>
   </si>
@@ -721,6 +722,102 @@
   </si>
   <si>
     <t>Drive World | Twin Atlas</t>
+  </si>
+  <si>
+    <t>Top Experiences 50 on Roblox (Data fetched from RoMonitor as of 01:42 PM EDT, 2024-07-25)</t>
+  </si>
+  <si>
+    <t>[UPD🌗] Anime Defenders</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Adopt Me!</t>
+  </si>
+  <si>
+    <t>@Onett</t>
+  </si>
+  <si>
+    <t>Pet Simulator 99! 💎💸</t>
+  </si>
+  <si>
+    <t>[🏖️EP 76 PART 1] Toilet Tower Defense</t>
+  </si>
+  <si>
+    <t>[UPD4] Gym League</t>
+  </si>
+  <si>
+    <t>Blade Ball</t>
+  </si>
+  <si>
+    <t>BedWars [⭐ Epilogue]</t>
+  </si>
+  <si>
+    <t>[GUIDE] Slap Battles👏</t>
+  </si>
+  <si>
+    <t>[UPD]Metro Life 🏙️ City RP</t>
+  </si>
+  <si>
+    <t>[🚀🌐 WORLD 2 + 📈PATCH] Anime Last Stand</t>
+  </si>
+  <si>
+    <t>Anime Last Stand</t>
+  </si>
+  <si>
+    <t>[UPD 🎉] RIVALS</t>
+  </si>
+  <si>
+    <t>FPS</t>
+  </si>
+  <si>
+    <t>Nosniy Games</t>
+  </si>
+  <si>
+    <t>a dusty trip [🚜BOSS]</t>
+  </si>
+  <si>
+    <t>Pressure</t>
+  </si>
+  <si>
+    <t>Urbanshade: Hadal Division</t>
+  </si>
+  <si>
+    <t>🍄 Creatures of Sonaria 👁️ Survive Kaiju Animals</t>
+  </si>
+  <si>
+    <t>[NEW AUDIS] Driving Empire 🏎️ Car Racing</t>
+  </si>
+  <si>
+    <t>Bayside High School 🍎</t>
+  </si>
+  <si>
+    <t>Double Bandit Studios</t>
+  </si>
+  <si>
+    <t>Livetopia🏛️ Town Hall</t>
+  </si>
+  <si>
+    <t>Baddies 💅</t>
+  </si>
+  <si>
+    <t>Meow Meow Games!</t>
+  </si>
+  <si>
+    <t>[Invictus] War Tycoon</t>
+  </si>
+  <si>
+    <t>Color or Die 🎨</t>
+  </si>
+  <si>
+    <t>BIGworks Games</t>
+  </si>
+  <si>
+    <t>[🔥SEASON 5]Grand Piece Online</t>
+  </si>
+  <si>
+    <t>[BULLET] untitled boxing game🥊</t>
   </si>
 </sst>
 </file>
@@ -1143,11 +1240,2150 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B937581-5BFE-0C43-9A8A-CAE8581C0F34}">
+  <dimension ref="A1:M52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="18.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="3" customWidth="1"/>
+    <col min="6" max="7" width="18.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="2">
+        <v>827765</v>
+      </c>
+      <c r="D3" s="2">
+        <v>51316166265</v>
+      </c>
+      <c r="E3" s="3">
+        <v>43941</v>
+      </c>
+      <c r="F3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0.86620000000000008</v>
+      </c>
+      <c r="I3">
+        <v>16.82</v>
+      </c>
+      <c r="J3" s="2">
+        <v>21382315</v>
+      </c>
+      <c r="K3" s="2">
+        <v>5732974</v>
+      </c>
+      <c r="L3" s="2">
+        <v>885712</v>
+      </c>
+      <c r="M3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="2">
+        <v>633625</v>
+      </c>
+      <c r="D4" s="2">
+        <v>36991820089</v>
+      </c>
+      <c r="E4" s="3">
+        <v>43480</v>
+      </c>
+      <c r="F4" t="s">
+        <v>99</v>
+      </c>
+      <c r="G4" t="s">
+        <v>104</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0.92920000000000003</v>
+      </c>
+      <c r="I4">
+        <v>15.75</v>
+      </c>
+      <c r="J4" s="2">
+        <v>12743641</v>
+      </c>
+      <c r="K4" s="2">
+        <v>7776083</v>
+      </c>
+      <c r="L4" s="2">
+        <v>592807</v>
+      </c>
+      <c r="M4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C5" s="2">
+        <v>303464</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1272936705</v>
+      </c>
+      <c r="E5" s="3">
+        <v>45386</v>
+      </c>
+      <c r="F5" t="s">
+        <v>235</v>
+      </c>
+      <c r="G5" t="s">
+        <v>105</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0.97589999999999999</v>
+      </c>
+      <c r="I5">
+        <v>15.18</v>
+      </c>
+      <c r="J5" s="2">
+        <v>528117</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1579295</v>
+      </c>
+      <c r="L5" s="2">
+        <v>38950</v>
+      </c>
+      <c r="M5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="2">
+        <v>252833</v>
+      </c>
+      <c r="D6" s="2">
+        <v>16181655836</v>
+      </c>
+      <c r="E6" s="3">
+        <v>41656</v>
+      </c>
+      <c r="F6" t="s">
+        <v>100</v>
+      </c>
+      <c r="G6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0.91189999999999993</v>
+      </c>
+      <c r="I6">
+        <v>12.14</v>
+      </c>
+      <c r="J6" s="2">
+        <v>18553679</v>
+      </c>
+      <c r="K6" s="2">
+        <v>7455289</v>
+      </c>
+      <c r="L6" s="2">
+        <v>720008</v>
+      </c>
+      <c r="M6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="2">
+        <v>172326</v>
+      </c>
+      <c r="D7" s="2">
+        <v>6573661453</v>
+      </c>
+      <c r="E7" s="3">
+        <v>44774</v>
+      </c>
+      <c r="F7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7" t="s">
+        <v>108</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0.84050000000000002</v>
+      </c>
+      <c r="I7">
+        <v>9.76</v>
+      </c>
+      <c r="J7" s="2">
+        <v>3432880</v>
+      </c>
+      <c r="K7" s="2">
+        <v>2346564</v>
+      </c>
+      <c r="L7" s="2">
+        <v>445265</v>
+      </c>
+      <c r="M7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="2">
+        <v>167087</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1477368173</v>
+      </c>
+      <c r="E8" s="3">
+        <v>45216</v>
+      </c>
+      <c r="F8" t="s">
+        <v>235</v>
+      </c>
+      <c r="G8" t="s">
+        <v>110</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0.90980000000000005</v>
+      </c>
+      <c r="I8">
+        <v>14.24</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1479142</v>
+      </c>
+      <c r="K8" s="2">
+        <v>829894</v>
+      </c>
+      <c r="L8" s="2">
+        <v>82321</v>
+      </c>
+      <c r="M8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C9" s="2">
+        <v>158091</v>
+      </c>
+      <c r="D9" s="2">
+        <v>36888700900</v>
+      </c>
+      <c r="E9" s="3">
+        <v>42929</v>
+      </c>
+      <c r="F9" t="s">
+        <v>102</v>
+      </c>
+      <c r="G9" t="s">
+        <v>111</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0.83489999999999998</v>
+      </c>
+      <c r="I9">
+        <v>17.260000000000002</v>
+      </c>
+      <c r="J9" s="2">
+        <v>26836545</v>
+      </c>
+      <c r="K9" s="2">
+        <v>7169208</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1417976</v>
+      </c>
+      <c r="M9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="2">
+        <v>139487</v>
+      </c>
+      <c r="D10" s="2">
+        <v>3720779722</v>
+      </c>
+      <c r="E10" s="3">
+        <v>44567</v>
+      </c>
+      <c r="F10" t="s">
+        <v>98</v>
+      </c>
+      <c r="G10" t="s">
+        <v>113</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0.87019999999999997</v>
+      </c>
+      <c r="I10">
+        <v>14.16</v>
+      </c>
+      <c r="J10" s="2">
+        <v>2064240</v>
+      </c>
+      <c r="K10" s="2">
+        <v>577667</v>
+      </c>
+      <c r="L10" s="2">
+        <v>86131</v>
+      </c>
+      <c r="M10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="2">
+        <v>95516</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2769775849</v>
+      </c>
+      <c r="E11" s="3">
+        <v>43179</v>
+      </c>
+      <c r="F11" t="s">
+        <v>99</v>
+      </c>
+      <c r="G11" t="s">
+        <v>237</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0.94950000000000001</v>
+      </c>
+      <c r="I11">
+        <v>33.47</v>
+      </c>
+      <c r="J11" s="2">
+        <v>5867412</v>
+      </c>
+      <c r="K11" s="2">
+        <v>2216853</v>
+      </c>
+      <c r="L11" s="2">
+        <v>117966</v>
+      </c>
+      <c r="M11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C12" s="2">
+        <v>87657</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1267021821</v>
+      </c>
+      <c r="E12" s="3">
+        <v>44597</v>
+      </c>
+      <c r="F12" t="s">
+        <v>235</v>
+      </c>
+      <c r="G12" t="s">
+        <v>109</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0.96450000000000002</v>
+      </c>
+      <c r="I12">
+        <v>42.79</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1330609</v>
+      </c>
+      <c r="K12" s="2">
+        <v>2363491</v>
+      </c>
+      <c r="L12" s="2">
+        <v>86931</v>
+      </c>
+      <c r="M12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="2">
+        <v>69898</v>
+      </c>
+      <c r="D13" s="2">
+        <v>589909368</v>
+      </c>
+      <c r="E13" s="3">
+        <v>45262</v>
+      </c>
+      <c r="F13" t="s">
+        <v>235</v>
+      </c>
+      <c r="G13" t="s">
+        <v>107</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0.87529999999999997</v>
+      </c>
+      <c r="I13">
+        <v>40.909999999999997</v>
+      </c>
+      <c r="J13" s="2">
+        <v>550486</v>
+      </c>
+      <c r="K13" s="2">
+        <v>603815</v>
+      </c>
+      <c r="L13" s="2">
+        <v>86044</v>
+      </c>
+      <c r="M13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C14" s="2">
+        <v>61307</v>
+      </c>
+      <c r="D14" s="2">
+        <v>391606169</v>
+      </c>
+      <c r="E14" s="3">
+        <v>45121</v>
+      </c>
+      <c r="F14" t="s">
+        <v>101</v>
+      </c>
+      <c r="G14" t="s">
+        <v>190</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0.81459999999999999</v>
+      </c>
+      <c r="I14">
+        <v>24.13</v>
+      </c>
+      <c r="J14" s="2">
+        <v>297606</v>
+      </c>
+      <c r="K14" s="2">
+        <v>216262</v>
+      </c>
+      <c r="L14" s="2">
+        <v>49212</v>
+      </c>
+      <c r="M14" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="2">
+        <v>54762</v>
+      </c>
+      <c r="D15" s="2">
+        <v>4502496652</v>
+      </c>
+      <c r="E15" s="3">
+        <v>44721</v>
+      </c>
+      <c r="F15" t="s">
+        <v>100</v>
+      </c>
+      <c r="G15" t="s">
+        <v>116</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0.94480000000000008</v>
+      </c>
+      <c r="I15">
+        <v>10.44</v>
+      </c>
+      <c r="J15" s="2">
+        <v>4927612</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1902924</v>
+      </c>
+      <c r="L15" s="2">
+        <v>111208</v>
+      </c>
+      <c r="M15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C16" s="2">
+        <v>53534</v>
+      </c>
+      <c r="D16" s="2">
+        <v>4507589212</v>
+      </c>
+      <c r="E16" s="3">
+        <v>45093</v>
+      </c>
+      <c r="F16" t="s">
+        <v>235</v>
+      </c>
+      <c r="G16" t="s">
+        <v>112</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0.88349999999999995</v>
+      </c>
+      <c r="I16">
+        <v>13.86</v>
+      </c>
+      <c r="J16" s="2">
+        <v>1021734</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1031014</v>
+      </c>
+      <c r="L16" s="2">
+        <v>135913</v>
+      </c>
+      <c r="M16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="2">
+        <v>50190</v>
+      </c>
+      <c r="D17" s="2">
+        <v>773610625</v>
+      </c>
+      <c r="E17" s="3">
+        <v>45111</v>
+      </c>
+      <c r="F17" t="s">
+        <v>98</v>
+      </c>
+      <c r="G17" t="s">
+        <v>123</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0.92959999999999998</v>
+      </c>
+      <c r="I17">
+        <v>16.04</v>
+      </c>
+      <c r="J17" s="2">
+        <v>888248</v>
+      </c>
+      <c r="K17" s="2">
+        <v>324315</v>
+      </c>
+      <c r="L17" s="2">
+        <v>24545</v>
+      </c>
+      <c r="M17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C18" s="2">
+        <v>48388</v>
+      </c>
+      <c r="D18" s="2">
+        <v>215718350</v>
+      </c>
+      <c r="E18" s="3">
+        <v>45421</v>
+      </c>
+      <c r="F18" t="s">
+        <v>235</v>
+      </c>
+      <c r="G18" t="s">
+        <v>114</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0.98</v>
+      </c>
+      <c r="I18">
+        <v>20.239999999999998</v>
+      </c>
+      <c r="J18" s="2">
+        <v>3584371</v>
+      </c>
+      <c r="K18" s="2">
+        <v>843194</v>
+      </c>
+      <c r="L18" s="2">
+        <v>17196</v>
+      </c>
+      <c r="M18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="2">
+        <v>48037</v>
+      </c>
+      <c r="D19" s="2">
+        <v>8804543457</v>
+      </c>
+      <c r="E19" s="3">
+        <v>41946</v>
+      </c>
+      <c r="F19" t="s">
+        <v>98</v>
+      </c>
+      <c r="G19" t="s">
+        <v>115</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0.88109999999999999</v>
+      </c>
+      <c r="I19">
+        <v>20.84</v>
+      </c>
+      <c r="J19" s="2">
+        <v>13470768</v>
+      </c>
+      <c r="K19" s="2">
+        <v>5231441</v>
+      </c>
+      <c r="L19" s="2">
+        <v>705836</v>
+      </c>
+      <c r="M19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="2">
+        <v>46098</v>
+      </c>
+      <c r="D20" s="2">
+        <v>2494432307</v>
+      </c>
+      <c r="E20" s="3">
+        <v>44380</v>
+      </c>
+      <c r="F20" t="s">
+        <v>164</v>
+      </c>
+      <c r="G20" t="s">
+        <v>122</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0.91359999999999997</v>
+      </c>
+      <c r="I20">
+        <v>12.22</v>
+      </c>
+      <c r="J20" s="2">
+        <v>3190637</v>
+      </c>
+      <c r="K20" s="2">
+        <v>1211958</v>
+      </c>
+      <c r="L20" s="2">
+        <v>114626</v>
+      </c>
+      <c r="M20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="C21" s="2">
+        <v>44948</v>
+      </c>
+      <c r="D21" s="2">
+        <v>4014892454</v>
+      </c>
+      <c r="E21" s="3">
+        <v>45093</v>
+      </c>
+      <c r="F21" t="s">
+        <v>101</v>
+      </c>
+      <c r="G21" t="s">
+        <v>117</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0.93629999999999991</v>
+      </c>
+      <c r="I21">
+        <v>11.33</v>
+      </c>
+      <c r="J21" s="2">
+        <v>9129525</v>
+      </c>
+      <c r="K21" s="2">
+        <v>6022825</v>
+      </c>
+      <c r="L21" s="2">
+        <v>409479</v>
+      </c>
+      <c r="M21" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C22" s="2">
+        <v>44349</v>
+      </c>
+      <c r="D22" s="2">
+        <v>9337871354</v>
+      </c>
+      <c r="E22" s="3">
+        <v>44342</v>
+      </c>
+      <c r="F22" t="s">
+        <v>101</v>
+      </c>
+      <c r="G22" t="s">
+        <v>118</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0.8256</v>
+      </c>
+      <c r="I22">
+        <v>13.26</v>
+      </c>
+      <c r="J22" s="2">
+        <v>4149134</v>
+      </c>
+      <c r="K22" s="2">
+        <v>2122967</v>
+      </c>
+      <c r="L22" s="2">
+        <v>448446</v>
+      </c>
+      <c r="M22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C23" s="2">
+        <v>45225</v>
+      </c>
+      <c r="D23" s="2">
+        <v>9337972666</v>
+      </c>
+      <c r="E23" s="3">
+        <v>44342</v>
+      </c>
+      <c r="F23" t="s">
+        <v>101</v>
+      </c>
+      <c r="G23" t="s">
+        <v>118</v>
+      </c>
+      <c r="H23" s="4">
+        <v>0.8256</v>
+      </c>
+      <c r="I23">
+        <v>13.26</v>
+      </c>
+      <c r="J23" s="2">
+        <v>4149151</v>
+      </c>
+      <c r="K23" s="2">
+        <v>2122989</v>
+      </c>
+      <c r="L23" s="2">
+        <v>448460</v>
+      </c>
+      <c r="M23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="2">
+        <v>40416</v>
+      </c>
+      <c r="D24" s="2">
+        <v>3912026455</v>
+      </c>
+      <c r="E24" s="3">
+        <v>42676</v>
+      </c>
+      <c r="F24" t="s">
+        <v>99</v>
+      </c>
+      <c r="G24" t="s">
+        <v>124</v>
+      </c>
+      <c r="H24" s="4">
+        <v>0.93069999999999997</v>
+      </c>
+      <c r="I24">
+        <v>20.32</v>
+      </c>
+      <c r="J24" s="2">
+        <v>7526608</v>
+      </c>
+      <c r="K24" s="2">
+        <v>2959126</v>
+      </c>
+      <c r="L24" s="2">
+        <v>220503</v>
+      </c>
+      <c r="M24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C25" s="2">
+        <v>38236</v>
+      </c>
+      <c r="D25" s="2">
+        <v>2130759244</v>
+      </c>
+      <c r="E25" s="3">
+        <v>44243</v>
+      </c>
+      <c r="F25" t="s">
+        <v>101</v>
+      </c>
+      <c r="G25" t="s">
+        <v>131</v>
+      </c>
+      <c r="H25" s="4">
+        <v>0.85450000000000004</v>
+      </c>
+      <c r="I25">
+        <v>9.73</v>
+      </c>
+      <c r="J25" s="2">
+        <v>2030036</v>
+      </c>
+      <c r="K25" s="2">
+        <v>1322117</v>
+      </c>
+      <c r="L25" s="2">
+        <v>225165</v>
+      </c>
+      <c r="M25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C26" s="2">
+        <v>37019</v>
+      </c>
+      <c r="D26" s="2">
+        <v>814164211</v>
+      </c>
+      <c r="E26" s="3">
+        <v>45018</v>
+      </c>
+      <c r="F26" t="s">
+        <v>98</v>
+      </c>
+      <c r="G26" t="s">
+        <v>128</v>
+      </c>
+      <c r="H26" s="4">
+        <v>0.86840000000000006</v>
+      </c>
+      <c r="I26">
+        <v>17.64</v>
+      </c>
+      <c r="J26" s="2">
+        <v>16162337</v>
+      </c>
+      <c r="K26" s="2">
+        <v>138003</v>
+      </c>
+      <c r="L26" s="2">
+        <v>20916</v>
+      </c>
+      <c r="M26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" s="2">
+        <v>36261</v>
+      </c>
+      <c r="D27" s="2">
+        <v>12869595926</v>
+      </c>
+      <c r="E27" s="3">
+        <v>43852</v>
+      </c>
+      <c r="F27" t="s">
+        <v>100</v>
+      </c>
+      <c r="G27" t="s">
+        <v>144</v>
+      </c>
+      <c r="H27" s="4">
+        <v>0.89910000000000001</v>
+      </c>
+      <c r="I27">
+        <v>10.66</v>
+      </c>
+      <c r="J27" s="2">
+        <v>11583126</v>
+      </c>
+      <c r="K27" s="2">
+        <v>3540143</v>
+      </c>
+      <c r="L27" s="2">
+        <v>397288</v>
+      </c>
+      <c r="M27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="2">
+        <v>34869</v>
+      </c>
+      <c r="D28" s="2">
+        <v>2206004485</v>
+      </c>
+      <c r="E28" s="3">
+        <v>43485</v>
+      </c>
+      <c r="F28" t="s">
+        <v>100</v>
+      </c>
+      <c r="G28" t="s">
+        <v>119</v>
+      </c>
+      <c r="H28" s="4">
+        <v>0.9154000000000001</v>
+      </c>
+      <c r="I28">
+        <v>20.57</v>
+      </c>
+      <c r="J28" s="2">
+        <v>4691792</v>
+      </c>
+      <c r="K28" s="2">
+        <v>1585526</v>
+      </c>
+      <c r="L28" s="2">
+        <v>146445</v>
+      </c>
+      <c r="M28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="C29" s="2">
+        <v>30288</v>
+      </c>
+      <c r="D29" s="2">
+        <v>297698397</v>
+      </c>
+      <c r="E29" s="3">
+        <v>45008</v>
+      </c>
+      <c r="F29" t="s">
+        <v>99</v>
+      </c>
+      <c r="G29" t="s">
+        <v>246</v>
+      </c>
+      <c r="H29" s="4">
+        <v>0.92040000000000011</v>
+      </c>
+      <c r="I29">
+        <v>19.510000000000002</v>
+      </c>
+      <c r="J29" s="2">
+        <v>197673</v>
+      </c>
+      <c r="K29" s="2">
+        <v>204983</v>
+      </c>
+      <c r="L29" s="2">
+        <v>17728</v>
+      </c>
+      <c r="M29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="2">
+        <v>29880</v>
+      </c>
+      <c r="D30" s="2">
+        <v>2532139417</v>
+      </c>
+      <c r="E30" s="3">
+        <v>44594</v>
+      </c>
+      <c r="F30" t="s">
+        <v>99</v>
+      </c>
+      <c r="G30" t="s">
+        <v>133</v>
+      </c>
+      <c r="H30" s="4">
+        <v>0.58219999999999994</v>
+      </c>
+      <c r="I30">
+        <v>9.39</v>
+      </c>
+      <c r="J30" s="2">
+        <v>1128949</v>
+      </c>
+      <c r="K30" s="2">
+        <v>259955</v>
+      </c>
+      <c r="L30" s="2">
+        <v>186584</v>
+      </c>
+      <c r="M30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C31" s="2">
+        <v>27847</v>
+      </c>
+      <c r="D31" s="2">
+        <v>2536455291</v>
+      </c>
+      <c r="E31" s="3">
+        <v>44596</v>
+      </c>
+      <c r="F31" t="s">
+        <v>165</v>
+      </c>
+      <c r="G31" t="s">
+        <v>129</v>
+      </c>
+      <c r="H31" s="4">
+        <v>0.92870000000000008</v>
+      </c>
+      <c r="I31">
+        <v>8.7200000000000006</v>
+      </c>
+      <c r="J31" s="2">
+        <v>2878387</v>
+      </c>
+      <c r="K31" s="2">
+        <v>2066817</v>
+      </c>
+      <c r="L31" s="2">
+        <v>158741</v>
+      </c>
+      <c r="M31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C32" s="2">
+        <v>27201</v>
+      </c>
+      <c r="D32" s="2">
+        <v>61443311</v>
+      </c>
+      <c r="E32" s="3">
+        <v>45437</v>
+      </c>
+      <c r="F32" t="s">
+        <v>248</v>
+      </c>
+      <c r="G32" t="s">
+        <v>249</v>
+      </c>
+      <c r="H32" s="4">
+        <v>0.95019999999999993</v>
+      </c>
+      <c r="I32">
+        <v>5.92</v>
+      </c>
+      <c r="J32" s="2">
+        <v>1779358</v>
+      </c>
+      <c r="K32" s="2">
+        <v>504143</v>
+      </c>
+      <c r="L32" s="2">
+        <v>26410</v>
+      </c>
+      <c r="M32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C33" s="2">
+        <v>27032</v>
+      </c>
+      <c r="D33" s="2">
+        <v>848957706</v>
+      </c>
+      <c r="E33" s="3">
+        <v>45337</v>
+      </c>
+      <c r="F33" t="s">
+        <v>99</v>
+      </c>
+      <c r="G33" t="s">
+        <v>125</v>
+      </c>
+      <c r="H33" s="4">
+        <v>0.91870000000000007</v>
+      </c>
+      <c r="I33">
+        <v>9.64</v>
+      </c>
+      <c r="J33" s="2">
+        <v>1058477</v>
+      </c>
+      <c r="K33" s="2">
+        <v>1304904</v>
+      </c>
+      <c r="L33" s="2">
+        <v>115459</v>
+      </c>
+      <c r="M33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C34" s="2">
+        <v>26859</v>
+      </c>
+      <c r="D34" s="2">
+        <v>6958363966</v>
+      </c>
+      <c r="E34" s="3">
+        <v>42740</v>
+      </c>
+      <c r="F34" t="s">
+        <v>98</v>
+      </c>
+      <c r="G34" t="s">
+        <v>137</v>
+      </c>
+      <c r="H34" s="4">
+        <v>0.87819999999999998</v>
+      </c>
+      <c r="I34">
+        <v>14.59</v>
+      </c>
+      <c r="J34" s="2">
+        <v>18199081</v>
+      </c>
+      <c r="K34" s="2">
+        <v>5468147</v>
+      </c>
+      <c r="L34" s="2">
+        <v>758735</v>
+      </c>
+      <c r="M34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C35" s="2">
+        <v>26796</v>
+      </c>
+      <c r="D35" s="2">
+        <v>5079769723</v>
+      </c>
+      <c r="E35" s="3">
+        <v>44268</v>
+      </c>
+      <c r="F35" t="s">
+        <v>99</v>
+      </c>
+      <c r="G35" t="s">
+        <v>195</v>
+      </c>
+      <c r="H35" s="4">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="I35">
+        <v>8.76</v>
+      </c>
+      <c r="J35" s="2">
+        <v>6257334</v>
+      </c>
+      <c r="K35" s="2">
+        <v>3517476</v>
+      </c>
+      <c r="L35" s="2">
+        <v>248654</v>
+      </c>
+      <c r="M35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C36" s="2">
+        <v>26753</v>
+      </c>
+      <c r="D36" s="2">
+        <v>24958983</v>
+      </c>
+      <c r="E36" s="3">
+        <v>44963</v>
+      </c>
+      <c r="F36" t="s">
+        <v>100</v>
+      </c>
+      <c r="G36" t="s">
+        <v>252</v>
+      </c>
+      <c r="H36" s="4">
+        <v>0.95609999999999995</v>
+      </c>
+      <c r="I36">
+        <v>15.4</v>
+      </c>
+      <c r="J36" s="2">
+        <v>388144</v>
+      </c>
+      <c r="K36" s="2">
+        <v>113927</v>
+      </c>
+      <c r="L36" s="2">
+        <v>5225</v>
+      </c>
+      <c r="M36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="C37" s="2">
+        <v>25563</v>
+      </c>
+      <c r="D37" s="2">
+        <v>833945120</v>
+      </c>
+      <c r="E37" s="3">
+        <v>44006</v>
+      </c>
+      <c r="F37" t="s">
+        <v>235</v>
+      </c>
+      <c r="G37" t="s">
+        <v>134</v>
+      </c>
+      <c r="H37" s="4">
+        <v>0.89459999999999995</v>
+      </c>
+      <c r="I37">
+        <v>22.27</v>
+      </c>
+      <c r="J37" s="2">
+        <v>2490852</v>
+      </c>
+      <c r="K37" s="2">
+        <v>558803</v>
+      </c>
+      <c r="L37" s="2">
+        <v>65852</v>
+      </c>
+      <c r="M37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" s="2">
+        <v>25299</v>
+      </c>
+      <c r="D38" s="2">
+        <v>3522145473</v>
+      </c>
+      <c r="E38" s="3">
+        <v>44513</v>
+      </c>
+      <c r="F38" t="s">
+        <v>100</v>
+      </c>
+      <c r="G38" t="s">
+        <v>145</v>
+      </c>
+      <c r="H38" s="4">
+        <v>0.8234999999999999</v>
+      </c>
+      <c r="I38">
+        <v>7.71</v>
+      </c>
+      <c r="J38" s="2">
+        <v>3113597</v>
+      </c>
+      <c r="K38" s="2">
+        <v>1270225</v>
+      </c>
+      <c r="L38" s="2">
+        <v>272228</v>
+      </c>
+      <c r="M38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="C39" s="2">
+        <v>24671</v>
+      </c>
+      <c r="D39" s="2">
+        <v>4460099502</v>
+      </c>
+      <c r="E39" s="3">
+        <v>42916</v>
+      </c>
+      <c r="F39" t="s">
+        <v>100</v>
+      </c>
+      <c r="G39" t="s">
+        <v>228</v>
+      </c>
+      <c r="H39" s="4">
+        <v>0.92090000000000005</v>
+      </c>
+      <c r="I39">
+        <v>11.3</v>
+      </c>
+      <c r="J39" s="2">
+        <v>8835263</v>
+      </c>
+      <c r="K39" s="2">
+        <v>2282112</v>
+      </c>
+      <c r="L39" s="2">
+        <v>196019</v>
+      </c>
+      <c r="M39" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C40" s="2">
+        <v>24086</v>
+      </c>
+      <c r="D40" s="2">
+        <v>2400010282</v>
+      </c>
+      <c r="E40" s="3">
+        <v>44016</v>
+      </c>
+      <c r="F40" t="s">
+        <v>98</v>
+      </c>
+      <c r="G40" t="s">
+        <v>199</v>
+      </c>
+      <c r="H40" s="4">
+        <v>0.75249999999999995</v>
+      </c>
+      <c r="I40">
+        <v>22.57</v>
+      </c>
+      <c r="J40" s="2">
+        <v>2400797</v>
+      </c>
+      <c r="K40" s="2">
+        <v>554365</v>
+      </c>
+      <c r="L40" s="2">
+        <v>182288</v>
+      </c>
+      <c r="M40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C41" s="2">
+        <v>24075</v>
+      </c>
+      <c r="D41" s="2">
+        <v>23471426839</v>
+      </c>
+      <c r="E41" s="3">
+        <v>43269</v>
+      </c>
+      <c r="F41" t="s">
+        <v>99</v>
+      </c>
+      <c r="G41" t="s">
+        <v>143</v>
+      </c>
+      <c r="H41" s="4">
+        <v>0.74209999999999998</v>
+      </c>
+      <c r="I41">
+        <v>4.18</v>
+      </c>
+      <c r="J41" s="2">
+        <v>11111505</v>
+      </c>
+      <c r="K41" s="2">
+        <v>3809530</v>
+      </c>
+      <c r="L41" s="2">
+        <v>1323821</v>
+      </c>
+      <c r="M41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" s="2">
+        <v>23817</v>
+      </c>
+      <c r="D42" s="2">
+        <v>845881301</v>
+      </c>
+      <c r="E42" s="3">
+        <v>44958</v>
+      </c>
+      <c r="F42" t="s">
+        <v>101</v>
+      </c>
+      <c r="G42" t="s">
+        <v>140</v>
+      </c>
+      <c r="H42" s="4">
+        <v>0.84470000000000001</v>
+      </c>
+      <c r="I42">
+        <v>11.31</v>
+      </c>
+      <c r="J42" s="2">
+        <v>573061</v>
+      </c>
+      <c r="K42" s="2">
+        <v>243436</v>
+      </c>
+      <c r="L42" s="2">
+        <v>44754</v>
+      </c>
+      <c r="M42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C43" s="2">
+        <v>21944</v>
+      </c>
+      <c r="D43" s="2">
+        <v>1393281346</v>
+      </c>
+      <c r="E43" s="3">
+        <v>43638</v>
+      </c>
+      <c r="F43" t="s">
+        <v>99</v>
+      </c>
+      <c r="G43" t="s">
+        <v>148</v>
+      </c>
+      <c r="H43" s="4">
+        <v>0.93049999999999999</v>
+      </c>
+      <c r="I43">
+        <v>12.06</v>
+      </c>
+      <c r="J43" s="2">
+        <v>9963950</v>
+      </c>
+      <c r="K43" s="2">
+        <v>1351417</v>
+      </c>
+      <c r="L43" s="2">
+        <v>100990</v>
+      </c>
+      <c r="M43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C44" s="2">
+        <v>20933</v>
+      </c>
+      <c r="D44" s="2">
+        <v>345974852</v>
+      </c>
+      <c r="E44" s="3">
+        <v>44984</v>
+      </c>
+      <c r="F44" t="s">
+        <v>98</v>
+      </c>
+      <c r="G44" t="s">
+        <v>256</v>
+      </c>
+      <c r="H44" s="4">
+        <v>0.87450000000000006</v>
+      </c>
+      <c r="I44">
+        <v>16.11</v>
+      </c>
+      <c r="J44" s="2">
+        <v>407887</v>
+      </c>
+      <c r="K44" s="2">
+        <v>124518</v>
+      </c>
+      <c r="L44" s="2">
+        <v>17871</v>
+      </c>
+      <c r="M44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="C45" s="2">
+        <v>20343</v>
+      </c>
+      <c r="D45" s="2">
+        <v>4555247557</v>
+      </c>
+      <c r="E45" s="3">
+        <v>44313</v>
+      </c>
+      <c r="F45" t="s">
+        <v>98</v>
+      </c>
+      <c r="G45" t="s">
+        <v>132</v>
+      </c>
+      <c r="H45" s="4">
+        <v>0.90239999999999998</v>
+      </c>
+      <c r="I45">
+        <v>15.75</v>
+      </c>
+      <c r="J45" s="2">
+        <v>20796036</v>
+      </c>
+      <c r="K45" s="2">
+        <v>1229030</v>
+      </c>
+      <c r="L45" s="2">
+        <v>132907</v>
+      </c>
+      <c r="M45" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C46" s="2">
+        <v>19092</v>
+      </c>
+      <c r="D46" s="2">
+        <v>61316863</v>
+      </c>
+      <c r="E46" s="3">
+        <v>44836</v>
+      </c>
+      <c r="F46" t="s">
+        <v>235</v>
+      </c>
+      <c r="G46" t="s">
+        <v>259</v>
+      </c>
+      <c r="H46" s="4">
+        <v>0.75870000000000004</v>
+      </c>
+      <c r="I46">
+        <v>12.71</v>
+      </c>
+      <c r="J46" s="2">
+        <v>2088943</v>
+      </c>
+      <c r="K46" s="2">
+        <v>28178</v>
+      </c>
+      <c r="L46" s="2">
+        <v>8963</v>
+      </c>
+      <c r="M46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C47" s="2">
+        <v>18901</v>
+      </c>
+      <c r="D47" s="2">
+        <v>485150159</v>
+      </c>
+      <c r="E47" s="3">
+        <v>43858</v>
+      </c>
+      <c r="F47" t="s">
+        <v>101</v>
+      </c>
+      <c r="G47" t="s">
+        <v>147</v>
+      </c>
+      <c r="H47" s="4">
+        <v>0.91310000000000002</v>
+      </c>
+      <c r="I47">
+        <v>24.46</v>
+      </c>
+      <c r="J47" s="2">
+        <v>1899183</v>
+      </c>
+      <c r="K47" s="2">
+        <v>686528</v>
+      </c>
+      <c r="L47" s="2">
+        <v>65365</v>
+      </c>
+      <c r="M47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C48" s="2">
+        <v>18839</v>
+      </c>
+      <c r="D48" s="2">
+        <v>661801743</v>
+      </c>
+      <c r="E48" s="3">
+        <v>45206</v>
+      </c>
+      <c r="F48" t="s">
+        <v>167</v>
+      </c>
+      <c r="G48" t="s">
+        <v>135</v>
+      </c>
+      <c r="H48" s="4">
+        <v>0.96560000000000001</v>
+      </c>
+      <c r="I48">
+        <v>12.72</v>
+      </c>
+      <c r="J48" s="2">
+        <v>934017</v>
+      </c>
+      <c r="K48" s="2">
+        <v>1909283</v>
+      </c>
+      <c r="L48" s="2">
+        <v>67983</v>
+      </c>
+      <c r="M48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C49" s="2">
+        <v>18467</v>
+      </c>
+      <c r="D49" s="2">
+        <v>561797458</v>
+      </c>
+      <c r="E49" s="3">
+        <v>45013</v>
+      </c>
+      <c r="F49" t="s">
+        <v>99</v>
+      </c>
+      <c r="G49" t="s">
+        <v>262</v>
+      </c>
+      <c r="H49" s="4">
+        <v>0.91099999999999992</v>
+      </c>
+      <c r="I49">
+        <v>12.7</v>
+      </c>
+      <c r="J49" s="2">
+        <v>1015984</v>
+      </c>
+      <c r="K49" s="2">
+        <v>1099782</v>
+      </c>
+      <c r="L49" s="2">
+        <v>107415</v>
+      </c>
+      <c r="M49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50" s="2">
+        <v>18387</v>
+      </c>
+      <c r="D50" s="2">
+        <v>372523919</v>
+      </c>
+      <c r="E50" s="3">
+        <v>45026</v>
+      </c>
+      <c r="F50" t="s">
+        <v>101</v>
+      </c>
+      <c r="G50" t="s">
+        <v>136</v>
+      </c>
+      <c r="H50" s="4">
+        <v>0.82680000000000009</v>
+      </c>
+      <c r="I50">
+        <v>13.41</v>
+      </c>
+      <c r="J50" s="2">
+        <v>632785</v>
+      </c>
+      <c r="K50" s="2">
+        <v>333740</v>
+      </c>
+      <c r="L50" s="2">
+        <v>69900</v>
+      </c>
+      <c r="M50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C51" s="2">
+        <v>18195</v>
+      </c>
+      <c r="D51" s="2">
+        <v>963763756</v>
+      </c>
+      <c r="E51" s="3">
+        <v>43226</v>
+      </c>
+      <c r="F51" t="s">
+        <v>99</v>
+      </c>
+      <c r="G51" t="s">
+        <v>138</v>
+      </c>
+      <c r="H51" s="4">
+        <v>0.90339999999999998</v>
+      </c>
+      <c r="I51">
+        <v>31.74</v>
+      </c>
+      <c r="J51" s="2">
+        <v>1406496</v>
+      </c>
+      <c r="K51" s="2">
+        <v>962106</v>
+      </c>
+      <c r="L51" s="2">
+        <v>102927</v>
+      </c>
+      <c r="M51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C52" s="2">
+        <v>17875</v>
+      </c>
+      <c r="D52" s="2">
+        <v>520914162</v>
+      </c>
+      <c r="E52" s="3">
+        <v>45078</v>
+      </c>
+      <c r="F52" t="s">
+        <v>101</v>
+      </c>
+      <c r="G52" t="s">
+        <v>126</v>
+      </c>
+      <c r="H52" s="4">
+        <v>0.85959999999999992</v>
+      </c>
+      <c r="I52">
+        <v>13.68</v>
+      </c>
+      <c r="J52" s="2">
+        <v>685190</v>
+      </c>
+      <c r="K52" s="2">
+        <v>586210</v>
+      </c>
+      <c r="L52" s="2">
+        <v>95742</v>
+      </c>
+      <c r="M52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:M1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D4922F-A22D-1547-8F5C-336FD651258D}">
   <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3404,7 +5640,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M52"/>
   <sheetViews>
@@ -5546,7 +7782,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CD5A4D4-8172-B14E-80EB-29CD406E771F}">
   <dimension ref="A1:M52"/>
   <sheetViews>

</xml_diff>

<commit_message>
updated roblox genres in most recent pull
</commit_message>
<xml_diff>
--- a/data/total_roblox_experiences.xlsx
+++ b/data/total_roblox_experiences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenwang/Desktop/Makers/Steam_Roblox_Streamlit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19F3F3A5-ED45-D74D-A48B-9EB4C9F509F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B02FEAE-EFC8-BE4E-B0E1-A558CD848808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5840" yWindow="1100" windowWidth="23460" windowHeight="18020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="264">
   <si>
     <t>#1</t>
   </si>
@@ -728,9 +728,6 @@
   </si>
   <si>
     <t>[UPD🌗] Anime Defenders</t>
-  </si>
-  <si>
-    <t>All</t>
   </si>
   <si>
     <t>Adopt Me!</t>
@@ -1243,8 +1240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B937581-5BFE-0C43-9A8A-CAE8581C0F34}">
   <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1419,7 +1416,7 @@
         <v>45386</v>
       </c>
       <c r="F5" t="s">
-        <v>235</v>
+        <v>168</v>
       </c>
       <c r="G5" t="s">
         <v>105</v>
@@ -1542,7 +1539,7 @@
         <v>45216</v>
       </c>
       <c r="F8" t="s">
-        <v>235</v>
+        <v>164</v>
       </c>
       <c r="G8" t="s">
         <v>110</v>
@@ -1571,7 +1568,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C9" s="2">
         <v>158091</v>
@@ -1668,7 +1665,7 @@
         <v>99</v>
       </c>
       <c r="G11" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H11" s="4">
         <v>0.94950000000000001</v>
@@ -1694,7 +1691,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C12" s="2">
         <v>87657</v>
@@ -1706,7 +1703,7 @@
         <v>44597</v>
       </c>
       <c r="F12" t="s">
-        <v>235</v>
+        <v>163</v>
       </c>
       <c r="G12" t="s">
         <v>109</v>
@@ -1747,7 +1744,7 @@
         <v>45262</v>
       </c>
       <c r="F13" t="s">
-        <v>235</v>
+        <v>169</v>
       </c>
       <c r="G13" t="s">
         <v>107</v>
@@ -1858,7 +1855,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C16" s="2">
         <v>53534</v>
@@ -1870,7 +1867,7 @@
         <v>45093</v>
       </c>
       <c r="F16" t="s">
-        <v>235</v>
+        <v>168</v>
       </c>
       <c r="G16" t="s">
         <v>112</v>
@@ -1940,7 +1937,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C18" s="2">
         <v>48388</v>
@@ -1952,7 +1949,7 @@
         <v>45421</v>
       </c>
       <c r="F18" t="s">
-        <v>235</v>
+        <v>167</v>
       </c>
       <c r="G18" t="s">
         <v>114</v>
@@ -2063,7 +2060,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C21" s="2">
         <v>44948</v>
@@ -2104,7 +2101,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C22" s="2">
         <v>44349</v>
@@ -2145,7 +2142,7 @@
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C23" s="2">
         <v>45225</v>
@@ -2227,7 +2224,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C25" s="2">
         <v>38236</v>
@@ -2268,7 +2265,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C26" s="2">
         <v>37019</v>
@@ -2391,7 +2388,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C29" s="2">
         <v>30288</v>
@@ -2406,7 +2403,7 @@
         <v>99</v>
       </c>
       <c r="G29" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H29" s="4">
         <v>0.92040000000000011</v>
@@ -2514,7 +2511,7 @@
         <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C32" s="2">
         <v>27201</v>
@@ -2526,10 +2523,10 @@
         <v>45437</v>
       </c>
       <c r="F32" t="s">
+        <v>247</v>
+      </c>
+      <c r="G32" t="s">
         <v>248</v>
-      </c>
-      <c r="G32" t="s">
-        <v>249</v>
       </c>
       <c r="H32" s="4">
         <v>0.95019999999999993</v>
@@ -2555,7 +2552,7 @@
         <v>30</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C33" s="2">
         <v>27032</v>
@@ -2678,7 +2675,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C36" s="2">
         <v>26753</v>
@@ -2693,7 +2690,7 @@
         <v>100</v>
       </c>
       <c r="G36" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H36" s="4">
         <v>0.95609999999999995</v>
@@ -2719,7 +2716,7 @@
         <v>34</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C37" s="2">
         <v>25563</v>
@@ -2731,7 +2728,7 @@
         <v>44006</v>
       </c>
       <c r="F37" t="s">
-        <v>235</v>
+        <v>185</v>
       </c>
       <c r="G37" t="s">
         <v>134</v>
@@ -2965,7 +2962,7 @@
         <v>40</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C43" s="2">
         <v>21944</v>
@@ -3006,7 +3003,7 @@
         <v>41</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C44" s="2">
         <v>20933</v>
@@ -3021,7 +3018,7 @@
         <v>98</v>
       </c>
       <c r="G44" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H44" s="4">
         <v>0.87450000000000006</v>
@@ -3047,7 +3044,7 @@
         <v>42</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C45" s="2">
         <v>20343</v>
@@ -3088,7 +3085,7 @@
         <v>43</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C46" s="2">
         <v>19092</v>
@@ -3100,10 +3097,10 @@
         <v>44836</v>
       </c>
       <c r="F46" t="s">
-        <v>235</v>
+        <v>101</v>
       </c>
       <c r="G46" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H46" s="4">
         <v>0.75870000000000004</v>
@@ -3129,7 +3126,7 @@
         <v>44</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C47" s="2">
         <v>18901</v>
@@ -3211,7 +3208,7 @@
         <v>46</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C49" s="2">
         <v>18467</v>
@@ -3226,7 +3223,7 @@
         <v>99</v>
       </c>
       <c r="G49" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H49" s="4">
         <v>0.91099999999999992</v>
@@ -3293,7 +3290,7 @@
         <v>48</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C51" s="2">
         <v>18195</v>
@@ -3334,7 +3331,7 @@
         <v>49</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C52" s="2">
         <v>17875</v>
@@ -3383,7 +3380,7 @@
   <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5648,7 +5645,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="B34" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add july 29 data
</commit_message>
<xml_diff>
--- a/data/total_roblox_experiences.xlsx
+++ b/data/total_roblox_experiences.xlsx
@@ -8,22 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenwang/Desktop/Makers/Steam_Roblox_Streamlit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B02FEAE-EFC8-BE4E-B0E1-A558CD848808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4F3BBE-313F-2F46-A128-9CC4C22A2A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5840" yWindow="1100" windowWidth="23460" windowHeight="18020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2024-07-25" sheetId="4" r:id="rId1"/>
-    <sheet name="2024-07-09" sheetId="3" r:id="rId2"/>
-    <sheet name="2024-07-01" sheetId="1" r:id="rId3"/>
-    <sheet name="2024-06-20" sheetId="2" r:id="rId4"/>
+    <sheet name="2024-07-29" sheetId="5" r:id="rId1"/>
+    <sheet name="2024-07-22" sheetId="4" r:id="rId2"/>
+    <sheet name="2024-07-09" sheetId="3" r:id="rId3"/>
+    <sheet name="2024-07-01" sheetId="1" r:id="rId4"/>
+    <sheet name="2024-06-20" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="334">
   <si>
     <t>#1</t>
   </si>
@@ -815,6 +816,216 @@
   </si>
   <si>
     <t>[BULLET] untitled boxing game🥊</t>
+  </si>
+  <si>
+    <t>Top Experiences 50 on Roblox (Data fetched from RoMonitor as of 02:22 AM EDT, 2024-07-29)</t>
+  </si>
+  <si>
+    <t>January 15, 2019</t>
+  </si>
+  <si>
+    <t>April 20, 2020</t>
+  </si>
+  <si>
+    <t>April 4, 2024</t>
+  </si>
+  <si>
+    <t>January 17, 2014</t>
+  </si>
+  <si>
+    <t>August 1, 2022</t>
+  </si>
+  <si>
+    <t>October 17, 2023</t>
+  </si>
+  <si>
+    <t>[🎁x2 Event] Bee Swarm Simulator</t>
+  </si>
+  <si>
+    <t>March 20, 2018</t>
+  </si>
+  <si>
+    <t>Pet Simulator 99! 🍍</t>
+  </si>
+  <si>
+    <t>February 4, 2022</t>
+  </si>
+  <si>
+    <t>July 13, 2017</t>
+  </si>
+  <si>
+    <t>[TEN SHADOWS] Jujutsu Shenanigans</t>
+  </si>
+  <si>
+    <t>April 16, 2022</t>
+  </si>
+  <si>
+    <t>January 6, 2022</t>
+  </si>
+  <si>
+    <t>December 2, 2023</t>
+  </si>
+  <si>
+    <t>TYPE://SOUL [UPDATE PART 2]</t>
+  </si>
+  <si>
+    <t>July 14, 2023</t>
+  </si>
+  <si>
+    <t>June 9, 2022</t>
+  </si>
+  <si>
+    <t>June 16, 2023</t>
+  </si>
+  <si>
+    <t>BedWars [😇 TRINITY REWORK]</t>
+  </si>
+  <si>
+    <t>May 26, 2021</t>
+  </si>
+  <si>
+    <t>July 2, 2021</t>
+  </si>
+  <si>
+    <t>LifeTogether 🏠 RP (UPDATE 21)</t>
+  </si>
+  <si>
+    <t>July 4, 2023</t>
+  </si>
+  <si>
+    <t>[UPD 📱] Baddies 💅</t>
+  </si>
+  <si>
+    <t>October 2, 2022</t>
+  </si>
+  <si>
+    <t>January 20, 2019</t>
+  </si>
+  <si>
+    <t>November 1, 2016</t>
+  </si>
+  <si>
+    <t>[KILLSTREAK 1000] Slap Battles👏</t>
+  </si>
+  <si>
+    <t>February 15, 2021</t>
+  </si>
+  <si>
+    <t>[⭐ x4 + CODE] Anime Last Stand</t>
+  </si>
+  <si>
+    <t>March 23, 2023</t>
+  </si>
+  <si>
+    <t>[B:S] ALS Team</t>
+  </si>
+  <si>
+    <t>[EVENT] Gym League</t>
+  </si>
+  <si>
+    <t>May 9, 2024</t>
+  </si>
+  <si>
+    <t>November 3, 2014</t>
+  </si>
+  <si>
+    <t>[UPDATE 4] Meme Sea</t>
+  </si>
+  <si>
+    <t>July 16, 2022</t>
+  </si>
+  <si>
+    <t>Meme Sea Group</t>
+  </si>
+  <si>
+    <t>April 2, 2023</t>
+  </si>
+  <si>
+    <t>May 25, 2024</t>
+  </si>
+  <si>
+    <t>February 6, 2023</t>
+  </si>
+  <si>
+    <t>🌊 Creatures of Sonaria 💙 Survive Kaiju Animals</t>
+  </si>
+  <si>
+    <t>June 24, 2020</t>
+  </si>
+  <si>
+    <t>a dusty trip [🤠 BOSS]</t>
+  </si>
+  <si>
+    <t>February 15, 2024</t>
+  </si>
+  <si>
+    <t>June 1, 2023</t>
+  </si>
+  <si>
+    <t>July 4, 2020</t>
+  </si>
+  <si>
+    <t>January 5, 2017</t>
+  </si>
+  <si>
+    <t>April 27, 2021</t>
+  </si>
+  <si>
+    <t>February 1, 2022</t>
+  </si>
+  <si>
+    <t>March 13, 2021</t>
+  </si>
+  <si>
+    <t>January 22, 2020</t>
+  </si>
+  <si>
+    <t>December 16, 2019</t>
+  </si>
+  <si>
+    <t>February 1, 2023</t>
+  </si>
+  <si>
+    <t>Fling Things and People</t>
+  </si>
+  <si>
+    <t>June 16, 2021</t>
+  </si>
+  <si>
+    <t>Comedy</t>
+  </si>
+  <si>
+    <t>Horomori</t>
+  </si>
+  <si>
+    <t>June 17, 2018</t>
+  </si>
+  <si>
+    <t>[LIMITED✨] Driving Empire 🏎️ Car Racing</t>
+  </si>
+  <si>
+    <t>June 22, 2019</t>
+  </si>
+  <si>
+    <t>Five Nights TD [MILITARY]</t>
+  </si>
+  <si>
+    <t>January 1, 2024</t>
+  </si>
+  <si>
+    <t>April 13, 2023</t>
+  </si>
+  <si>
+    <t>🐚Dandy's World [ALPHA]</t>
+  </si>
+  <si>
+    <t>January 25, 2024</t>
+  </si>
+  <si>
+    <t>BlushCrunch Studio</t>
+  </si>
+  <si>
+    <t>November 13, 2021</t>
   </si>
 </sst>
 </file>
@@ -1237,11 +1448,2147 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99C60782-7F66-D04D-A716-667EE5D461B9}">
+  <dimension ref="A1:M52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="1" customWidth="1"/>
+    <col min="3" max="7" width="18.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="4" customWidth="1"/>
+    <col min="9" max="10" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" customWidth="1"/>
+    <col min="13" max="13" width="18.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="2">
+        <v>479600</v>
+      </c>
+      <c r="D3" s="2">
+        <v>37191190699</v>
+      </c>
+      <c r="E3" s="2">
+        <v>12781988</v>
+      </c>
+      <c r="F3" s="2">
+        <v>7812016</v>
+      </c>
+      <c r="G3" s="2">
+        <v>596308</v>
+      </c>
+      <c r="H3" s="4">
+        <v>0.92909999999999993</v>
+      </c>
+      <c r="I3">
+        <v>16.18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>265</v>
+      </c>
+      <c r="K3" t="s">
+        <v>99</v>
+      </c>
+      <c r="L3" t="s">
+        <v>104</v>
+      </c>
+      <c r="M3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="2">
+        <v>435137</v>
+      </c>
+      <c r="D4" s="2">
+        <v>51546629458</v>
+      </c>
+      <c r="E4" s="2">
+        <v>21420731</v>
+      </c>
+      <c r="F4" s="2">
+        <v>5754306</v>
+      </c>
+      <c r="G4" s="2">
+        <v>890025</v>
+      </c>
+      <c r="H4" s="4">
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="I4">
+        <v>17.29</v>
+      </c>
+      <c r="J4" t="s">
+        <v>266</v>
+      </c>
+      <c r="K4" t="s">
+        <v>98</v>
+      </c>
+      <c r="L4" t="s">
+        <v>103</v>
+      </c>
+      <c r="M4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C5" s="2">
+        <v>298489</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1371411535</v>
+      </c>
+      <c r="E5" s="2">
+        <v>541797</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1613146</v>
+      </c>
+      <c r="G5" s="2">
+        <v>40072</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0.9758</v>
+      </c>
+      <c r="I5">
+        <v>15.45</v>
+      </c>
+      <c r="J5" t="s">
+        <v>267</v>
+      </c>
+      <c r="K5" t="s">
+        <v>168</v>
+      </c>
+      <c r="L5" t="s">
+        <v>105</v>
+      </c>
+      <c r="M5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="2">
+        <v>159900</v>
+      </c>
+      <c r="D6" s="2">
+        <v>16278459940</v>
+      </c>
+      <c r="E6" s="2">
+        <v>18589623</v>
+      </c>
+      <c r="F6" s="2">
+        <v>7481912</v>
+      </c>
+      <c r="G6" s="2">
+        <v>723097</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0.91189999999999993</v>
+      </c>
+      <c r="I6">
+        <v>12.86</v>
+      </c>
+      <c r="J6" t="s">
+        <v>268</v>
+      </c>
+      <c r="K6" t="s">
+        <v>100</v>
+      </c>
+      <c r="L6" t="s">
+        <v>106</v>
+      </c>
+      <c r="M6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="2">
+        <v>125472</v>
+      </c>
+      <c r="D7" s="2">
+        <v>6664536140</v>
+      </c>
+      <c r="E7" s="2">
+        <v>3463774</v>
+      </c>
+      <c r="F7" s="2">
+        <v>2371578</v>
+      </c>
+      <c r="G7" s="2">
+        <v>450781</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0.84030000000000005</v>
+      </c>
+      <c r="I7">
+        <v>9.52</v>
+      </c>
+      <c r="J7" t="s">
+        <v>269</v>
+      </c>
+      <c r="K7" t="s">
+        <v>101</v>
+      </c>
+      <c r="L7" t="s">
+        <v>108</v>
+      </c>
+      <c r="M7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="2">
+        <v>117251</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1536110208</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1535854</v>
+      </c>
+      <c r="F8" s="2">
+        <v>863496</v>
+      </c>
+      <c r="G8" s="2">
+        <v>84899</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0.91049999999999998</v>
+      </c>
+      <c r="I8">
+        <v>15.24</v>
+      </c>
+      <c r="J8" t="s">
+        <v>270</v>
+      </c>
+      <c r="K8" t="s">
+        <v>164</v>
+      </c>
+      <c r="L8" t="s">
+        <v>110</v>
+      </c>
+      <c r="M8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="C9" s="2">
+        <v>103126</v>
+      </c>
+      <c r="D9" s="2">
+        <v>2785155338</v>
+      </c>
+      <c r="E9" s="2">
+        <v>5876916</v>
+      </c>
+      <c r="F9" s="2">
+        <v>2226562</v>
+      </c>
+      <c r="G9" s="2">
+        <v>118450</v>
+      </c>
+      <c r="H9" s="4">
+        <v>0.94950000000000001</v>
+      </c>
+      <c r="I9">
+        <v>40.64</v>
+      </c>
+      <c r="J9" t="s">
+        <v>272</v>
+      </c>
+      <c r="K9" t="s">
+        <v>99</v>
+      </c>
+      <c r="L9" t="s">
+        <v>121</v>
+      </c>
+      <c r="M9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C10" s="2">
+        <v>102905</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1280546290</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1341397</v>
+      </c>
+      <c r="F10" s="2">
+        <v>2378754</v>
+      </c>
+      <c r="G10" s="2">
+        <v>88417</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0.96420000000000006</v>
+      </c>
+      <c r="I10">
+        <v>51.22</v>
+      </c>
+      <c r="J10" t="s">
+        <v>274</v>
+      </c>
+      <c r="K10" t="s">
+        <v>163</v>
+      </c>
+      <c r="L10" t="s">
+        <v>109</v>
+      </c>
+      <c r="M10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="C11" s="2">
+        <v>90298</v>
+      </c>
+      <c r="D11" s="2">
+        <v>36927790087</v>
+      </c>
+      <c r="E11" s="2">
+        <v>26844319</v>
+      </c>
+      <c r="F11" s="2">
+        <v>7177490</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1419165</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0.83489999999999998</v>
+      </c>
+      <c r="I11">
+        <v>19.07</v>
+      </c>
+      <c r="J11" t="s">
+        <v>275</v>
+      </c>
+      <c r="K11" t="s">
+        <v>102</v>
+      </c>
+      <c r="L11" t="s">
+        <v>111</v>
+      </c>
+      <c r="M11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C12" s="2">
+        <v>72236</v>
+      </c>
+      <c r="D12" s="2">
+        <v>459123815</v>
+      </c>
+      <c r="E12" s="2">
+        <v>641868</v>
+      </c>
+      <c r="F12" s="2">
+        <v>461003</v>
+      </c>
+      <c r="G12" s="2">
+        <v>83942</v>
+      </c>
+      <c r="H12" s="4">
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="I12">
+        <v>14.1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>277</v>
+      </c>
+      <c r="K12" t="s">
+        <v>101</v>
+      </c>
+      <c r="L12" t="s">
+        <v>120</v>
+      </c>
+      <c r="M12" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C13" s="2">
+        <v>70976</v>
+      </c>
+      <c r="D13" s="2">
+        <v>459276141</v>
+      </c>
+      <c r="E13" s="2">
+        <v>641978</v>
+      </c>
+      <c r="F13" s="2">
+        <v>461003</v>
+      </c>
+      <c r="G13" s="2">
+        <v>83942</v>
+      </c>
+      <c r="H13" s="4">
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="I13">
+        <v>14.1</v>
+      </c>
+      <c r="J13" t="s">
+        <v>277</v>
+      </c>
+      <c r="K13" t="s">
+        <v>101</v>
+      </c>
+      <c r="L13" t="s">
+        <v>120</v>
+      </c>
+      <c r="M13" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="2">
+        <v>68536</v>
+      </c>
+      <c r="D14" s="2">
+        <v>3764152141</v>
+      </c>
+      <c r="E14" s="2">
+        <v>2079318</v>
+      </c>
+      <c r="F14" s="2">
+        <v>584039</v>
+      </c>
+      <c r="G14" s="2">
+        <v>86819</v>
+      </c>
+      <c r="H14" s="4">
+        <v>0.87060000000000004</v>
+      </c>
+      <c r="I14">
+        <v>13.99</v>
+      </c>
+      <c r="J14" t="s">
+        <v>278</v>
+      </c>
+      <c r="K14" t="s">
+        <v>98</v>
+      </c>
+      <c r="L14" t="s">
+        <v>113</v>
+      </c>
+      <c r="M14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="2">
+        <v>66956</v>
+      </c>
+      <c r="D15" s="2">
+        <v>598529126</v>
+      </c>
+      <c r="E15" s="2">
+        <v>555340</v>
+      </c>
+      <c r="F15" s="2">
+        <v>611694</v>
+      </c>
+      <c r="G15" s="2">
+        <v>86775</v>
+      </c>
+      <c r="H15" s="4">
+        <v>0.87580000000000002</v>
+      </c>
+      <c r="I15">
+        <v>44.39</v>
+      </c>
+      <c r="J15" t="s">
+        <v>279</v>
+      </c>
+      <c r="K15" t="s">
+        <v>169</v>
+      </c>
+      <c r="L15" t="s">
+        <v>107</v>
+      </c>
+      <c r="M15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C16" s="2">
+        <v>62135</v>
+      </c>
+      <c r="D16" s="2">
+        <v>405087843</v>
+      </c>
+      <c r="E16" s="2">
+        <v>301603</v>
+      </c>
+      <c r="F16" s="2">
+        <v>220439</v>
+      </c>
+      <c r="G16" s="2">
+        <v>50028</v>
+      </c>
+      <c r="H16" s="4">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="I16">
+        <v>33.25</v>
+      </c>
+      <c r="J16" t="s">
+        <v>281</v>
+      </c>
+      <c r="K16" t="s">
+        <v>101</v>
+      </c>
+      <c r="L16" t="s">
+        <v>190</v>
+      </c>
+      <c r="M16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="2">
+        <v>53714</v>
+      </c>
+      <c r="D17" s="2">
+        <v>4534132650</v>
+      </c>
+      <c r="E17" s="2">
+        <v>4947577</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1912328</v>
+      </c>
+      <c r="G17" s="2">
+        <v>111700</v>
+      </c>
+      <c r="H17" s="4">
+        <v>0.94480000000000008</v>
+      </c>
+      <c r="I17">
+        <v>10.42</v>
+      </c>
+      <c r="J17" t="s">
+        <v>282</v>
+      </c>
+      <c r="K17" t="s">
+        <v>100</v>
+      </c>
+      <c r="L17" t="s">
+        <v>116</v>
+      </c>
+      <c r="M17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="2">
+        <v>35893</v>
+      </c>
+      <c r="D18" s="2">
+        <v>4035912077</v>
+      </c>
+      <c r="E18" s="2">
+        <v>9178721</v>
+      </c>
+      <c r="F18" s="2">
+        <v>6047590</v>
+      </c>
+      <c r="G18" s="2">
+        <v>411157</v>
+      </c>
+      <c r="H18" s="4">
+        <v>0.93629999999999991</v>
+      </c>
+      <c r="I18">
+        <v>11.48</v>
+      </c>
+      <c r="J18" t="s">
+        <v>283</v>
+      </c>
+      <c r="K18" t="s">
+        <v>101</v>
+      </c>
+      <c r="L18" t="s">
+        <v>117</v>
+      </c>
+      <c r="M18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C19" s="2">
+        <v>34811</v>
+      </c>
+      <c r="D19" s="2">
+        <v>9356733065</v>
+      </c>
+      <c r="E19" s="2">
+        <v>4151908</v>
+      </c>
+      <c r="F19" s="2">
+        <v>2125966</v>
+      </c>
+      <c r="G19" s="2">
+        <v>449168</v>
+      </c>
+      <c r="H19" s="4">
+        <v>0.8256</v>
+      </c>
+      <c r="I19">
+        <v>13.48</v>
+      </c>
+      <c r="J19" t="s">
+        <v>285</v>
+      </c>
+      <c r="K19" t="s">
+        <v>101</v>
+      </c>
+      <c r="L19" t="s">
+        <v>118</v>
+      </c>
+      <c r="M19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="2">
+        <v>31598</v>
+      </c>
+      <c r="D20" s="2">
+        <v>2512164284</v>
+      </c>
+      <c r="E20" s="2">
+        <v>3202857</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1221808</v>
+      </c>
+      <c r="G20" s="2">
+        <v>115012</v>
+      </c>
+      <c r="H20" s="4">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="I20">
+        <v>12.52</v>
+      </c>
+      <c r="J20" t="s">
+        <v>286</v>
+      </c>
+      <c r="K20" t="s">
+        <v>164</v>
+      </c>
+      <c r="L20" t="s">
+        <v>122</v>
+      </c>
+      <c r="M20" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C21" s="2">
+        <v>29876</v>
+      </c>
+      <c r="D21" s="2">
+        <v>788227346</v>
+      </c>
+      <c r="E21" s="2">
+        <v>941534</v>
+      </c>
+      <c r="F21" s="2">
+        <v>328623</v>
+      </c>
+      <c r="G21" s="2">
+        <v>25007</v>
+      </c>
+      <c r="H21" s="4">
+        <v>0.92930000000000001</v>
+      </c>
+      <c r="I21">
+        <v>17.850000000000001</v>
+      </c>
+      <c r="J21" t="s">
+        <v>288</v>
+      </c>
+      <c r="K21" t="s">
+        <v>98</v>
+      </c>
+      <c r="L21" t="s">
+        <v>123</v>
+      </c>
+      <c r="M21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="C22" s="2">
+        <v>27742</v>
+      </c>
+      <c r="D22" s="2">
+        <v>71673374</v>
+      </c>
+      <c r="E22" s="2">
+        <v>2230806</v>
+      </c>
+      <c r="F22" s="2">
+        <v>31073</v>
+      </c>
+      <c r="G22" s="2">
+        <v>10025</v>
+      </c>
+      <c r="H22" s="4">
+        <v>0.75609999999999999</v>
+      </c>
+      <c r="I22">
+        <v>12.89</v>
+      </c>
+      <c r="J22" t="s">
+        <v>290</v>
+      </c>
+      <c r="K22" t="s">
+        <v>101</v>
+      </c>
+      <c r="L22" t="s">
+        <v>258</v>
+      </c>
+      <c r="M22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="2">
+        <v>26310</v>
+      </c>
+      <c r="D23" s="2">
+        <v>2213846982</v>
+      </c>
+      <c r="E23" s="2">
+        <v>4699496</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1589129</v>
+      </c>
+      <c r="G23" s="2">
+        <v>146759</v>
+      </c>
+      <c r="H23" s="4">
+        <v>0.91549999999999998</v>
+      </c>
+      <c r="I23">
+        <v>20.79</v>
+      </c>
+      <c r="J23" t="s">
+        <v>291</v>
+      </c>
+      <c r="K23" t="s">
+        <v>100</v>
+      </c>
+      <c r="L23" t="s">
+        <v>119</v>
+      </c>
+      <c r="M23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" s="2">
+        <v>26293</v>
+      </c>
+      <c r="D24" s="2">
+        <v>3921265656</v>
+      </c>
+      <c r="E24" s="2">
+        <v>7532166</v>
+      </c>
+      <c r="F24" s="2">
+        <v>2964109</v>
+      </c>
+      <c r="G24" s="2">
+        <v>220907</v>
+      </c>
+      <c r="H24" s="4">
+        <v>0.93059999999999998</v>
+      </c>
+      <c r="I24">
+        <v>19.87</v>
+      </c>
+      <c r="J24" t="s">
+        <v>292</v>
+      </c>
+      <c r="K24" t="s">
+        <v>99</v>
+      </c>
+      <c r="L24" t="s">
+        <v>124</v>
+      </c>
+      <c r="M24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="C25" s="2">
+        <v>25552</v>
+      </c>
+      <c r="D25" s="2">
+        <v>2150952561</v>
+      </c>
+      <c r="E25" s="2">
+        <v>2038782</v>
+      </c>
+      <c r="F25" s="2">
+        <v>1330598</v>
+      </c>
+      <c r="G25" s="2">
+        <v>226904</v>
+      </c>
+      <c r="H25" s="4">
+        <v>0.85430000000000006</v>
+      </c>
+      <c r="I25">
+        <v>9.44</v>
+      </c>
+      <c r="J25" t="s">
+        <v>294</v>
+      </c>
+      <c r="K25" t="s">
+        <v>101</v>
+      </c>
+      <c r="L25" t="s">
+        <v>131</v>
+      </c>
+      <c r="M25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="C26" s="2">
+        <v>25254</v>
+      </c>
+      <c r="D26" s="2">
+        <v>305151668</v>
+      </c>
+      <c r="E26" s="2">
+        <v>200221</v>
+      </c>
+      <c r="F26" s="2">
+        <v>209221</v>
+      </c>
+      <c r="G26" s="2">
+        <v>17924</v>
+      </c>
+      <c r="H26" s="4">
+        <v>0.92110000000000003</v>
+      </c>
+      <c r="I26">
+        <v>23.53</v>
+      </c>
+      <c r="J26" t="s">
+        <v>296</v>
+      </c>
+      <c r="K26" t="s">
+        <v>99</v>
+      </c>
+      <c r="L26" t="s">
+        <v>297</v>
+      </c>
+      <c r="M26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C27" s="2">
+        <v>23708</v>
+      </c>
+      <c r="D27" s="2">
+        <v>224948798</v>
+      </c>
+      <c r="E27" s="2">
+        <v>3688400</v>
+      </c>
+      <c r="F27" s="2">
+        <v>859754</v>
+      </c>
+      <c r="G27" s="2">
+        <v>17840</v>
+      </c>
+      <c r="H27" s="4">
+        <v>0.97970000000000002</v>
+      </c>
+      <c r="I27">
+        <v>17.670000000000002</v>
+      </c>
+      <c r="J27" t="s">
+        <v>299</v>
+      </c>
+      <c r="K27" t="s">
+        <v>167</v>
+      </c>
+      <c r="L27" t="s">
+        <v>114</v>
+      </c>
+      <c r="M27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C28" s="2">
+        <v>23505</v>
+      </c>
+      <c r="D28" s="2">
+        <v>8814396111</v>
+      </c>
+      <c r="E28" s="2">
+        <v>13474770</v>
+      </c>
+      <c r="F28" s="2">
+        <v>5235321</v>
+      </c>
+      <c r="G28" s="2">
+        <v>706279</v>
+      </c>
+      <c r="H28" s="4">
+        <v>0.88109999999999999</v>
+      </c>
+      <c r="I28">
+        <v>22.76</v>
+      </c>
+      <c r="J28" t="s">
+        <v>300</v>
+      </c>
+      <c r="K28" t="s">
+        <v>98</v>
+      </c>
+      <c r="L28" t="s">
+        <v>115</v>
+      </c>
+      <c r="M28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C29" s="2">
+        <v>21635</v>
+      </c>
+      <c r="D29" s="2">
+        <v>22145433</v>
+      </c>
+      <c r="E29" s="2">
+        <v>50548</v>
+      </c>
+      <c r="F29" s="2">
+        <v>32603</v>
+      </c>
+      <c r="G29" s="2">
+        <v>2677</v>
+      </c>
+      <c r="H29" s="4">
+        <v>0.92409999999999992</v>
+      </c>
+      <c r="I29">
+        <v>22.01</v>
+      </c>
+      <c r="J29" t="s">
+        <v>302</v>
+      </c>
+      <c r="K29" t="s">
+        <v>99</v>
+      </c>
+      <c r="L29" t="s">
+        <v>303</v>
+      </c>
+      <c r="M29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="2">
+        <v>21206</v>
+      </c>
+      <c r="D30" s="2">
+        <v>2550278028</v>
+      </c>
+      <c r="E30" s="2">
+        <v>2887818</v>
+      </c>
+      <c r="F30" s="2">
+        <v>2077616</v>
+      </c>
+      <c r="G30" s="2">
+        <v>159424</v>
+      </c>
+      <c r="H30" s="4">
+        <v>0.92870000000000008</v>
+      </c>
+      <c r="I30">
+        <v>9.86</v>
+      </c>
+      <c r="J30" t="s">
+        <v>274</v>
+      </c>
+      <c r="K30" t="s">
+        <v>165</v>
+      </c>
+      <c r="L30" t="s">
+        <v>129</v>
+      </c>
+      <c r="M30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="2">
+        <v>21136</v>
+      </c>
+      <c r="D31" s="2">
+        <v>823275247</v>
+      </c>
+      <c r="E31" s="2">
+        <v>16565979</v>
+      </c>
+      <c r="F31" s="2">
+        <v>139248</v>
+      </c>
+      <c r="G31" s="2">
+        <v>21216</v>
+      </c>
+      <c r="H31" s="4">
+        <v>0.86780000000000002</v>
+      </c>
+      <c r="I31">
+        <v>18.53</v>
+      </c>
+      <c r="J31" t="s">
+        <v>304</v>
+      </c>
+      <c r="K31" t="s">
+        <v>98</v>
+      </c>
+      <c r="L31" t="s">
+        <v>128</v>
+      </c>
+      <c r="M31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C32" s="2">
+        <v>20925</v>
+      </c>
+      <c r="D32" s="2">
+        <v>84734150</v>
+      </c>
+      <c r="E32" s="2">
+        <v>2126376</v>
+      </c>
+      <c r="F32" s="2">
+        <v>595242</v>
+      </c>
+      <c r="G32" s="2">
+        <v>29953</v>
+      </c>
+      <c r="H32" s="4">
+        <v>0.95209999999999995</v>
+      </c>
+      <c r="I32">
+        <v>6.12</v>
+      </c>
+      <c r="J32" t="s">
+        <v>305</v>
+      </c>
+      <c r="K32" t="s">
+        <v>247</v>
+      </c>
+      <c r="L32" t="s">
+        <v>248</v>
+      </c>
+      <c r="M32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C33" s="2">
+        <v>20786</v>
+      </c>
+      <c r="D33" s="2">
+        <v>33396102</v>
+      </c>
+      <c r="E33" s="2">
+        <v>452960</v>
+      </c>
+      <c r="F33" s="2">
+        <v>140636</v>
+      </c>
+      <c r="G33" s="2">
+        <v>6468</v>
+      </c>
+      <c r="H33" s="4">
+        <v>0.95599999999999996</v>
+      </c>
+      <c r="I33">
+        <v>15.92</v>
+      </c>
+      <c r="J33" t="s">
+        <v>306</v>
+      </c>
+      <c r="K33" t="s">
+        <v>100</v>
+      </c>
+      <c r="L33" t="s">
+        <v>251</v>
+      </c>
+      <c r="M33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C34" s="2">
+        <v>20165</v>
+      </c>
+      <c r="D34" s="2">
+        <v>839708636</v>
+      </c>
+      <c r="E34" s="2">
+        <v>2519706</v>
+      </c>
+      <c r="F34" s="2">
+        <v>562343</v>
+      </c>
+      <c r="G34" s="2">
+        <v>66130</v>
+      </c>
+      <c r="H34" s="4">
+        <v>0.89480000000000004</v>
+      </c>
+      <c r="I34">
+        <v>24.23</v>
+      </c>
+      <c r="J34" t="s">
+        <v>308</v>
+      </c>
+      <c r="K34" t="s">
+        <v>185</v>
+      </c>
+      <c r="L34" t="s">
+        <v>134</v>
+      </c>
+      <c r="M34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C35" s="2">
+        <v>17889</v>
+      </c>
+      <c r="D35" s="2">
+        <v>860915389</v>
+      </c>
+      <c r="E35" s="2">
+        <v>1064670</v>
+      </c>
+      <c r="F35" s="2">
+        <v>1314089</v>
+      </c>
+      <c r="G35" s="2">
+        <v>116488</v>
+      </c>
+      <c r="H35" s="4">
+        <v>0.91859999999999997</v>
+      </c>
+      <c r="I35">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="J35" t="s">
+        <v>310</v>
+      </c>
+      <c r="K35" t="s">
+        <v>99</v>
+      </c>
+      <c r="L35" t="s">
+        <v>125</v>
+      </c>
+      <c r="M35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="C36" s="2">
+        <v>17061</v>
+      </c>
+      <c r="D36" s="2">
+        <v>528477503</v>
+      </c>
+      <c r="E36" s="2">
+        <v>691241</v>
+      </c>
+      <c r="F36" s="2">
+        <v>595269</v>
+      </c>
+      <c r="G36" s="2">
+        <v>96787</v>
+      </c>
+      <c r="H36" s="4">
+        <v>0.86010000000000009</v>
+      </c>
+      <c r="I36">
+        <v>13.19</v>
+      </c>
+      <c r="J36" t="s">
+        <v>311</v>
+      </c>
+      <c r="K36" t="s">
+        <v>101</v>
+      </c>
+      <c r="L36" t="s">
+        <v>126</v>
+      </c>
+      <c r="M36" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C37" s="2">
+        <v>16103</v>
+      </c>
+      <c r="D37" s="2">
+        <v>2404954316</v>
+      </c>
+      <c r="E37" s="2">
+        <v>2402322</v>
+      </c>
+      <c r="F37" s="2">
+        <v>555240</v>
+      </c>
+      <c r="G37" s="2">
+        <v>182393</v>
+      </c>
+      <c r="H37" s="4">
+        <v>0.75269999999999992</v>
+      </c>
+      <c r="I37">
+        <v>22.8</v>
+      </c>
+      <c r="J37" t="s">
+        <v>312</v>
+      </c>
+      <c r="K37" t="s">
+        <v>98</v>
+      </c>
+      <c r="L37" t="s">
+        <v>199</v>
+      </c>
+      <c r="M37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C38" s="2">
+        <v>15973</v>
+      </c>
+      <c r="D38" s="2">
+        <v>6966078799</v>
+      </c>
+      <c r="E38" s="2">
+        <v>18202097</v>
+      </c>
+      <c r="F38" s="2">
+        <v>5471078</v>
+      </c>
+      <c r="G38" s="2">
+        <v>759312</v>
+      </c>
+      <c r="H38" s="4">
+        <v>0.87809999999999999</v>
+      </c>
+      <c r="I38">
+        <v>14.48</v>
+      </c>
+      <c r="J38" t="s">
+        <v>313</v>
+      </c>
+      <c r="K38" t="s">
+        <v>98</v>
+      </c>
+      <c r="L38" t="s">
+        <v>137</v>
+      </c>
+      <c r="M38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C39" s="2">
+        <v>15620</v>
+      </c>
+      <c r="D39" s="2">
+        <v>4561781536</v>
+      </c>
+      <c r="E39" s="2">
+        <v>21108197</v>
+      </c>
+      <c r="F39" s="2">
+        <v>1229762</v>
+      </c>
+      <c r="G39" s="2">
+        <v>133069</v>
+      </c>
+      <c r="H39" s="4">
+        <v>0.90239999999999998</v>
+      </c>
+      <c r="I39">
+        <v>16.649999999999999</v>
+      </c>
+      <c r="J39" t="s">
+        <v>314</v>
+      </c>
+      <c r="K39" t="s">
+        <v>98</v>
+      </c>
+      <c r="L39" t="s">
+        <v>132</v>
+      </c>
+      <c r="M39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40" s="2">
+        <v>15607</v>
+      </c>
+      <c r="D40" s="2">
+        <v>2545868303</v>
+      </c>
+      <c r="E40" s="2">
+        <v>1132321</v>
+      </c>
+      <c r="F40" s="2">
+        <v>260860</v>
+      </c>
+      <c r="G40" s="2">
+        <v>187303</v>
+      </c>
+      <c r="H40" s="4">
+        <v>0.58210000000000006</v>
+      </c>
+      <c r="I40">
+        <v>9.69</v>
+      </c>
+      <c r="J40" t="s">
+        <v>315</v>
+      </c>
+      <c r="K40" t="s">
+        <v>99</v>
+      </c>
+      <c r="L40" t="s">
+        <v>133</v>
+      </c>
+      <c r="M40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C41" s="2">
+        <v>15569</v>
+      </c>
+      <c r="D41" s="2">
+        <v>5092782393</v>
+      </c>
+      <c r="E41" s="2">
+        <v>6266920</v>
+      </c>
+      <c r="F41" s="2">
+        <v>3523840</v>
+      </c>
+      <c r="G41" s="2">
+        <v>249308</v>
+      </c>
+      <c r="H41" s="4">
+        <v>0.93389999999999995</v>
+      </c>
+      <c r="I41">
+        <v>8.64</v>
+      </c>
+      <c r="J41" t="s">
+        <v>316</v>
+      </c>
+      <c r="K41" t="s">
+        <v>99</v>
+      </c>
+      <c r="L41" t="s">
+        <v>195</v>
+      </c>
+      <c r="M41" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" s="2">
+        <v>15411</v>
+      </c>
+      <c r="D42" s="2">
+        <v>12884245204</v>
+      </c>
+      <c r="E42" s="2">
+        <v>11588284</v>
+      </c>
+      <c r="F42" s="2">
+        <v>3545107</v>
+      </c>
+      <c r="G42" s="2">
+        <v>397863</v>
+      </c>
+      <c r="H42" s="4">
+        <v>0.89910000000000001</v>
+      </c>
+      <c r="I42">
+        <v>11.1</v>
+      </c>
+      <c r="J42" t="s">
+        <v>317</v>
+      </c>
+      <c r="K42" t="s">
+        <v>100</v>
+      </c>
+      <c r="L42" t="s">
+        <v>144</v>
+      </c>
+      <c r="M42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="2">
+        <v>15153</v>
+      </c>
+      <c r="D43" s="2">
+        <v>12884286490</v>
+      </c>
+      <c r="E43" s="2">
+        <v>11588287</v>
+      </c>
+      <c r="F43" s="2">
+        <v>3545107</v>
+      </c>
+      <c r="G43" s="2">
+        <v>397863</v>
+      </c>
+      <c r="H43" s="4">
+        <v>0.89910000000000001</v>
+      </c>
+      <c r="I43">
+        <v>11.1</v>
+      </c>
+      <c r="J43" t="s">
+        <v>317</v>
+      </c>
+      <c r="K43" t="s">
+        <v>100</v>
+      </c>
+      <c r="L43" t="s">
+        <v>144</v>
+      </c>
+      <c r="M43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44" s="2">
+        <v>15068</v>
+      </c>
+      <c r="D44" s="2">
+        <v>3049225856</v>
+      </c>
+      <c r="E44" s="2">
+        <v>2247852</v>
+      </c>
+      <c r="F44" s="2">
+        <v>1294088</v>
+      </c>
+      <c r="G44" s="2">
+        <v>131497</v>
+      </c>
+      <c r="H44" s="4">
+        <v>0.90780000000000005</v>
+      </c>
+      <c r="I44">
+        <v>17.3</v>
+      </c>
+      <c r="J44" t="s">
+        <v>318</v>
+      </c>
+      <c r="K44" t="s">
+        <v>99</v>
+      </c>
+      <c r="L44" t="s">
+        <v>146</v>
+      </c>
+      <c r="M44" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C45" s="2">
+        <v>14860</v>
+      </c>
+      <c r="D45" s="2">
+        <v>856012261</v>
+      </c>
+      <c r="E45" s="2">
+        <v>577971</v>
+      </c>
+      <c r="F45" s="2">
+        <v>246326</v>
+      </c>
+      <c r="G45" s="2">
+        <v>45293</v>
+      </c>
+      <c r="H45" s="4">
+        <v>0.84470000000000001</v>
+      </c>
+      <c r="I45">
+        <v>11.37</v>
+      </c>
+      <c r="J45" t="s">
+        <v>319</v>
+      </c>
+      <c r="K45" t="s">
+        <v>101</v>
+      </c>
+      <c r="L45" t="s">
+        <v>140</v>
+      </c>
+      <c r="M45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C46" s="2">
+        <v>14500</v>
+      </c>
+      <c r="D46" s="2">
+        <v>993329561</v>
+      </c>
+      <c r="E46" s="2">
+        <v>1550709</v>
+      </c>
+      <c r="F46" s="2">
+        <v>477958</v>
+      </c>
+      <c r="G46" s="2">
+        <v>141034</v>
+      </c>
+      <c r="H46" s="4">
+        <v>0.7722</v>
+      </c>
+      <c r="I46">
+        <v>12.92</v>
+      </c>
+      <c r="J46" t="s">
+        <v>321</v>
+      </c>
+      <c r="K46" t="s">
+        <v>322</v>
+      </c>
+      <c r="L46" t="s">
+        <v>323</v>
+      </c>
+      <c r="M46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C47" s="2">
+        <v>14021</v>
+      </c>
+      <c r="D47" s="2">
+        <v>23495706846</v>
+      </c>
+      <c r="E47" s="2">
+        <v>11114427</v>
+      </c>
+      <c r="F47" s="2">
+        <v>3812449</v>
+      </c>
+      <c r="G47" s="2">
+        <v>1325135</v>
+      </c>
+      <c r="H47" s="4">
+        <v>0.74209999999999998</v>
+      </c>
+      <c r="I47">
+        <v>4.21</v>
+      </c>
+      <c r="J47" t="s">
+        <v>324</v>
+      </c>
+      <c r="K47" t="s">
+        <v>99</v>
+      </c>
+      <c r="L47" t="s">
+        <v>143</v>
+      </c>
+      <c r="M47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C48" s="2">
+        <v>13927</v>
+      </c>
+      <c r="D48" s="2">
+        <v>1402084023</v>
+      </c>
+      <c r="E48" s="2">
+        <v>10146953</v>
+      </c>
+      <c r="F48" s="2">
+        <v>1363900</v>
+      </c>
+      <c r="G48" s="2">
+        <v>101614</v>
+      </c>
+      <c r="H48" s="4">
+        <v>0.93069999999999997</v>
+      </c>
+      <c r="I48">
+        <v>13.74</v>
+      </c>
+      <c r="J48" t="s">
+        <v>326</v>
+      </c>
+      <c r="K48" t="s">
+        <v>99</v>
+      </c>
+      <c r="L48" t="s">
+        <v>148</v>
+      </c>
+      <c r="M48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C49" s="2">
+        <v>13498</v>
+      </c>
+      <c r="D49" s="2">
+        <v>91516003</v>
+      </c>
+      <c r="E49" s="2">
+        <v>120757</v>
+      </c>
+      <c r="F49" s="2">
+        <v>82659</v>
+      </c>
+      <c r="G49" s="2">
+        <v>8364</v>
+      </c>
+      <c r="H49" s="4">
+        <v>0.90810000000000002</v>
+      </c>
+      <c r="I49">
+        <v>9.7899999999999991</v>
+      </c>
+      <c r="J49" t="s">
+        <v>328</v>
+      </c>
+      <c r="K49" t="s">
+        <v>168</v>
+      </c>
+      <c r="L49" t="s">
+        <v>139</v>
+      </c>
+      <c r="M49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C50" s="2">
+        <v>13313</v>
+      </c>
+      <c r="D50" s="2">
+        <v>949400870</v>
+      </c>
+      <c r="E50" s="2">
+        <v>857811</v>
+      </c>
+      <c r="F50" s="2">
+        <v>1117424</v>
+      </c>
+      <c r="G50" s="2">
+        <v>54586</v>
+      </c>
+      <c r="H50" s="4">
+        <v>0.95340000000000003</v>
+      </c>
+      <c r="I50">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="J50" t="s">
+        <v>329</v>
+      </c>
+      <c r="K50" t="s">
+        <v>167</v>
+      </c>
+      <c r="L50" t="s">
+        <v>141</v>
+      </c>
+      <c r="M50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C51" s="2">
+        <v>13138</v>
+      </c>
+      <c r="D51" s="2">
+        <v>41234013</v>
+      </c>
+      <c r="E51" s="2">
+        <v>108841</v>
+      </c>
+      <c r="F51" s="2">
+        <v>45902</v>
+      </c>
+      <c r="G51" s="2">
+        <v>3708</v>
+      </c>
+      <c r="H51" s="4">
+        <v>0.92530000000000001</v>
+      </c>
+      <c r="I51">
+        <v>13.11</v>
+      </c>
+      <c r="J51" t="s">
+        <v>331</v>
+      </c>
+      <c r="K51" t="s">
+        <v>100</v>
+      </c>
+      <c r="L51" t="s">
+        <v>332</v>
+      </c>
+      <c r="M51" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C52" s="2">
+        <v>12865</v>
+      </c>
+      <c r="D52" s="2">
+        <v>3534971607</v>
+      </c>
+      <c r="E52" s="2">
+        <v>3117442</v>
+      </c>
+      <c r="F52" s="2">
+        <v>1272561</v>
+      </c>
+      <c r="G52" s="2">
+        <v>272528</v>
+      </c>
+      <c r="H52" s="4">
+        <v>0.8236</v>
+      </c>
+      <c r="I52">
+        <v>8.19</v>
+      </c>
+      <c r="J52" t="s">
+        <v>333</v>
+      </c>
+      <c r="K52" t="s">
+        <v>100</v>
+      </c>
+      <c r="L52" t="s">
+        <v>145</v>
+      </c>
+      <c r="M52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:M1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B937581-5BFE-0C43-9A8A-CAE8581C0F34}">
   <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3375,7 +5722,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D4922F-A22D-1547-8F5C-336FD651258D}">
   <dimension ref="A1:M55"/>
   <sheetViews>
@@ -5637,7 +7984,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M52"/>
   <sheetViews>
@@ -7779,7 +10126,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CD5A4D4-8172-B14E-80EB-29CD406E771F}">
   <dimension ref="A1:M52"/>
   <sheetViews>

</xml_diff>

<commit_message>
fixed roblox data format
</commit_message>
<xml_diff>
--- a/data/total_roblox_experiences.xlsx
+++ b/data/total_roblox_experiences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenwang/Desktop/Makers/Steam_Roblox_Streamlit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4F3BBE-313F-2F46-A128-9CC4C22A2A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E472DA82-4A5F-5E42-A228-544BA103E374}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5840" yWindow="1100" windowWidth="23460" windowHeight="18020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1132" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="287">
   <si>
     <t>#1</t>
   </si>
@@ -818,214 +818,73 @@
     <t>[BULLET] untitled boxing game🥊</t>
   </si>
   <si>
-    <t>Top Experiences 50 on Roblox (Data fetched from RoMonitor as of 02:22 AM EDT, 2024-07-29)</t>
-  </si>
-  <si>
-    <t>January 15, 2019</t>
-  </si>
-  <si>
-    <t>April 20, 2020</t>
-  </si>
-  <si>
-    <t>April 4, 2024</t>
-  </si>
-  <si>
-    <t>January 17, 2014</t>
-  </si>
-  <si>
-    <t>August 1, 2022</t>
-  </si>
-  <si>
-    <t>October 17, 2023</t>
-  </si>
-  <si>
     <t>[🎁x2 Event] Bee Swarm Simulator</t>
   </si>
   <si>
-    <t>March 20, 2018</t>
-  </si>
-  <si>
     <t>Pet Simulator 99! 🍍</t>
   </si>
   <si>
-    <t>February 4, 2022</t>
-  </si>
-  <si>
-    <t>July 13, 2017</t>
-  </si>
-  <si>
     <t>[TEN SHADOWS] Jujutsu Shenanigans</t>
   </si>
   <si>
-    <t>April 16, 2022</t>
-  </si>
-  <si>
-    <t>January 6, 2022</t>
-  </si>
-  <si>
-    <t>December 2, 2023</t>
-  </si>
-  <si>
     <t>TYPE://SOUL [UPDATE PART 2]</t>
   </si>
   <si>
-    <t>July 14, 2023</t>
-  </si>
-  <si>
-    <t>June 9, 2022</t>
-  </si>
-  <si>
-    <t>June 16, 2023</t>
-  </si>
-  <si>
     <t>BedWars [😇 TRINITY REWORK]</t>
   </si>
   <si>
-    <t>May 26, 2021</t>
-  </si>
-  <si>
-    <t>July 2, 2021</t>
-  </si>
-  <si>
     <t>LifeTogether 🏠 RP (UPDATE 21)</t>
   </si>
   <si>
-    <t>July 4, 2023</t>
-  </si>
-  <si>
     <t>[UPD 📱] Baddies 💅</t>
   </si>
   <si>
-    <t>October 2, 2022</t>
-  </si>
-  <si>
-    <t>January 20, 2019</t>
-  </si>
-  <si>
-    <t>November 1, 2016</t>
-  </si>
-  <si>
     <t>[KILLSTREAK 1000] Slap Battles👏</t>
   </si>
   <si>
-    <t>February 15, 2021</t>
-  </si>
-  <si>
     <t>[⭐ x4 + CODE] Anime Last Stand</t>
   </si>
   <si>
-    <t>March 23, 2023</t>
-  </si>
-  <si>
     <t>[B:S] ALS Team</t>
   </si>
   <si>
     <t>[EVENT] Gym League</t>
   </si>
   <si>
-    <t>May 9, 2024</t>
-  </si>
-  <si>
-    <t>November 3, 2014</t>
-  </si>
-  <si>
     <t>[UPDATE 4] Meme Sea</t>
   </si>
   <si>
-    <t>July 16, 2022</t>
-  </si>
-  <si>
     <t>Meme Sea Group</t>
   </si>
   <si>
-    <t>April 2, 2023</t>
-  </si>
-  <si>
-    <t>May 25, 2024</t>
-  </si>
-  <si>
-    <t>February 6, 2023</t>
-  </si>
-  <si>
     <t>🌊 Creatures of Sonaria 💙 Survive Kaiju Animals</t>
   </si>
   <si>
-    <t>June 24, 2020</t>
-  </si>
-  <si>
     <t>a dusty trip [🤠 BOSS]</t>
   </si>
   <si>
-    <t>February 15, 2024</t>
-  </si>
-  <si>
-    <t>June 1, 2023</t>
-  </si>
-  <si>
-    <t>July 4, 2020</t>
-  </si>
-  <si>
-    <t>January 5, 2017</t>
-  </si>
-  <si>
-    <t>April 27, 2021</t>
-  </si>
-  <si>
-    <t>February 1, 2022</t>
-  </si>
-  <si>
-    <t>March 13, 2021</t>
-  </si>
-  <si>
-    <t>January 22, 2020</t>
-  </si>
-  <si>
-    <t>December 16, 2019</t>
-  </si>
-  <si>
-    <t>February 1, 2023</t>
-  </si>
-  <si>
     <t>Fling Things and People</t>
   </si>
   <si>
-    <t>June 16, 2021</t>
-  </si>
-  <si>
     <t>Comedy</t>
   </si>
   <si>
     <t>Horomori</t>
   </si>
   <si>
-    <t>June 17, 2018</t>
-  </si>
-  <si>
     <t>[LIMITED✨] Driving Empire 🏎️ Car Racing</t>
   </si>
   <si>
-    <t>June 22, 2019</t>
-  </si>
-  <si>
     <t>Five Nights TD [MILITARY]</t>
   </si>
   <si>
-    <t>January 1, 2024</t>
-  </si>
-  <si>
-    <t>April 13, 2023</t>
-  </si>
-  <si>
     <t>🐚Dandy's World [ALPHA]</t>
   </si>
   <si>
-    <t>January 25, 2024</t>
-  </si>
-  <si>
     <t>BlushCrunch Studio</t>
   </si>
   <si>
-    <t>November 13, 2021</t>
+    <t>Top Experiences 50 on Roblox (Data fetched from RoMonitor as of 10:18 AM EDT, 2024-07-29)</t>
   </si>
 </sst>
 </file>
@@ -1451,25 +1310,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99C60782-7F66-D04D-A716-667EE5D461B9}">
   <dimension ref="A1:M52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="30.6640625" style="1" customWidth="1"/>
-    <col min="3" max="7" width="18.6640625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="18.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="3" customWidth="1"/>
+    <col min="6" max="7" width="18.6640625" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" style="4" customWidth="1"/>
-    <col min="9" max="10" width="12.6640625" customWidth="1"/>
-    <col min="11" max="11" width="20.6640625" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" style="2" customWidth="1"/>
     <col min="13" max="13" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
-        <v>264</v>
+        <v>286</v>
       </c>
       <c r="B1" s="13"/>
       <c r="C1" s="13"/>
@@ -1498,13 +1360,13 @@
         <v>153</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="H2" s="5" t="s">
         <v>157</v>
@@ -1513,13 +1375,13 @@
         <v>158</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="M2" s="5" t="s">
         <v>162</v>
@@ -1538,14 +1400,14 @@
       <c r="D3" s="2">
         <v>37191190699</v>
       </c>
-      <c r="E3" s="2">
-        <v>12781988</v>
-      </c>
-      <c r="F3" s="2">
-        <v>7812016</v>
-      </c>
-      <c r="G3" s="2">
-        <v>596308</v>
+      <c r="E3" s="3">
+        <v>43480</v>
+      </c>
+      <c r="F3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G3" t="s">
+        <v>104</v>
       </c>
       <c r="H3" s="4">
         <v>0.92909999999999993</v>
@@ -1553,14 +1415,14 @@
       <c r="I3">
         <v>16.18</v>
       </c>
-      <c r="J3" t="s">
-        <v>265</v>
-      </c>
-      <c r="K3" t="s">
-        <v>99</v>
-      </c>
-      <c r="L3" t="s">
-        <v>104</v>
+      <c r="J3" s="2">
+        <v>12781988</v>
+      </c>
+      <c r="K3" s="2">
+        <v>7812016</v>
+      </c>
+      <c r="L3" s="2">
+        <v>596308</v>
       </c>
       <c r="M3" t="b">
         <v>0</v>
@@ -1579,14 +1441,14 @@
       <c r="D4" s="2">
         <v>51546629458</v>
       </c>
-      <c r="E4" s="2">
-        <v>21420731</v>
-      </c>
-      <c r="F4" s="2">
-        <v>5754306</v>
-      </c>
-      <c r="G4" s="2">
-        <v>890025</v>
+      <c r="E4" s="3">
+        <v>43941</v>
+      </c>
+      <c r="F4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" t="s">
+        <v>103</v>
       </c>
       <c r="H4" s="4">
         <v>0.86599999999999999</v>
@@ -1594,14 +1456,14 @@
       <c r="I4">
         <v>17.29</v>
       </c>
-      <c r="J4" t="s">
-        <v>266</v>
-      </c>
-      <c r="K4" t="s">
-        <v>98</v>
-      </c>
-      <c r="L4" t="s">
-        <v>103</v>
+      <c r="J4" s="2">
+        <v>21420731</v>
+      </c>
+      <c r="K4" s="2">
+        <v>5754306</v>
+      </c>
+      <c r="L4" s="2">
+        <v>890025</v>
       </c>
       <c r="M4" t="b">
         <v>0</v>
@@ -1620,14 +1482,14 @@
       <c r="D5" s="2">
         <v>1371411535</v>
       </c>
-      <c r="E5" s="2">
-        <v>541797</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1613146</v>
-      </c>
-      <c r="G5" s="2">
-        <v>40072</v>
+      <c r="E5" s="3">
+        <v>45386</v>
+      </c>
+      <c r="F5" t="s">
+        <v>168</v>
+      </c>
+      <c r="G5" t="s">
+        <v>105</v>
       </c>
       <c r="H5" s="4">
         <v>0.9758</v>
@@ -1635,14 +1497,14 @@
       <c r="I5">
         <v>15.45</v>
       </c>
-      <c r="J5" t="s">
-        <v>267</v>
-      </c>
-      <c r="K5" t="s">
-        <v>168</v>
-      </c>
-      <c r="L5" t="s">
-        <v>105</v>
+      <c r="J5" s="2">
+        <v>541797</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1613146</v>
+      </c>
+      <c r="L5" s="2">
+        <v>40072</v>
       </c>
       <c r="M5" t="b">
         <v>1</v>
@@ -1661,14 +1523,14 @@
       <c r="D6" s="2">
         <v>16278459940</v>
       </c>
-      <c r="E6" s="2">
-        <v>18589623</v>
-      </c>
-      <c r="F6" s="2">
-        <v>7481912</v>
-      </c>
-      <c r="G6" s="2">
-        <v>723097</v>
+      <c r="E6" s="3">
+        <v>41656</v>
+      </c>
+      <c r="F6" t="s">
+        <v>100</v>
+      </c>
+      <c r="G6" t="s">
+        <v>106</v>
       </c>
       <c r="H6" s="4">
         <v>0.91189999999999993</v>
@@ -1676,14 +1538,14 @@
       <c r="I6">
         <v>12.86</v>
       </c>
-      <c r="J6" t="s">
-        <v>268</v>
-      </c>
-      <c r="K6" t="s">
-        <v>100</v>
-      </c>
-      <c r="L6" t="s">
-        <v>106</v>
+      <c r="J6" s="2">
+        <v>18589623</v>
+      </c>
+      <c r="K6" s="2">
+        <v>7481912</v>
+      </c>
+      <c r="L6" s="2">
+        <v>723097</v>
       </c>
       <c r="M6" t="b">
         <v>1</v>
@@ -1702,14 +1564,14 @@
       <c r="D7" s="2">
         <v>6664536140</v>
       </c>
-      <c r="E7" s="2">
-        <v>3463774</v>
-      </c>
-      <c r="F7" s="2">
-        <v>2371578</v>
-      </c>
-      <c r="G7" s="2">
-        <v>450781</v>
+      <c r="E7" s="3">
+        <v>44774</v>
+      </c>
+      <c r="F7" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7" t="s">
+        <v>108</v>
       </c>
       <c r="H7" s="4">
         <v>0.84030000000000005</v>
@@ -1717,14 +1579,14 @@
       <c r="I7">
         <v>9.52</v>
       </c>
-      <c r="J7" t="s">
-        <v>269</v>
-      </c>
-      <c r="K7" t="s">
-        <v>101</v>
-      </c>
-      <c r="L7" t="s">
-        <v>108</v>
+      <c r="J7" s="2">
+        <v>3463774</v>
+      </c>
+      <c r="K7" s="2">
+        <v>2371578</v>
+      </c>
+      <c r="L7" s="2">
+        <v>450781</v>
       </c>
       <c r="M7" t="b">
         <v>1</v>
@@ -1743,14 +1605,14 @@
       <c r="D8" s="2">
         <v>1536110208</v>
       </c>
-      <c r="E8" s="2">
-        <v>1535854</v>
-      </c>
-      <c r="F8" s="2">
-        <v>863496</v>
-      </c>
-      <c r="G8" s="2">
-        <v>84899</v>
+      <c r="E8" s="3">
+        <v>45216</v>
+      </c>
+      <c r="F8" t="s">
+        <v>164</v>
+      </c>
+      <c r="G8" t="s">
+        <v>110</v>
       </c>
       <c r="H8" s="4">
         <v>0.91049999999999998</v>
@@ -1758,14 +1620,14 @@
       <c r="I8">
         <v>15.24</v>
       </c>
-      <c r="J8" t="s">
-        <v>270</v>
-      </c>
-      <c r="K8" t="s">
-        <v>164</v>
-      </c>
-      <c r="L8" t="s">
-        <v>110</v>
+      <c r="J8" s="2">
+        <v>1535854</v>
+      </c>
+      <c r="K8" s="2">
+        <v>863496</v>
+      </c>
+      <c r="L8" s="2">
+        <v>84899</v>
       </c>
       <c r="M8" t="b">
         <v>1</v>
@@ -1776,7 +1638,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="C9" s="2">
         <v>103126</v>
@@ -1784,14 +1646,14 @@
       <c r="D9" s="2">
         <v>2785155338</v>
       </c>
-      <c r="E9" s="2">
-        <v>5876916</v>
-      </c>
-      <c r="F9" s="2">
-        <v>2226562</v>
-      </c>
-      <c r="G9" s="2">
-        <v>118450</v>
+      <c r="E9" s="3">
+        <v>43179</v>
+      </c>
+      <c r="F9" t="s">
+        <v>99</v>
+      </c>
+      <c r="G9" t="s">
+        <v>121</v>
       </c>
       <c r="H9" s="4">
         <v>0.94950000000000001</v>
@@ -1799,14 +1661,14 @@
       <c r="I9">
         <v>40.64</v>
       </c>
-      <c r="J9" t="s">
-        <v>272</v>
-      </c>
-      <c r="K9" t="s">
-        <v>99</v>
-      </c>
-      <c r="L9" t="s">
-        <v>121</v>
+      <c r="J9" s="2">
+        <v>5876916</v>
+      </c>
+      <c r="K9" s="2">
+        <v>2226562</v>
+      </c>
+      <c r="L9" s="2">
+        <v>118450</v>
       </c>
       <c r="M9" t="b">
         <v>0</v>
@@ -1817,7 +1679,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="C10" s="2">
         <v>102905</v>
@@ -1825,14 +1687,14 @@
       <c r="D10" s="2">
         <v>1280546290</v>
       </c>
-      <c r="E10" s="2">
-        <v>1341397</v>
-      </c>
-      <c r="F10" s="2">
-        <v>2378754</v>
-      </c>
-      <c r="G10" s="2">
-        <v>88417</v>
+      <c r="E10" s="3">
+        <v>44596</v>
+      </c>
+      <c r="F10" t="s">
+        <v>163</v>
+      </c>
+      <c r="G10" t="s">
+        <v>109</v>
       </c>
       <c r="H10" s="4">
         <v>0.96420000000000006</v>
@@ -1840,14 +1702,14 @@
       <c r="I10">
         <v>51.22</v>
       </c>
-      <c r="J10" t="s">
-        <v>274</v>
-      </c>
-      <c r="K10" t="s">
-        <v>163</v>
-      </c>
-      <c r="L10" t="s">
-        <v>109</v>
+      <c r="J10" s="2">
+        <v>1341397</v>
+      </c>
+      <c r="K10" s="2">
+        <v>2378754</v>
+      </c>
+      <c r="L10" s="2">
+        <v>88417</v>
       </c>
       <c r="M10" t="b">
         <v>1</v>
@@ -1866,14 +1728,14 @@
       <c r="D11" s="2">
         <v>36927790087</v>
       </c>
-      <c r="E11" s="2">
-        <v>26844319</v>
-      </c>
-      <c r="F11" s="2">
-        <v>7177490</v>
-      </c>
-      <c r="G11" s="2">
-        <v>1419165</v>
+      <c r="E11" s="3">
+        <v>42929</v>
+      </c>
+      <c r="F11" t="s">
+        <v>102</v>
+      </c>
+      <c r="G11" t="s">
+        <v>111</v>
       </c>
       <c r="H11" s="4">
         <v>0.83489999999999998</v>
@@ -1881,14 +1743,14 @@
       <c r="I11">
         <v>19.07</v>
       </c>
-      <c r="J11" t="s">
-        <v>275</v>
-      </c>
-      <c r="K11" t="s">
-        <v>102</v>
-      </c>
-      <c r="L11" t="s">
-        <v>111</v>
+      <c r="J11" s="2">
+        <v>26844319</v>
+      </c>
+      <c r="K11" s="2">
+        <v>7177490</v>
+      </c>
+      <c r="L11" s="2">
+        <v>1419165</v>
       </c>
       <c r="M11" t="b">
         <v>0</v>
@@ -1899,7 +1761,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="C12" s="2">
         <v>72236</v>
@@ -1907,14 +1769,14 @@
       <c r="D12" s="2">
         <v>459123815</v>
       </c>
-      <c r="E12" s="2">
-        <v>641868</v>
-      </c>
-      <c r="F12" s="2">
-        <v>461003</v>
-      </c>
-      <c r="G12" s="2">
-        <v>83942</v>
+      <c r="E12" s="3">
+        <v>44667</v>
+      </c>
+      <c r="F12" t="s">
+        <v>101</v>
+      </c>
+      <c r="G12" t="s">
+        <v>120</v>
       </c>
       <c r="H12" s="4">
         <v>0.84599999999999997</v>
@@ -1922,14 +1784,14 @@
       <c r="I12">
         <v>14.1</v>
       </c>
-      <c r="J12" t="s">
-        <v>277</v>
-      </c>
-      <c r="K12" t="s">
-        <v>101</v>
-      </c>
-      <c r="L12" t="s">
-        <v>120</v>
+      <c r="J12" s="2">
+        <v>641868</v>
+      </c>
+      <c r="K12" s="2">
+        <v>461003</v>
+      </c>
+      <c r="L12" s="2">
+        <v>83942</v>
       </c>
       <c r="M12" t="b">
         <v>1</v>
@@ -1940,7 +1802,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="C13" s="2">
         <v>70976</v>
@@ -1948,14 +1810,14 @@
       <c r="D13" s="2">
         <v>459276141</v>
       </c>
-      <c r="E13" s="2">
-        <v>641978</v>
-      </c>
-      <c r="F13" s="2">
-        <v>461003</v>
-      </c>
-      <c r="G13" s="2">
-        <v>83942</v>
+      <c r="E13" s="3">
+        <v>44667</v>
+      </c>
+      <c r="F13" t="s">
+        <v>101</v>
+      </c>
+      <c r="G13" t="s">
+        <v>120</v>
       </c>
       <c r="H13" s="4">
         <v>0.84599999999999997</v>
@@ -1963,14 +1825,14 @@
       <c r="I13">
         <v>14.1</v>
       </c>
-      <c r="J13" t="s">
-        <v>277</v>
-      </c>
-      <c r="K13" t="s">
-        <v>101</v>
-      </c>
-      <c r="L13" t="s">
-        <v>120</v>
+      <c r="J13" s="2">
+        <v>641978</v>
+      </c>
+      <c r="K13" s="2">
+        <v>461003</v>
+      </c>
+      <c r="L13" s="2">
+        <v>83942</v>
       </c>
       <c r="M13" t="b">
         <v>1</v>
@@ -1989,14 +1851,14 @@
       <c r="D14" s="2">
         <v>3764152141</v>
       </c>
-      <c r="E14" s="2">
-        <v>2079318</v>
-      </c>
-      <c r="F14" s="2">
-        <v>584039</v>
-      </c>
-      <c r="G14" s="2">
-        <v>86819</v>
+      <c r="E14" s="3">
+        <v>44567</v>
+      </c>
+      <c r="F14" t="s">
+        <v>98</v>
+      </c>
+      <c r="G14" t="s">
+        <v>113</v>
       </c>
       <c r="H14" s="4">
         <v>0.87060000000000004</v>
@@ -2004,14 +1866,14 @@
       <c r="I14">
         <v>13.99</v>
       </c>
-      <c r="J14" t="s">
-        <v>278</v>
-      </c>
-      <c r="K14" t="s">
-        <v>98</v>
-      </c>
-      <c r="L14" t="s">
-        <v>113</v>
+      <c r="J14" s="2">
+        <v>2079318</v>
+      </c>
+      <c r="K14" s="2">
+        <v>584039</v>
+      </c>
+      <c r="L14" s="2">
+        <v>86819</v>
       </c>
       <c r="M14" t="b">
         <v>0</v>
@@ -2030,14 +1892,14 @@
       <c r="D15" s="2">
         <v>598529126</v>
       </c>
-      <c r="E15" s="2">
-        <v>555340</v>
-      </c>
-      <c r="F15" s="2">
-        <v>611694</v>
-      </c>
-      <c r="G15" s="2">
-        <v>86775</v>
+      <c r="E15" s="3">
+        <v>45262</v>
+      </c>
+      <c r="F15" t="s">
+        <v>169</v>
+      </c>
+      <c r="G15" t="s">
+        <v>107</v>
       </c>
       <c r="H15" s="4">
         <v>0.87580000000000002</v>
@@ -2045,14 +1907,14 @@
       <c r="I15">
         <v>44.39</v>
       </c>
-      <c r="J15" t="s">
-        <v>279</v>
-      </c>
-      <c r="K15" t="s">
-        <v>169</v>
-      </c>
-      <c r="L15" t="s">
-        <v>107</v>
+      <c r="J15" s="2">
+        <v>555340</v>
+      </c>
+      <c r="K15" s="2">
+        <v>611694</v>
+      </c>
+      <c r="L15" s="2">
+        <v>86775</v>
       </c>
       <c r="M15" t="b">
         <v>1</v>
@@ -2063,7 +1925,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="C16" s="2">
         <v>62135</v>
@@ -2071,14 +1933,14 @@
       <c r="D16" s="2">
         <v>405087843</v>
       </c>
-      <c r="E16" s="2">
-        <v>301603</v>
-      </c>
-      <c r="F16" s="2">
-        <v>220439</v>
-      </c>
-      <c r="G16" s="2">
-        <v>50028</v>
+      <c r="E16" s="3">
+        <v>45121</v>
+      </c>
+      <c r="F16" t="s">
+        <v>101</v>
+      </c>
+      <c r="G16" t="s">
+        <v>190</v>
       </c>
       <c r="H16" s="4">
         <v>0.81499999999999995</v>
@@ -2086,14 +1948,14 @@
       <c r="I16">
         <v>33.25</v>
       </c>
-      <c r="J16" t="s">
-        <v>281</v>
-      </c>
-      <c r="K16" t="s">
-        <v>101</v>
-      </c>
-      <c r="L16" t="s">
-        <v>190</v>
+      <c r="J16" s="2">
+        <v>301603</v>
+      </c>
+      <c r="K16" s="2">
+        <v>220439</v>
+      </c>
+      <c r="L16" s="2">
+        <v>50028</v>
       </c>
       <c r="M16" t="b">
         <v>1</v>
@@ -2112,14 +1974,14 @@
       <c r="D17" s="2">
         <v>4534132650</v>
       </c>
-      <c r="E17" s="2">
-        <v>4947577</v>
-      </c>
-      <c r="F17" s="2">
-        <v>1912328</v>
-      </c>
-      <c r="G17" s="2">
-        <v>111700</v>
+      <c r="E17" s="3">
+        <v>44721</v>
+      </c>
+      <c r="F17" t="s">
+        <v>100</v>
+      </c>
+      <c r="G17" t="s">
+        <v>116</v>
       </c>
       <c r="H17" s="4">
         <v>0.94480000000000008</v>
@@ -2127,14 +1989,14 @@
       <c r="I17">
         <v>10.42</v>
       </c>
-      <c r="J17" t="s">
-        <v>282</v>
-      </c>
-      <c r="K17" t="s">
-        <v>100</v>
-      </c>
-      <c r="L17" t="s">
-        <v>116</v>
+      <c r="J17" s="2">
+        <v>4947577</v>
+      </c>
+      <c r="K17" s="2">
+        <v>1912328</v>
+      </c>
+      <c r="L17" s="2">
+        <v>111700</v>
       </c>
       <c r="M17" t="b">
         <v>1</v>
@@ -2153,14 +2015,14 @@
       <c r="D18" s="2">
         <v>4035912077</v>
       </c>
-      <c r="E18" s="2">
-        <v>9178721</v>
-      </c>
-      <c r="F18" s="2">
-        <v>6047590</v>
-      </c>
-      <c r="G18" s="2">
-        <v>411157</v>
+      <c r="E18" s="3">
+        <v>45093</v>
+      </c>
+      <c r="F18" t="s">
+        <v>101</v>
+      </c>
+      <c r="G18" t="s">
+        <v>117</v>
       </c>
       <c r="H18" s="4">
         <v>0.93629999999999991</v>
@@ -2168,14 +2030,14 @@
       <c r="I18">
         <v>11.48</v>
       </c>
-      <c r="J18" t="s">
-        <v>283</v>
-      </c>
-      <c r="K18" t="s">
-        <v>101</v>
-      </c>
-      <c r="L18" t="s">
-        <v>117</v>
+      <c r="J18" s="2">
+        <v>9178721</v>
+      </c>
+      <c r="K18" s="2">
+        <v>6047590</v>
+      </c>
+      <c r="L18" s="2">
+        <v>411157</v>
       </c>
       <c r="M18" t="b">
         <v>1</v>
@@ -2186,7 +2048,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>284</v>
+        <v>268</v>
       </c>
       <c r="C19" s="2">
         <v>34811</v>
@@ -2194,14 +2056,14 @@
       <c r="D19" s="2">
         <v>9356733065</v>
       </c>
-      <c r="E19" s="2">
-        <v>4151908</v>
-      </c>
-      <c r="F19" s="2">
-        <v>2125966</v>
-      </c>
-      <c r="G19" s="2">
-        <v>449168</v>
+      <c r="E19" s="3">
+        <v>44342</v>
+      </c>
+      <c r="F19" t="s">
+        <v>101</v>
+      </c>
+      <c r="G19" t="s">
+        <v>118</v>
       </c>
       <c r="H19" s="4">
         <v>0.8256</v>
@@ -2209,14 +2071,14 @@
       <c r="I19">
         <v>13.48</v>
       </c>
-      <c r="J19" t="s">
-        <v>285</v>
-      </c>
-      <c r="K19" t="s">
-        <v>101</v>
-      </c>
-      <c r="L19" t="s">
-        <v>118</v>
+      <c r="J19" s="2">
+        <v>4151908</v>
+      </c>
+      <c r="K19" s="2">
+        <v>2125966</v>
+      </c>
+      <c r="L19" s="2">
+        <v>449168</v>
       </c>
       <c r="M19" t="b">
         <v>1</v>
@@ -2235,14 +2097,14 @@
       <c r="D20" s="2">
         <v>2512164284</v>
       </c>
-      <c r="E20" s="2">
-        <v>3202857</v>
-      </c>
-      <c r="F20" s="2">
-        <v>1221808</v>
-      </c>
-      <c r="G20" s="2">
-        <v>115012</v>
+      <c r="E20" s="3">
+        <v>44379</v>
+      </c>
+      <c r="F20" t="s">
+        <v>164</v>
+      </c>
+      <c r="G20" t="s">
+        <v>122</v>
       </c>
       <c r="H20" s="4">
         <v>0.91400000000000003</v>
@@ -2250,14 +2112,14 @@
       <c r="I20">
         <v>12.52</v>
       </c>
-      <c r="J20" t="s">
-        <v>286</v>
-      </c>
-      <c r="K20" t="s">
-        <v>164</v>
-      </c>
-      <c r="L20" t="s">
-        <v>122</v>
+      <c r="J20" s="2">
+        <v>3202857</v>
+      </c>
+      <c r="K20" s="2">
+        <v>1221808</v>
+      </c>
+      <c r="L20" s="2">
+        <v>115012</v>
       </c>
       <c r="M20" t="b">
         <v>1</v>
@@ -2268,7 +2130,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>287</v>
+        <v>269</v>
       </c>
       <c r="C21" s="2">
         <v>29876</v>
@@ -2276,14 +2138,14 @@
       <c r="D21" s="2">
         <v>788227346</v>
       </c>
-      <c r="E21" s="2">
-        <v>941534</v>
-      </c>
-      <c r="F21" s="2">
-        <v>328623</v>
-      </c>
-      <c r="G21" s="2">
-        <v>25007</v>
+      <c r="E21" s="3">
+        <v>45111</v>
+      </c>
+      <c r="F21" t="s">
+        <v>98</v>
+      </c>
+      <c r="G21" t="s">
+        <v>123</v>
       </c>
       <c r="H21" s="4">
         <v>0.92930000000000001</v>
@@ -2291,14 +2153,14 @@
       <c r="I21">
         <v>17.850000000000001</v>
       </c>
-      <c r="J21" t="s">
-        <v>288</v>
-      </c>
-      <c r="K21" t="s">
-        <v>98</v>
-      </c>
-      <c r="L21" t="s">
-        <v>123</v>
+      <c r="J21" s="2">
+        <v>941534</v>
+      </c>
+      <c r="K21" s="2">
+        <v>328623</v>
+      </c>
+      <c r="L21" s="2">
+        <v>25007</v>
       </c>
       <c r="M21" t="b">
         <v>0</v>
@@ -2309,7 +2171,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="C22" s="2">
         <v>27742</v>
@@ -2317,14 +2179,14 @@
       <c r="D22" s="2">
         <v>71673374</v>
       </c>
-      <c r="E22" s="2">
-        <v>2230806</v>
-      </c>
-      <c r="F22" s="2">
-        <v>31073</v>
-      </c>
-      <c r="G22" s="2">
-        <v>10025</v>
+      <c r="E22" s="3">
+        <v>44836</v>
+      </c>
+      <c r="F22" t="s">
+        <v>101</v>
+      </c>
+      <c r="G22" t="s">
+        <v>258</v>
       </c>
       <c r="H22" s="4">
         <v>0.75609999999999999</v>
@@ -2332,14 +2194,14 @@
       <c r="I22">
         <v>12.89</v>
       </c>
-      <c r="J22" t="s">
-        <v>290</v>
-      </c>
-      <c r="K22" t="s">
-        <v>101</v>
-      </c>
-      <c r="L22" t="s">
-        <v>258</v>
+      <c r="J22" s="2">
+        <v>2230806</v>
+      </c>
+      <c r="K22" s="2">
+        <v>31073</v>
+      </c>
+      <c r="L22" s="2">
+        <v>10025</v>
       </c>
       <c r="M22" t="b">
         <v>1</v>
@@ -2358,14 +2220,14 @@
       <c r="D23" s="2">
         <v>2213846982</v>
       </c>
-      <c r="E23" s="2">
-        <v>4699496</v>
-      </c>
-      <c r="F23" s="2">
-        <v>1589129</v>
-      </c>
-      <c r="G23" s="2">
-        <v>146759</v>
+      <c r="E23" s="3">
+        <v>43485</v>
+      </c>
+      <c r="F23" t="s">
+        <v>100</v>
+      </c>
+      <c r="G23" t="s">
+        <v>119</v>
       </c>
       <c r="H23" s="4">
         <v>0.91549999999999998</v>
@@ -2373,14 +2235,14 @@
       <c r="I23">
         <v>20.79</v>
       </c>
-      <c r="J23" t="s">
-        <v>291</v>
-      </c>
-      <c r="K23" t="s">
-        <v>100</v>
-      </c>
-      <c r="L23" t="s">
-        <v>119</v>
+      <c r="J23" s="2">
+        <v>4699496</v>
+      </c>
+      <c r="K23" s="2">
+        <v>1589129</v>
+      </c>
+      <c r="L23" s="2">
+        <v>146759</v>
       </c>
       <c r="M23" t="b">
         <v>1</v>
@@ -2399,14 +2261,14 @@
       <c r="D24" s="2">
         <v>3921265656</v>
       </c>
-      <c r="E24" s="2">
-        <v>7532166</v>
-      </c>
-      <c r="F24" s="2">
-        <v>2964109</v>
-      </c>
-      <c r="G24" s="2">
-        <v>220907</v>
+      <c r="E24" s="3">
+        <v>42675</v>
+      </c>
+      <c r="F24" t="s">
+        <v>99</v>
+      </c>
+      <c r="G24" t="s">
+        <v>124</v>
       </c>
       <c r="H24" s="4">
         <v>0.93059999999999998</v>
@@ -2414,14 +2276,14 @@
       <c r="I24">
         <v>19.87</v>
       </c>
-      <c r="J24" t="s">
-        <v>292</v>
-      </c>
-      <c r="K24" t="s">
-        <v>99</v>
-      </c>
-      <c r="L24" t="s">
-        <v>124</v>
+      <c r="J24" s="2">
+        <v>7532166</v>
+      </c>
+      <c r="K24" s="2">
+        <v>2964109</v>
+      </c>
+      <c r="L24" s="2">
+        <v>220907</v>
       </c>
       <c r="M24" t="b">
         <v>1</v>
@@ -2432,7 +2294,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>293</v>
+        <v>271</v>
       </c>
       <c r="C25" s="2">
         <v>25552</v>
@@ -2440,14 +2302,14 @@
       <c r="D25" s="2">
         <v>2150952561</v>
       </c>
-      <c r="E25" s="2">
-        <v>2038782</v>
-      </c>
-      <c r="F25" s="2">
-        <v>1330598</v>
-      </c>
-      <c r="G25" s="2">
-        <v>226904</v>
+      <c r="E25" s="3">
+        <v>44242</v>
+      </c>
+      <c r="F25" t="s">
+        <v>101</v>
+      </c>
+      <c r="G25" t="s">
+        <v>131</v>
       </c>
       <c r="H25" s="4">
         <v>0.85430000000000006</v>
@@ -2455,14 +2317,14 @@
       <c r="I25">
         <v>9.44</v>
       </c>
-      <c r="J25" t="s">
-        <v>294</v>
-      </c>
-      <c r="K25" t="s">
-        <v>101</v>
-      </c>
-      <c r="L25" t="s">
-        <v>131</v>
+      <c r="J25" s="2">
+        <v>2038782</v>
+      </c>
+      <c r="K25" s="2">
+        <v>1330598</v>
+      </c>
+      <c r="L25" s="2">
+        <v>226904</v>
       </c>
       <c r="M25" t="b">
         <v>1</v>
@@ -2473,7 +2335,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>295</v>
+        <v>272</v>
       </c>
       <c r="C26" s="2">
         <v>25254</v>
@@ -2481,14 +2343,14 @@
       <c r="D26" s="2">
         <v>305151668</v>
       </c>
-      <c r="E26" s="2">
-        <v>200221</v>
-      </c>
-      <c r="F26" s="2">
-        <v>209221</v>
-      </c>
-      <c r="G26" s="2">
-        <v>17924</v>
+      <c r="E26" s="3">
+        <v>45008</v>
+      </c>
+      <c r="F26" t="s">
+        <v>99</v>
+      </c>
+      <c r="G26" t="s">
+        <v>273</v>
       </c>
       <c r="H26" s="4">
         <v>0.92110000000000003</v>
@@ -2496,14 +2358,14 @@
       <c r="I26">
         <v>23.53</v>
       </c>
-      <c r="J26" t="s">
-        <v>296</v>
-      </c>
-      <c r="K26" t="s">
-        <v>99</v>
-      </c>
-      <c r="L26" t="s">
-        <v>297</v>
+      <c r="J26" s="2">
+        <v>200221</v>
+      </c>
+      <c r="K26" s="2">
+        <v>209221</v>
+      </c>
+      <c r="L26" s="2">
+        <v>17924</v>
       </c>
       <c r="M26" t="b">
         <v>0</v>
@@ -2514,7 +2376,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>298</v>
+        <v>274</v>
       </c>
       <c r="C27" s="2">
         <v>23708</v>
@@ -2522,14 +2384,14 @@
       <c r="D27" s="2">
         <v>224948798</v>
       </c>
-      <c r="E27" s="2">
-        <v>3688400</v>
-      </c>
-      <c r="F27" s="2">
-        <v>859754</v>
-      </c>
-      <c r="G27" s="2">
-        <v>17840</v>
+      <c r="E27" s="3">
+        <v>45421</v>
+      </c>
+      <c r="F27" t="s">
+        <v>167</v>
+      </c>
+      <c r="G27" t="s">
+        <v>114</v>
       </c>
       <c r="H27" s="4">
         <v>0.97970000000000002</v>
@@ -2537,14 +2399,14 @@
       <c r="I27">
         <v>17.670000000000002</v>
       </c>
-      <c r="J27" t="s">
-        <v>299</v>
-      </c>
-      <c r="K27" t="s">
-        <v>167</v>
-      </c>
-      <c r="L27" t="s">
-        <v>114</v>
+      <c r="J27" s="2">
+        <v>3688400</v>
+      </c>
+      <c r="K27" s="2">
+        <v>859754</v>
+      </c>
+      <c r="L27" s="2">
+        <v>17840</v>
       </c>
       <c r="M27" t="b">
         <v>1</v>
@@ -2563,14 +2425,14 @@
       <c r="D28" s="2">
         <v>8814396111</v>
       </c>
-      <c r="E28" s="2">
-        <v>13474770</v>
-      </c>
-      <c r="F28" s="2">
-        <v>5235321</v>
-      </c>
-      <c r="G28" s="2">
-        <v>706279</v>
+      <c r="E28" s="3">
+        <v>41946</v>
+      </c>
+      <c r="F28" t="s">
+        <v>98</v>
+      </c>
+      <c r="G28" t="s">
+        <v>115</v>
       </c>
       <c r="H28" s="4">
         <v>0.88109999999999999</v>
@@ -2578,14 +2440,14 @@
       <c r="I28">
         <v>22.76</v>
       </c>
-      <c r="J28" t="s">
-        <v>300</v>
-      </c>
-      <c r="K28" t="s">
-        <v>98</v>
-      </c>
-      <c r="L28" t="s">
-        <v>115</v>
+      <c r="J28" s="2">
+        <v>13474770</v>
+      </c>
+      <c r="K28" s="2">
+        <v>5235321</v>
+      </c>
+      <c r="L28" s="2">
+        <v>706279</v>
       </c>
       <c r="M28" t="b">
         <v>0</v>
@@ -2596,7 +2458,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>301</v>
+        <v>275</v>
       </c>
       <c r="C29" s="2">
         <v>21635</v>
@@ -2604,14 +2466,14 @@
       <c r="D29" s="2">
         <v>22145433</v>
       </c>
-      <c r="E29" s="2">
-        <v>50548</v>
-      </c>
-      <c r="F29" s="2">
-        <v>32603</v>
-      </c>
-      <c r="G29" s="2">
-        <v>2677</v>
+      <c r="E29" s="3">
+        <v>44758</v>
+      </c>
+      <c r="F29" t="s">
+        <v>99</v>
+      </c>
+      <c r="G29" t="s">
+        <v>276</v>
       </c>
       <c r="H29" s="4">
         <v>0.92409999999999992</v>
@@ -2619,14 +2481,14 @@
       <c r="I29">
         <v>22.01</v>
       </c>
-      <c r="J29" t="s">
-        <v>302</v>
-      </c>
-      <c r="K29" t="s">
-        <v>99</v>
-      </c>
-      <c r="L29" t="s">
-        <v>303</v>
+      <c r="J29" s="2">
+        <v>50548</v>
+      </c>
+      <c r="K29" s="2">
+        <v>32603</v>
+      </c>
+      <c r="L29" s="2">
+        <v>2677</v>
       </c>
       <c r="M29" t="b">
         <v>1</v>
@@ -2645,14 +2507,14 @@
       <c r="D30" s="2">
         <v>2550278028</v>
       </c>
-      <c r="E30" s="2">
-        <v>2887818</v>
-      </c>
-      <c r="F30" s="2">
-        <v>2077616</v>
-      </c>
-      <c r="G30" s="2">
-        <v>159424</v>
+      <c r="E30" s="3">
+        <v>44596</v>
+      </c>
+      <c r="F30" t="s">
+        <v>165</v>
+      </c>
+      <c r="G30" t="s">
+        <v>129</v>
       </c>
       <c r="H30" s="4">
         <v>0.92870000000000008</v>
@@ -2660,14 +2522,14 @@
       <c r="I30">
         <v>9.86</v>
       </c>
-      <c r="J30" t="s">
-        <v>274</v>
-      </c>
-      <c r="K30" t="s">
-        <v>165</v>
-      </c>
-      <c r="L30" t="s">
-        <v>129</v>
+      <c r="J30" s="2">
+        <v>2887818</v>
+      </c>
+      <c r="K30" s="2">
+        <v>2077616</v>
+      </c>
+      <c r="L30" s="2">
+        <v>159424</v>
       </c>
       <c r="M30" t="b">
         <v>1</v>
@@ -2686,14 +2548,14 @@
       <c r="D31" s="2">
         <v>823275247</v>
       </c>
-      <c r="E31" s="2">
-        <v>16565979</v>
-      </c>
-      <c r="F31" s="2">
-        <v>139248</v>
-      </c>
-      <c r="G31" s="2">
-        <v>21216</v>
+      <c r="E31" s="3">
+        <v>45018</v>
+      </c>
+      <c r="F31" t="s">
+        <v>98</v>
+      </c>
+      <c r="G31" t="s">
+        <v>128</v>
       </c>
       <c r="H31" s="4">
         <v>0.86780000000000002</v>
@@ -2701,14 +2563,14 @@
       <c r="I31">
         <v>18.53</v>
       </c>
-      <c r="J31" t="s">
-        <v>304</v>
-      </c>
-      <c r="K31" t="s">
-        <v>98</v>
-      </c>
-      <c r="L31" t="s">
-        <v>128</v>
+      <c r="J31" s="2">
+        <v>16565979</v>
+      </c>
+      <c r="K31" s="2">
+        <v>139248</v>
+      </c>
+      <c r="L31" s="2">
+        <v>21216</v>
       </c>
       <c r="M31" t="b">
         <v>0</v>
@@ -2727,14 +2589,14 @@
       <c r="D32" s="2">
         <v>84734150</v>
       </c>
-      <c r="E32" s="2">
-        <v>2126376</v>
-      </c>
-      <c r="F32" s="2">
-        <v>595242</v>
-      </c>
-      <c r="G32" s="2">
-        <v>29953</v>
+      <c r="E32" s="3">
+        <v>45437</v>
+      </c>
+      <c r="F32" t="s">
+        <v>247</v>
+      </c>
+      <c r="G32" t="s">
+        <v>248</v>
       </c>
       <c r="H32" s="4">
         <v>0.95209999999999995</v>
@@ -2742,14 +2604,14 @@
       <c r="I32">
         <v>6.12</v>
       </c>
-      <c r="J32" t="s">
-        <v>305</v>
-      </c>
-      <c r="K32" t="s">
-        <v>247</v>
-      </c>
-      <c r="L32" t="s">
-        <v>248</v>
+      <c r="J32" s="2">
+        <v>2126376</v>
+      </c>
+      <c r="K32" s="2">
+        <v>595242</v>
+      </c>
+      <c r="L32" s="2">
+        <v>29953</v>
       </c>
       <c r="M32" t="b">
         <v>1</v>
@@ -2768,14 +2630,14 @@
       <c r="D33" s="2">
         <v>33396102</v>
       </c>
-      <c r="E33" s="2">
-        <v>452960</v>
-      </c>
-      <c r="F33" s="2">
-        <v>140636</v>
-      </c>
-      <c r="G33" s="2">
-        <v>6468</v>
+      <c r="E33" s="3">
+        <v>44963</v>
+      </c>
+      <c r="F33" t="s">
+        <v>100</v>
+      </c>
+      <c r="G33" t="s">
+        <v>251</v>
       </c>
       <c r="H33" s="4">
         <v>0.95599999999999996</v>
@@ -2783,14 +2645,14 @@
       <c r="I33">
         <v>15.92</v>
       </c>
-      <c r="J33" t="s">
-        <v>306</v>
-      </c>
-      <c r="K33" t="s">
-        <v>100</v>
-      </c>
-      <c r="L33" t="s">
-        <v>251</v>
+      <c r="J33" s="2">
+        <v>452960</v>
+      </c>
+      <c r="K33" s="2">
+        <v>140636</v>
+      </c>
+      <c r="L33" s="2">
+        <v>6468</v>
       </c>
       <c r="M33" t="b">
         <v>1</v>
@@ -2801,7 +2663,7 @@
         <v>31</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>307</v>
+        <v>277</v>
       </c>
       <c r="C34" s="2">
         <v>20165</v>
@@ -2809,14 +2671,14 @@
       <c r="D34" s="2">
         <v>839708636</v>
       </c>
-      <c r="E34" s="2">
-        <v>2519706</v>
-      </c>
-      <c r="F34" s="2">
-        <v>562343</v>
-      </c>
-      <c r="G34" s="2">
-        <v>66130</v>
+      <c r="E34" s="3">
+        <v>44006</v>
+      </c>
+      <c r="F34" t="s">
+        <v>185</v>
+      </c>
+      <c r="G34" t="s">
+        <v>134</v>
       </c>
       <c r="H34" s="4">
         <v>0.89480000000000004</v>
@@ -2824,14 +2686,14 @@
       <c r="I34">
         <v>24.23</v>
       </c>
-      <c r="J34" t="s">
-        <v>308</v>
-      </c>
-      <c r="K34" t="s">
-        <v>185</v>
-      </c>
-      <c r="L34" t="s">
-        <v>134</v>
+      <c r="J34" s="2">
+        <v>2519706</v>
+      </c>
+      <c r="K34" s="2">
+        <v>562343</v>
+      </c>
+      <c r="L34" s="2">
+        <v>66130</v>
       </c>
       <c r="M34" t="b">
         <v>0</v>
@@ -2842,7 +2704,7 @@
         <v>32</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>309</v>
+        <v>278</v>
       </c>
       <c r="C35" s="2">
         <v>17889</v>
@@ -2850,14 +2712,14 @@
       <c r="D35" s="2">
         <v>860915389</v>
       </c>
-      <c r="E35" s="2">
-        <v>1064670</v>
-      </c>
-      <c r="F35" s="2">
-        <v>1314089</v>
-      </c>
-      <c r="G35" s="2">
-        <v>116488</v>
+      <c r="E35" s="3">
+        <v>45337</v>
+      </c>
+      <c r="F35" t="s">
+        <v>99</v>
+      </c>
+      <c r="G35" t="s">
+        <v>125</v>
       </c>
       <c r="H35" s="4">
         <v>0.91859999999999997</v>
@@ -2865,14 +2727,14 @@
       <c r="I35">
         <v>9.9499999999999993</v>
       </c>
-      <c r="J35" t="s">
-        <v>310</v>
-      </c>
-      <c r="K35" t="s">
-        <v>99</v>
-      </c>
-      <c r="L35" t="s">
-        <v>125</v>
+      <c r="J35" s="2">
+        <v>1064670</v>
+      </c>
+      <c r="K35" s="2">
+        <v>1314089</v>
+      </c>
+      <c r="L35" s="2">
+        <v>116488</v>
       </c>
       <c r="M35" t="b">
         <v>1</v>
@@ -2891,14 +2753,14 @@
       <c r="D36" s="2">
         <v>528477503</v>
       </c>
-      <c r="E36" s="2">
-        <v>691241</v>
-      </c>
-      <c r="F36" s="2">
-        <v>595269</v>
-      </c>
-      <c r="G36" s="2">
-        <v>96787</v>
+      <c r="E36" s="3">
+        <v>45078</v>
+      </c>
+      <c r="F36" t="s">
+        <v>101</v>
+      </c>
+      <c r="G36" t="s">
+        <v>126</v>
       </c>
       <c r="H36" s="4">
         <v>0.86010000000000009</v>
@@ -2906,14 +2768,14 @@
       <c r="I36">
         <v>13.19</v>
       </c>
-      <c r="J36" t="s">
-        <v>311</v>
-      </c>
-      <c r="K36" t="s">
-        <v>101</v>
-      </c>
-      <c r="L36" t="s">
-        <v>126</v>
+      <c r="J36" s="2">
+        <v>691241</v>
+      </c>
+      <c r="K36" s="2">
+        <v>595269</v>
+      </c>
+      <c r="L36" s="2">
+        <v>96787</v>
       </c>
       <c r="M36" t="b">
         <v>1</v>
@@ -2932,14 +2794,14 @@
       <c r="D37" s="2">
         <v>2404954316</v>
       </c>
-      <c r="E37" s="2">
-        <v>2402322</v>
-      </c>
-      <c r="F37" s="2">
-        <v>555240</v>
-      </c>
-      <c r="G37" s="2">
-        <v>182393</v>
+      <c r="E37" s="3">
+        <v>44016</v>
+      </c>
+      <c r="F37" t="s">
+        <v>98</v>
+      </c>
+      <c r="G37" t="s">
+        <v>199</v>
       </c>
       <c r="H37" s="4">
         <v>0.75269999999999992</v>
@@ -2947,14 +2809,14 @@
       <c r="I37">
         <v>22.8</v>
       </c>
-      <c r="J37" t="s">
-        <v>312</v>
-      </c>
-      <c r="K37" t="s">
-        <v>98</v>
-      </c>
-      <c r="L37" t="s">
-        <v>199</v>
+      <c r="J37" s="2">
+        <v>2402322</v>
+      </c>
+      <c r="K37" s="2">
+        <v>555240</v>
+      </c>
+      <c r="L37" s="2">
+        <v>182393</v>
       </c>
       <c r="M37" t="b">
         <v>0</v>
@@ -2973,14 +2835,14 @@
       <c r="D38" s="2">
         <v>6966078799</v>
       </c>
-      <c r="E38" s="2">
-        <v>18202097</v>
-      </c>
-      <c r="F38" s="2">
-        <v>5471078</v>
-      </c>
-      <c r="G38" s="2">
-        <v>759312</v>
+      <c r="E38" s="3">
+        <v>42740</v>
+      </c>
+      <c r="F38" t="s">
+        <v>98</v>
+      </c>
+      <c r="G38" t="s">
+        <v>137</v>
       </c>
       <c r="H38" s="4">
         <v>0.87809999999999999</v>
@@ -2988,14 +2850,14 @@
       <c r="I38">
         <v>14.48</v>
       </c>
-      <c r="J38" t="s">
-        <v>313</v>
-      </c>
-      <c r="K38" t="s">
-        <v>98</v>
-      </c>
-      <c r="L38" t="s">
-        <v>137</v>
+      <c r="J38" s="2">
+        <v>18202097</v>
+      </c>
+      <c r="K38" s="2">
+        <v>5471078</v>
+      </c>
+      <c r="L38" s="2">
+        <v>759312</v>
       </c>
       <c r="M38" t="b">
         <v>1</v>
@@ -3014,14 +2876,14 @@
       <c r="D39" s="2">
         <v>4561781536</v>
       </c>
-      <c r="E39" s="2">
-        <v>21108197</v>
-      </c>
-      <c r="F39" s="2">
-        <v>1229762</v>
-      </c>
-      <c r="G39" s="2">
-        <v>133069</v>
+      <c r="E39" s="3">
+        <v>44313</v>
+      </c>
+      <c r="F39" t="s">
+        <v>98</v>
+      </c>
+      <c r="G39" t="s">
+        <v>132</v>
       </c>
       <c r="H39" s="4">
         <v>0.90239999999999998</v>
@@ -3029,14 +2891,14 @@
       <c r="I39">
         <v>16.649999999999999</v>
       </c>
-      <c r="J39" t="s">
-        <v>314</v>
-      </c>
-      <c r="K39" t="s">
-        <v>98</v>
-      </c>
-      <c r="L39" t="s">
-        <v>132</v>
+      <c r="J39" s="2">
+        <v>21108197</v>
+      </c>
+      <c r="K39" s="2">
+        <v>1229762</v>
+      </c>
+      <c r="L39" s="2">
+        <v>133069</v>
       </c>
       <c r="M39" t="b">
         <v>0</v>
@@ -3055,14 +2917,14 @@
       <c r="D40" s="2">
         <v>2545868303</v>
       </c>
-      <c r="E40" s="2">
-        <v>1132321</v>
-      </c>
-      <c r="F40" s="2">
-        <v>260860</v>
-      </c>
-      <c r="G40" s="2">
-        <v>187303</v>
+      <c r="E40" s="3">
+        <v>44593</v>
+      </c>
+      <c r="F40" t="s">
+        <v>99</v>
+      </c>
+      <c r="G40" t="s">
+        <v>133</v>
       </c>
       <c r="H40" s="4">
         <v>0.58210000000000006</v>
@@ -3070,14 +2932,14 @@
       <c r="I40">
         <v>9.69</v>
       </c>
-      <c r="J40" t="s">
-        <v>315</v>
-      </c>
-      <c r="K40" t="s">
-        <v>99</v>
-      </c>
-      <c r="L40" t="s">
-        <v>133</v>
+      <c r="J40" s="2">
+        <v>1132321</v>
+      </c>
+      <c r="K40" s="2">
+        <v>260860</v>
+      </c>
+      <c r="L40" s="2">
+        <v>187303</v>
       </c>
       <c r="M40" t="b">
         <v>1</v>
@@ -3096,14 +2958,14 @@
       <c r="D41" s="2">
         <v>5092782393</v>
       </c>
-      <c r="E41" s="2">
-        <v>6266920</v>
-      </c>
-      <c r="F41" s="2">
-        <v>3523840</v>
-      </c>
-      <c r="G41" s="2">
-        <v>249308</v>
+      <c r="E41" s="3">
+        <v>44268</v>
+      </c>
+      <c r="F41" t="s">
+        <v>99</v>
+      </c>
+      <c r="G41" t="s">
+        <v>195</v>
       </c>
       <c r="H41" s="4">
         <v>0.93389999999999995</v>
@@ -3111,14 +2973,14 @@
       <c r="I41">
         <v>8.64</v>
       </c>
-      <c r="J41" t="s">
-        <v>316</v>
-      </c>
-      <c r="K41" t="s">
-        <v>99</v>
-      </c>
-      <c r="L41" t="s">
-        <v>195</v>
+      <c r="J41" s="2">
+        <v>6266920</v>
+      </c>
+      <c r="K41" s="2">
+        <v>3523840</v>
+      </c>
+      <c r="L41" s="2">
+        <v>249308</v>
       </c>
       <c r="M41" t="b">
         <v>1</v>
@@ -3137,14 +2999,14 @@
       <c r="D42" s="2">
         <v>12884245204</v>
       </c>
-      <c r="E42" s="2">
-        <v>11588284</v>
-      </c>
-      <c r="F42" s="2">
-        <v>3545107</v>
-      </c>
-      <c r="G42" s="2">
-        <v>397863</v>
+      <c r="E42" s="3">
+        <v>43852</v>
+      </c>
+      <c r="F42" t="s">
+        <v>100</v>
+      </c>
+      <c r="G42" t="s">
+        <v>144</v>
       </c>
       <c r="H42" s="4">
         <v>0.89910000000000001</v>
@@ -3152,14 +3014,14 @@
       <c r="I42">
         <v>11.1</v>
       </c>
-      <c r="J42" t="s">
-        <v>317</v>
-      </c>
-      <c r="K42" t="s">
-        <v>100</v>
-      </c>
-      <c r="L42" t="s">
-        <v>144</v>
+      <c r="J42" s="2">
+        <v>11588284</v>
+      </c>
+      <c r="K42" s="2">
+        <v>3545107</v>
+      </c>
+      <c r="L42" s="2">
+        <v>397863</v>
       </c>
       <c r="M42" t="b">
         <v>1</v>
@@ -3178,14 +3040,14 @@
       <c r="D43" s="2">
         <v>12884286490</v>
       </c>
-      <c r="E43" s="2">
-        <v>11588287</v>
-      </c>
-      <c r="F43" s="2">
-        <v>3545107</v>
-      </c>
-      <c r="G43" s="2">
-        <v>397863</v>
+      <c r="E43" s="3">
+        <v>43852</v>
+      </c>
+      <c r="F43" t="s">
+        <v>100</v>
+      </c>
+      <c r="G43" t="s">
+        <v>144</v>
       </c>
       <c r="H43" s="4">
         <v>0.89910000000000001</v>
@@ -3193,14 +3055,14 @@
       <c r="I43">
         <v>11.1</v>
       </c>
-      <c r="J43" t="s">
-        <v>317</v>
-      </c>
-      <c r="K43" t="s">
-        <v>100</v>
-      </c>
-      <c r="L43" t="s">
-        <v>144</v>
+      <c r="J43" s="2">
+        <v>11588287</v>
+      </c>
+      <c r="K43" s="2">
+        <v>3545107</v>
+      </c>
+      <c r="L43" s="2">
+        <v>397863</v>
       </c>
       <c r="M43" t="b">
         <v>1</v>
@@ -3219,14 +3081,14 @@
       <c r="D44" s="2">
         <v>3049225856</v>
       </c>
-      <c r="E44" s="2">
-        <v>2247852</v>
-      </c>
-      <c r="F44" s="2">
-        <v>1294088</v>
-      </c>
-      <c r="G44" s="2">
-        <v>131497</v>
+      <c r="E44" s="3">
+        <v>43815</v>
+      </c>
+      <c r="F44" t="s">
+        <v>99</v>
+      </c>
+      <c r="G44" t="s">
+        <v>146</v>
       </c>
       <c r="H44" s="4">
         <v>0.90780000000000005</v>
@@ -3234,14 +3096,14 @@
       <c r="I44">
         <v>17.3</v>
       </c>
-      <c r="J44" t="s">
-        <v>318</v>
-      </c>
-      <c r="K44" t="s">
-        <v>99</v>
-      </c>
-      <c r="L44" t="s">
-        <v>146</v>
+      <c r="J44" s="2">
+        <v>2247852</v>
+      </c>
+      <c r="K44" s="2">
+        <v>1294088</v>
+      </c>
+      <c r="L44" s="2">
+        <v>131497</v>
       </c>
       <c r="M44" t="b">
         <v>0</v>
@@ -3260,14 +3122,14 @@
       <c r="D45" s="2">
         <v>856012261</v>
       </c>
-      <c r="E45" s="2">
-        <v>577971</v>
-      </c>
-      <c r="F45" s="2">
-        <v>246326</v>
-      </c>
-      <c r="G45" s="2">
-        <v>45293</v>
+      <c r="E45" s="3">
+        <v>44958</v>
+      </c>
+      <c r="F45" t="s">
+        <v>101</v>
+      </c>
+      <c r="G45" t="s">
+        <v>140</v>
       </c>
       <c r="H45" s="4">
         <v>0.84470000000000001</v>
@@ -3275,14 +3137,14 @@
       <c r="I45">
         <v>11.37</v>
       </c>
-      <c r="J45" t="s">
-        <v>319</v>
-      </c>
-      <c r="K45" t="s">
-        <v>101</v>
-      </c>
-      <c r="L45" t="s">
-        <v>140</v>
+      <c r="J45" s="2">
+        <v>577971</v>
+      </c>
+      <c r="K45" s="2">
+        <v>246326</v>
+      </c>
+      <c r="L45" s="2">
+        <v>45293</v>
       </c>
       <c r="M45" t="b">
         <v>1</v>
@@ -3293,7 +3155,7 @@
         <v>43</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>320</v>
+        <v>279</v>
       </c>
       <c r="C46" s="2">
         <v>14500</v>
@@ -3301,14 +3163,14 @@
       <c r="D46" s="2">
         <v>993329561</v>
       </c>
-      <c r="E46" s="2">
-        <v>1550709</v>
-      </c>
-      <c r="F46" s="2">
-        <v>477958</v>
-      </c>
-      <c r="G46" s="2">
-        <v>141034</v>
+      <c r="E46" s="3">
+        <v>44363</v>
+      </c>
+      <c r="F46" t="s">
+        <v>280</v>
+      </c>
+      <c r="G46" t="s">
+        <v>281</v>
       </c>
       <c r="H46" s="4">
         <v>0.7722</v>
@@ -3316,14 +3178,14 @@
       <c r="I46">
         <v>12.92</v>
       </c>
-      <c r="J46" t="s">
-        <v>321</v>
-      </c>
-      <c r="K46" t="s">
-        <v>322</v>
-      </c>
-      <c r="L46" t="s">
-        <v>323</v>
+      <c r="J46" s="2">
+        <v>1550709</v>
+      </c>
+      <c r="K46" s="2">
+        <v>477958</v>
+      </c>
+      <c r="L46" s="2">
+        <v>141034</v>
       </c>
       <c r="M46" t="b">
         <v>1</v>
@@ -3342,14 +3204,14 @@
       <c r="D47" s="2">
         <v>23495706846</v>
       </c>
-      <c r="E47" s="2">
-        <v>11114427</v>
-      </c>
-      <c r="F47" s="2">
-        <v>3812449</v>
-      </c>
-      <c r="G47" s="2">
-        <v>1325135</v>
+      <c r="E47" s="3">
+        <v>43268</v>
+      </c>
+      <c r="F47" t="s">
+        <v>99</v>
+      </c>
+      <c r="G47" t="s">
+        <v>143</v>
       </c>
       <c r="H47" s="4">
         <v>0.74209999999999998</v>
@@ -3357,14 +3219,14 @@
       <c r="I47">
         <v>4.21</v>
       </c>
-      <c r="J47" t="s">
-        <v>324</v>
-      </c>
-      <c r="K47" t="s">
-        <v>99</v>
-      </c>
-      <c r="L47" t="s">
-        <v>143</v>
+      <c r="J47" s="2">
+        <v>11114427</v>
+      </c>
+      <c r="K47" s="2">
+        <v>3812449</v>
+      </c>
+      <c r="L47" s="2">
+        <v>1325135</v>
       </c>
       <c r="M47" t="b">
         <v>1</v>
@@ -3375,7 +3237,7 @@
         <v>45</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>325</v>
+        <v>282</v>
       </c>
       <c r="C48" s="2">
         <v>13927</v>
@@ -3383,14 +3245,14 @@
       <c r="D48" s="2">
         <v>1402084023</v>
       </c>
-      <c r="E48" s="2">
-        <v>10146953</v>
-      </c>
-      <c r="F48" s="2">
-        <v>1363900</v>
-      </c>
-      <c r="G48" s="2">
-        <v>101614</v>
+      <c r="E48" s="3">
+        <v>43638</v>
+      </c>
+      <c r="F48" t="s">
+        <v>99</v>
+      </c>
+      <c r="G48" t="s">
+        <v>148</v>
       </c>
       <c r="H48" s="4">
         <v>0.93069999999999997</v>
@@ -3398,14 +3260,14 @@
       <c r="I48">
         <v>13.74</v>
       </c>
-      <c r="J48" t="s">
-        <v>326</v>
-      </c>
-      <c r="K48" t="s">
-        <v>99</v>
-      </c>
-      <c r="L48" t="s">
-        <v>148</v>
+      <c r="J48" s="2">
+        <v>10146953</v>
+      </c>
+      <c r="K48" s="2">
+        <v>1363900</v>
+      </c>
+      <c r="L48" s="2">
+        <v>101614</v>
       </c>
       <c r="M48" t="b">
         <v>1</v>
@@ -3416,7 +3278,7 @@
         <v>46</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>327</v>
+        <v>283</v>
       </c>
       <c r="C49" s="2">
         <v>13498</v>
@@ -3424,14 +3286,14 @@
       <c r="D49" s="2">
         <v>91516003</v>
       </c>
-      <c r="E49" s="2">
-        <v>120757</v>
-      </c>
-      <c r="F49" s="2">
-        <v>82659</v>
-      </c>
-      <c r="G49" s="2">
-        <v>8364</v>
+      <c r="E49" s="3">
+        <v>45292</v>
+      </c>
+      <c r="F49" t="s">
+        <v>168</v>
+      </c>
+      <c r="G49" t="s">
+        <v>139</v>
       </c>
       <c r="H49" s="4">
         <v>0.90810000000000002</v>
@@ -3439,14 +3301,14 @@
       <c r="I49">
         <v>9.7899999999999991</v>
       </c>
-      <c r="J49" t="s">
-        <v>328</v>
-      </c>
-      <c r="K49" t="s">
-        <v>168</v>
-      </c>
-      <c r="L49" t="s">
-        <v>139</v>
+      <c r="J49" s="2">
+        <v>120757</v>
+      </c>
+      <c r="K49" s="2">
+        <v>82659</v>
+      </c>
+      <c r="L49" s="2">
+        <v>8364</v>
       </c>
       <c r="M49" t="b">
         <v>0</v>
@@ -3465,14 +3327,14 @@
       <c r="D50" s="2">
         <v>949400870</v>
       </c>
-      <c r="E50" s="2">
-        <v>857811</v>
-      </c>
-      <c r="F50" s="2">
-        <v>1117424</v>
-      </c>
-      <c r="G50" s="2">
-        <v>54586</v>
+      <c r="E50" s="3">
+        <v>45029</v>
+      </c>
+      <c r="F50" t="s">
+        <v>167</v>
+      </c>
+      <c r="G50" t="s">
+        <v>141</v>
       </c>
       <c r="H50" s="4">
         <v>0.95340000000000003</v>
@@ -3480,14 +3342,14 @@
       <c r="I50">
         <v>18.600000000000001</v>
       </c>
-      <c r="J50" t="s">
-        <v>329</v>
-      </c>
-      <c r="K50" t="s">
-        <v>167</v>
-      </c>
-      <c r="L50" t="s">
-        <v>141</v>
+      <c r="J50" s="2">
+        <v>857811</v>
+      </c>
+      <c r="K50" s="2">
+        <v>1117424</v>
+      </c>
+      <c r="L50" s="2">
+        <v>54586</v>
       </c>
       <c r="M50" t="b">
         <v>1</v>
@@ -3498,7 +3360,7 @@
         <v>48</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>330</v>
+        <v>284</v>
       </c>
       <c r="C51" s="2">
         <v>13138</v>
@@ -3506,14 +3368,14 @@
       <c r="D51" s="2">
         <v>41234013</v>
       </c>
-      <c r="E51" s="2">
-        <v>108841</v>
-      </c>
-      <c r="F51" s="2">
-        <v>45902</v>
-      </c>
-      <c r="G51" s="2">
-        <v>3708</v>
+      <c r="E51" s="3">
+        <v>45316</v>
+      </c>
+      <c r="F51" t="s">
+        <v>100</v>
+      </c>
+      <c r="G51" t="s">
+        <v>285</v>
       </c>
       <c r="H51" s="4">
         <v>0.92530000000000001</v>
@@ -3521,14 +3383,14 @@
       <c r="I51">
         <v>13.11</v>
       </c>
-      <c r="J51" t="s">
-        <v>331</v>
-      </c>
-      <c r="K51" t="s">
-        <v>100</v>
-      </c>
-      <c r="L51" t="s">
-        <v>332</v>
+      <c r="J51" s="2">
+        <v>108841</v>
+      </c>
+      <c r="K51" s="2">
+        <v>45902</v>
+      </c>
+      <c r="L51" s="2">
+        <v>3708</v>
       </c>
       <c r="M51" t="b">
         <v>0</v>
@@ -3547,14 +3409,14 @@
       <c r="D52" s="2">
         <v>3534971607</v>
       </c>
-      <c r="E52" s="2">
-        <v>3117442</v>
-      </c>
-      <c r="F52" s="2">
-        <v>1272561</v>
-      </c>
-      <c r="G52" s="2">
-        <v>272528</v>
+      <c r="E52" s="3">
+        <v>44513</v>
+      </c>
+      <c r="F52" t="s">
+        <v>100</v>
+      </c>
+      <c r="G52" t="s">
+        <v>145</v>
       </c>
       <c r="H52" s="4">
         <v>0.8236</v>
@@ -3562,14 +3424,14 @@
       <c r="I52">
         <v>8.19</v>
       </c>
-      <c r="J52" t="s">
-        <v>333</v>
-      </c>
-      <c r="K52" t="s">
-        <v>100</v>
-      </c>
-      <c r="L52" t="s">
-        <v>145</v>
+      <c r="J52" s="2">
+        <v>3117442</v>
+      </c>
+      <c r="K52" s="2">
+        <v>1272561</v>
+      </c>
+      <c r="L52" s="2">
+        <v>272528</v>
       </c>
       <c r="M52" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
fix historical new entries roblox
</commit_message>
<xml_diff>
--- a/data/total_roblox_experiences.xlsx
+++ b/data/total_roblox_experiences.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenwang/Desktop/Makers/Steam_Roblox_Streamlit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30ABD34F-212A-2040-9152-1B287FF244A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E586EB4E-6F2D-4740-AB5F-E244760C6B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5840" yWindow="1100" windowWidth="23460" windowHeight="18020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5840" yWindow="1100" windowWidth="23460" windowHeight="18020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2024-08-05" sheetId="6" r:id="rId1"/>
@@ -1614,7 +1614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B5663F-5CC2-A347-8216-F8FF4AE5954D}">
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -8358,8 +8358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D4922F-A22D-1547-8F5C-336FD651258D}">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8799,7 +8799,7 @@
         <v>214</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>360</v>
+        <v>330</v>
       </c>
       <c r="D11" s="2">
         <v>108747</v>
@@ -10608,10 +10608,10 @@
   <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C55" sqref="C55"/>
+      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
august 12 2024 data push
</commit_message>
<xml_diff>
--- a/data/total_roblox_experiences.xlsx
+++ b/data/total_roblox_experiences.xlsx
@@ -8,24 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenwang/Desktop/Makers/Steam_Roblox_Streamlit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E586EB4E-6F2D-4740-AB5F-E244760C6B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2681867F-FD93-484D-977F-0E3CE0EA4C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5840" yWindow="1100" windowWidth="23460" windowHeight="18020" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5840" yWindow="1100" windowWidth="23460" windowHeight="18020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2024-08-05" sheetId="6" r:id="rId1"/>
-    <sheet name="2024-07-29" sheetId="5" r:id="rId2"/>
-    <sheet name="2024-07-22" sheetId="4" r:id="rId3"/>
-    <sheet name="2024-07-09" sheetId="3" r:id="rId4"/>
-    <sheet name="2024-07-01" sheetId="1" r:id="rId5"/>
-    <sheet name="2024-06-20" sheetId="2" r:id="rId6"/>
+    <sheet name="2024-08-12" sheetId="7" r:id="rId1"/>
+    <sheet name="2024-08-05" sheetId="6" r:id="rId2"/>
+    <sheet name="2024-07-29" sheetId="5" r:id="rId3"/>
+    <sheet name="2024-07-22" sheetId="4" r:id="rId4"/>
+    <sheet name="2024-07-09" sheetId="3" r:id="rId5"/>
+    <sheet name="2024-07-01" sheetId="1" r:id="rId6"/>
+    <sheet name="2024-06-20" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1555" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1820" uniqueCount="417">
   <si>
     <t>#1</t>
   </si>
@@ -1189,6 +1190,93 @@
   </si>
   <si>
     <t>/experience/192800/</t>
+  </si>
+  <si>
+    <t>Top Experiences 50 on Roblox (Data fetched from RoMonitor as of 10:04 AM EDT, 2024-08-12)</t>
+  </si>
+  <si>
+    <t>Pet Simulator 99! 🎲 RNG</t>
+  </si>
+  <si>
+    <t>[BOSS] The Strongest Battlegrounds</t>
+  </si>
+  <si>
+    <t>Dress To Impress 🌊</t>
+  </si>
+  <si>
+    <t>[TRADE] Blade Ball</t>
+  </si>
+  <si>
+    <t>[🔥ABYSMAL MODE] Toilet Tower Defense</t>
+  </si>
+  <si>
+    <t>BedWars [🔥3x XP]</t>
+  </si>
+  <si>
+    <t>RIVALS</t>
+  </si>
+  <si>
+    <t>LifeTogether 🏠 RP (UPDATE 23)</t>
+  </si>
+  <si>
+    <t>[📈 x4] Anime Last Stand</t>
+  </si>
+  <si>
+    <t>a dusty trip [🍦BOSS]</t>
+  </si>
+  <si>
+    <t>Realm Rampage</t>
+  </si>
+  <si>
+    <t>S0LID Foundation</t>
+  </si>
+  <si>
+    <t>[EXPLOSION HERO] Heroes Battlegrounds</t>
+  </si>
+  <si>
+    <t>Five Nights TD [MARKETPLACE]</t>
+  </si>
+  <si>
+    <t>[Friendly Fire] - Pressure</t>
+  </si>
+  <si>
+    <t>🌊 Creatures of Sonaria 🗻 Survive Kaiju Animals</t>
+  </si>
+  <si>
+    <t>[UPDATE🏐] Slap Battles👏</t>
+  </si>
+  <si>
+    <t>[UPD 6] Gym League</t>
+  </si>
+  <si>
+    <t>Livetopia🍣 Sushi Bar</t>
+  </si>
+  <si>
+    <t>[💪GEAR 5🗡️] A Universal Time 3.7 🏊‍♀️</t>
+  </si>
+  <si>
+    <t>Universe Time Studio</t>
+  </si>
+  <si>
+    <t>SOLSTICE ☀️ Dragon Adventures 🐉 Fantasy Pets ✨</t>
+  </si>
+  <si>
+    <t>🥊untitled boxing game🥊</t>
+  </si>
+  <si>
+    <t>[🚽 EVENT🚽] Skibidi Tower Defense</t>
+  </si>
+  <si>
+    <t>BARRY'S PRISON RUN! (BEETLEJUICE!)</t>
+  </si>
+  <si>
+    <t>@Horomori</t>
+  </si>
+  <si>
+    <t>/experience/17129858194/</t>
+  </si>
+  <si>
+    <t>/experience/5130598377/</t>
   </si>
 </sst>
 </file>
@@ -1284,7 +1372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1302,10 +1390,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1611,6 +1700,2288 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09C3FBEA-4DAA-4D4C-B801-8F0A46D4D9A9}">
+  <dimension ref="A1:N52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="24.1640625" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>388</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="D3" s="8">
+        <v>586690</v>
+      </c>
+      <c r="E3" s="8">
+        <v>37927733171</v>
+      </c>
+      <c r="F3" s="13">
+        <v>43480</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="I3" s="11">
+        <v>0.92879999999999996</v>
+      </c>
+      <c r="J3" s="10"/>
+      <c r="K3" s="8">
+        <v>12925701</v>
+      </c>
+      <c r="L3" s="8">
+        <v>7945421</v>
+      </c>
+      <c r="M3" s="8">
+        <v>609384</v>
+      </c>
+      <c r="N3" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="D4" s="8">
+        <v>558412</v>
+      </c>
+      <c r="E4" s="8">
+        <v>52380452969</v>
+      </c>
+      <c r="F4" s="13">
+        <v>43941</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="I4" s="11">
+        <v>0.8659</v>
+      </c>
+      <c r="J4" s="10">
+        <v>16.329999999999998</v>
+      </c>
+      <c r="K4" s="8">
+        <v>21559897</v>
+      </c>
+      <c r="L4" s="8">
+        <v>5828997</v>
+      </c>
+      <c r="M4" s="8">
+        <v>902961</v>
+      </c>
+      <c r="N4" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>389</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="D5" s="8">
+        <v>249852</v>
+      </c>
+      <c r="E5" s="8">
+        <v>1329177854</v>
+      </c>
+      <c r="F5" s="13">
+        <v>44596</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="I5" s="11">
+        <v>0.96319999999999995</v>
+      </c>
+      <c r="J5" s="10">
+        <v>58.88</v>
+      </c>
+      <c r="K5" s="8">
+        <v>1372713</v>
+      </c>
+      <c r="L5" s="8">
+        <v>2426397</v>
+      </c>
+      <c r="M5" s="8">
+        <v>92761</v>
+      </c>
+      <c r="N5" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="D6" s="8">
+        <v>230123</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1703938103</v>
+      </c>
+      <c r="F6" s="13">
+        <v>45386</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I6" s="11">
+        <v>0.97509999999999997</v>
+      </c>
+      <c r="J6" s="10">
+        <v>11.81</v>
+      </c>
+      <c r="K6" s="8">
+        <v>582633</v>
+      </c>
+      <c r="L6" s="8">
+        <v>1708684</v>
+      </c>
+      <c r="M6" s="8">
+        <v>43590</v>
+      </c>
+      <c r="N6" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="D7" s="8">
+        <v>204229</v>
+      </c>
+      <c r="E7" s="8">
+        <v>7019044382</v>
+      </c>
+      <c r="F7" s="13">
+        <v>44774</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="I7" s="11">
+        <v>0.84009999999999996</v>
+      </c>
+      <c r="J7" s="10">
+        <v>9.65</v>
+      </c>
+      <c r="K7" s="8">
+        <v>3587755</v>
+      </c>
+      <c r="L7" s="8">
+        <v>2469883</v>
+      </c>
+      <c r="M7" s="8">
+        <v>470018</v>
+      </c>
+      <c r="N7" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="D8" s="8">
+        <v>187323</v>
+      </c>
+      <c r="E8" s="8">
+        <v>16667421833</v>
+      </c>
+      <c r="F8" s="13">
+        <v>41656</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="I8" s="11">
+        <v>0.91159999999999997</v>
+      </c>
+      <c r="J8" s="10">
+        <v>12.03</v>
+      </c>
+      <c r="K8" s="8">
+        <v>18727772</v>
+      </c>
+      <c r="L8" s="8">
+        <v>7583873</v>
+      </c>
+      <c r="M8" s="8">
+        <v>735113</v>
+      </c>
+      <c r="N8" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>391</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="D9" s="8">
+        <v>146732</v>
+      </c>
+      <c r="E9" s="8">
+        <v>1888094264</v>
+      </c>
+      <c r="F9" s="13">
+        <v>45216</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="I9" s="11">
+        <v>0.91469999999999996</v>
+      </c>
+      <c r="J9" s="10">
+        <v>14.05</v>
+      </c>
+      <c r="K9" s="8">
+        <v>1833316</v>
+      </c>
+      <c r="L9" s="8">
+        <v>1073978</v>
+      </c>
+      <c r="M9" s="8">
+        <v>100194</v>
+      </c>
+      <c r="N9" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="D10" s="8">
+        <v>117324</v>
+      </c>
+      <c r="E10" s="8">
+        <v>37071366996</v>
+      </c>
+      <c r="F10" s="13">
+        <v>42929</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="I10" s="11">
+        <v>0.83509999999999995</v>
+      </c>
+      <c r="J10" s="10">
+        <v>16.86</v>
+      </c>
+      <c r="K10" s="8">
+        <v>26875810</v>
+      </c>
+      <c r="L10" s="8">
+        <v>7210492</v>
+      </c>
+      <c r="M10" s="8">
+        <v>1424071</v>
+      </c>
+      <c r="N10" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="D11" s="8">
+        <v>106609</v>
+      </c>
+      <c r="E11" s="8">
+        <v>78903209</v>
+      </c>
+      <c r="F11" s="13">
+        <v>44758</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="I11" s="11">
+        <v>0.93720000000000003</v>
+      </c>
+      <c r="J11" s="10">
+        <v>17.989999999999998</v>
+      </c>
+      <c r="K11" s="8">
+        <v>95143</v>
+      </c>
+      <c r="L11" s="8">
+        <v>85867</v>
+      </c>
+      <c r="M11" s="8">
+        <v>5753</v>
+      </c>
+      <c r="N11" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="D12" s="8">
+        <v>92805</v>
+      </c>
+      <c r="E12" s="8">
+        <v>2839655894</v>
+      </c>
+      <c r="F12" s="13">
+        <v>43179</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="I12" s="11">
+        <v>0.94930000000000003</v>
+      </c>
+      <c r="J12" s="10">
+        <v>41.17</v>
+      </c>
+      <c r="K12" s="8">
+        <v>5906523</v>
+      </c>
+      <c r="L12" s="8">
+        <v>2258553</v>
+      </c>
+      <c r="M12" s="8">
+        <v>120505</v>
+      </c>
+      <c r="N12" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="D13" s="8">
+        <v>86050</v>
+      </c>
+      <c r="E13" s="8">
+        <v>646075687</v>
+      </c>
+      <c r="F13" s="13">
+        <v>45262</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="I13" s="11">
+        <v>0.87809999999999999</v>
+      </c>
+      <c r="J13" s="10">
+        <v>41.6</v>
+      </c>
+      <c r="K13" s="8">
+        <v>579220</v>
+      </c>
+      <c r="L13" s="8">
+        <v>650614</v>
+      </c>
+      <c r="M13" s="8">
+        <v>90343</v>
+      </c>
+      <c r="N13" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="D14" s="8">
+        <v>65168</v>
+      </c>
+      <c r="E14" s="8">
+        <v>4662378002</v>
+      </c>
+      <c r="F14" s="13">
+        <v>44721</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="I14" s="11">
+        <v>0.94469999999999998</v>
+      </c>
+      <c r="J14" s="10">
+        <v>9.76</v>
+      </c>
+      <c r="K14" s="8">
+        <v>5024235</v>
+      </c>
+      <c r="L14" s="8">
+        <v>1952039</v>
+      </c>
+      <c r="M14" s="8">
+        <v>114171</v>
+      </c>
+      <c r="N14" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="D15" s="8">
+        <v>61197</v>
+      </c>
+      <c r="E15" s="8">
+        <v>4124584870</v>
+      </c>
+      <c r="F15" s="13">
+        <v>45093</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I15" s="11">
+        <v>0.93610000000000004</v>
+      </c>
+      <c r="J15" s="10">
+        <v>11.39</v>
+      </c>
+      <c r="K15" s="8">
+        <v>9366087</v>
+      </c>
+      <c r="L15" s="8">
+        <v>6142180</v>
+      </c>
+      <c r="M15" s="8">
+        <v>419250</v>
+      </c>
+      <c r="N15" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="D16" s="8">
+        <v>58743</v>
+      </c>
+      <c r="E16" s="8">
+        <v>3912967157</v>
+      </c>
+      <c r="F16" s="13">
+        <v>44567</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="I16" s="11">
+        <v>0.87109999999999999</v>
+      </c>
+      <c r="J16" s="10">
+        <v>14.36</v>
+      </c>
+      <c r="K16" s="8">
+        <v>2127682</v>
+      </c>
+      <c r="L16" s="8">
+        <v>603791</v>
+      </c>
+      <c r="M16" s="8">
+        <v>89328</v>
+      </c>
+      <c r="N16" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="D17" s="8">
+        <v>46899</v>
+      </c>
+      <c r="E17" s="8">
+        <v>4622404941</v>
+      </c>
+      <c r="F17" s="13">
+        <v>45093</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="I17" s="11">
+        <v>0.87970000000000004</v>
+      </c>
+      <c r="J17" s="10">
+        <v>12.01</v>
+      </c>
+      <c r="K17" s="8">
+        <v>1034459</v>
+      </c>
+      <c r="L17" s="8">
+        <v>1048890</v>
+      </c>
+      <c r="M17" s="8">
+        <v>143457</v>
+      </c>
+      <c r="N17" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="D18" s="8">
+        <v>40275</v>
+      </c>
+      <c r="E18" s="8">
+        <v>9428770159</v>
+      </c>
+      <c r="F18" s="13">
+        <v>44342</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="I18" s="11">
+        <v>0.82550000000000001</v>
+      </c>
+      <c r="J18" s="10">
+        <v>12.38</v>
+      </c>
+      <c r="K18" s="8">
+        <v>4162685</v>
+      </c>
+      <c r="L18" s="8">
+        <v>2137325</v>
+      </c>
+      <c r="M18" s="8">
+        <v>451817</v>
+      </c>
+      <c r="N18" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="D19" s="8">
+        <v>35555</v>
+      </c>
+      <c r="E19" s="8">
+        <v>2243243879</v>
+      </c>
+      <c r="F19" s="13">
+        <v>43484</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="I19" s="11">
+        <v>0.91549999999999998</v>
+      </c>
+      <c r="J19" s="10">
+        <v>19.98</v>
+      </c>
+      <c r="K19" s="8">
+        <v>4727904</v>
+      </c>
+      <c r="L19" s="8">
+        <v>1602909</v>
+      </c>
+      <c r="M19" s="8">
+        <v>147956</v>
+      </c>
+      <c r="N19" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="D20" s="8">
+        <v>34846</v>
+      </c>
+      <c r="E20" s="8">
+        <v>206195841</v>
+      </c>
+      <c r="F20" s="13">
+        <v>45437</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="I20" s="11">
+        <v>0.95740000000000003</v>
+      </c>
+      <c r="J20" s="10">
+        <v>5.76</v>
+      </c>
+      <c r="K20" s="8">
+        <v>3748540</v>
+      </c>
+      <c r="L20" s="8">
+        <v>1002545</v>
+      </c>
+      <c r="M20" s="8">
+        <v>44584</v>
+      </c>
+      <c r="N20" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="D21" s="8">
+        <v>34765</v>
+      </c>
+      <c r="E21" s="8">
+        <v>847720685</v>
+      </c>
+      <c r="F21" s="13">
+        <v>45111</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="I21" s="11">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="J21" s="10">
+        <v>17.7</v>
+      </c>
+      <c r="K21" s="8">
+        <v>1583909</v>
+      </c>
+      <c r="L21" s="8">
+        <v>346765</v>
+      </c>
+      <c r="M21" s="8">
+        <v>26495</v>
+      </c>
+      <c r="N21" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="D22" s="8">
+        <v>33267</v>
+      </c>
+      <c r="E22" s="8">
+        <v>440360013</v>
+      </c>
+      <c r="F22" s="13">
+        <v>45121</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="I22" s="11">
+        <v>0.81440000000000001</v>
+      </c>
+      <c r="J22" s="10">
+        <v>33.47</v>
+      </c>
+      <c r="K22" s="8">
+        <v>313805</v>
+      </c>
+      <c r="L22" s="8">
+        <v>232015</v>
+      </c>
+      <c r="M22" s="8">
+        <v>52868</v>
+      </c>
+      <c r="N22" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="D23" s="8">
+        <v>30481</v>
+      </c>
+      <c r="E23" s="8">
+        <v>550145560</v>
+      </c>
+      <c r="F23" s="13">
+        <v>44667</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="I23" s="11">
+        <v>0.84819999999999995</v>
+      </c>
+      <c r="J23" s="10">
+        <v>12.38</v>
+      </c>
+      <c r="K23" s="8">
+        <v>710845</v>
+      </c>
+      <c r="L23" s="8">
+        <v>529357</v>
+      </c>
+      <c r="M23" s="8">
+        <v>94712</v>
+      </c>
+      <c r="N23" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="D24" s="8">
+        <v>29947</v>
+      </c>
+      <c r="E24" s="8">
+        <v>2577901716</v>
+      </c>
+      <c r="F24" s="13">
+        <v>44379</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="I24" s="11">
+        <v>0.91500000000000004</v>
+      </c>
+      <c r="J24" s="10">
+        <v>11.38</v>
+      </c>
+      <c r="K24" s="8">
+        <v>3247136</v>
+      </c>
+      <c r="L24" s="8">
+        <v>1258102</v>
+      </c>
+      <c r="M24" s="8">
+        <v>116815</v>
+      </c>
+      <c r="N24" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="D25" s="8">
+        <v>29798</v>
+      </c>
+      <c r="E25" s="8">
+        <v>334086190</v>
+      </c>
+      <c r="F25" s="13">
+        <v>45008</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="I25" s="11">
+        <v>0.92359999999999998</v>
+      </c>
+      <c r="J25" s="10">
+        <v>23.27</v>
+      </c>
+      <c r="K25" s="8">
+        <v>211965</v>
+      </c>
+      <c r="L25" s="8">
+        <v>225813</v>
+      </c>
+      <c r="M25" s="8">
+        <v>18688</v>
+      </c>
+      <c r="N25" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>398</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D26" s="8">
+        <v>29567</v>
+      </c>
+      <c r="E26" s="8">
+        <v>912659603</v>
+      </c>
+      <c r="F26" s="13">
+        <v>45337</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="I26" s="11">
+        <v>0.91830000000000001</v>
+      </c>
+      <c r="J26" s="10">
+        <v>10.25</v>
+      </c>
+      <c r="K26" s="8">
+        <v>1095641</v>
+      </c>
+      <c r="L26" s="8">
+        <v>1355724</v>
+      </c>
+      <c r="M26" s="8">
+        <v>120620</v>
+      </c>
+      <c r="N26" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="D27" s="8">
+        <v>29444</v>
+      </c>
+      <c r="E27" s="8">
+        <v>9120038</v>
+      </c>
+      <c r="F27" s="13">
+        <v>45394</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="I27" s="11">
+        <v>0.91759999999999997</v>
+      </c>
+      <c r="J27" s="10">
+        <v>14.08</v>
+      </c>
+      <c r="K27" s="8">
+        <v>208421</v>
+      </c>
+      <c r="L27" s="8">
+        <v>81922</v>
+      </c>
+      <c r="M27" s="8">
+        <v>7354</v>
+      </c>
+      <c r="N27" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="D28" s="8">
+        <v>29423</v>
+      </c>
+      <c r="E28" s="8">
+        <v>3955156207</v>
+      </c>
+      <c r="F28" s="13">
+        <v>42675</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="I28" s="11">
+        <v>0.93069999999999997</v>
+      </c>
+      <c r="J28" s="10">
+        <v>19.02</v>
+      </c>
+      <c r="K28" s="8">
+        <v>7551818</v>
+      </c>
+      <c r="L28" s="8">
+        <v>2981466</v>
+      </c>
+      <c r="M28" s="8">
+        <v>222167</v>
+      </c>
+      <c r="N28" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>374</v>
+      </c>
+      <c r="D29" s="8">
+        <v>28121</v>
+      </c>
+      <c r="E29" s="8">
+        <v>407804993</v>
+      </c>
+      <c r="F29" s="13">
+        <v>45026</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="I29" s="11">
+        <v>0.82889999999999997</v>
+      </c>
+      <c r="J29" s="10">
+        <v>11.61</v>
+      </c>
+      <c r="K29" s="8">
+        <v>663850</v>
+      </c>
+      <c r="L29" s="8">
+        <v>359443</v>
+      </c>
+      <c r="M29" s="8">
+        <v>74217</v>
+      </c>
+      <c r="N29" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="D30" s="8">
+        <v>27623</v>
+      </c>
+      <c r="E30" s="8">
+        <v>124135620</v>
+      </c>
+      <c r="F30" s="13">
+        <v>45292</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="I30" s="11">
+        <v>0.91369999999999996</v>
+      </c>
+      <c r="J30" s="10">
+        <v>14.45</v>
+      </c>
+      <c r="K30" s="8">
+        <v>134243</v>
+      </c>
+      <c r="L30" s="8">
+        <v>98859</v>
+      </c>
+      <c r="M30" s="8">
+        <v>9342</v>
+      </c>
+      <c r="N30" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="D31" s="8">
+        <v>25245</v>
+      </c>
+      <c r="E31" s="8">
+        <v>68886119</v>
+      </c>
+      <c r="F31" s="13">
+        <v>44963</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="I31" s="11">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="J31" s="10">
+        <v>14.01</v>
+      </c>
+      <c r="K31" s="8">
+        <v>641595</v>
+      </c>
+      <c r="L31" s="8">
+        <v>231244</v>
+      </c>
+      <c r="M31" s="8">
+        <v>11138</v>
+      </c>
+      <c r="N31" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="D32" s="8">
+        <v>24034</v>
+      </c>
+      <c r="E32" s="8">
+        <v>864013068</v>
+      </c>
+      <c r="F32" s="13">
+        <v>44006</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="I32" s="11">
+        <v>0.89570000000000005</v>
+      </c>
+      <c r="J32" s="10"/>
+      <c r="K32" s="8">
+        <v>2677302</v>
+      </c>
+      <c r="L32" s="8">
+        <v>580917</v>
+      </c>
+      <c r="M32" s="8">
+        <v>67667</v>
+      </c>
+      <c r="N32" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="D33" s="8">
+        <v>23845</v>
+      </c>
+      <c r="E33" s="8">
+        <v>856737169</v>
+      </c>
+      <c r="F33" s="13">
+        <v>45018</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="I33" s="11">
+        <v>0.87060000000000004</v>
+      </c>
+      <c r="J33" s="10">
+        <v>16.21</v>
+      </c>
+      <c r="K33" s="8">
+        <v>18043544</v>
+      </c>
+      <c r="L33" s="8">
+        <v>149104</v>
+      </c>
+      <c r="M33" s="8">
+        <v>22161</v>
+      </c>
+      <c r="N33" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="D34" s="8">
+        <v>23230</v>
+      </c>
+      <c r="E34" s="8">
+        <v>2603132490</v>
+      </c>
+      <c r="F34" s="13">
+        <v>44596</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="I34" s="11">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="J34" s="10">
+        <v>8.92</v>
+      </c>
+      <c r="K34" s="8">
+        <v>2922823</v>
+      </c>
+      <c r="L34" s="8">
+        <v>2117586</v>
+      </c>
+      <c r="M34" s="8">
+        <v>161832</v>
+      </c>
+      <c r="N34" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="D35" s="8">
+        <v>21911</v>
+      </c>
+      <c r="E35" s="8">
+        <v>8849277751</v>
+      </c>
+      <c r="F35" s="13">
+        <v>41946</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="I35" s="11">
+        <v>0.88109999999999999</v>
+      </c>
+      <c r="J35" s="10">
+        <v>21.51</v>
+      </c>
+      <c r="K35" s="8">
+        <v>13490134</v>
+      </c>
+      <c r="L35" s="8">
+        <v>5249152</v>
+      </c>
+      <c r="M35" s="8">
+        <v>708401</v>
+      </c>
+      <c r="N35" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="D36" s="8">
+        <v>21358</v>
+      </c>
+      <c r="E36" s="8">
+        <v>2211316216</v>
+      </c>
+      <c r="F36" s="13">
+        <v>44242</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I36" s="11">
+        <v>0.85409999999999997</v>
+      </c>
+      <c r="J36" s="10">
+        <v>10.68</v>
+      </c>
+      <c r="K36" s="8">
+        <v>2068434</v>
+      </c>
+      <c r="L36" s="8">
+        <v>1360495</v>
+      </c>
+      <c r="M36" s="8">
+        <v>232457</v>
+      </c>
+      <c r="N36" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="D37" s="8">
+        <v>20807</v>
+      </c>
+      <c r="E37" s="8">
+        <v>252357525</v>
+      </c>
+      <c r="F37" s="13">
+        <v>45421</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="H37" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I37" s="11">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="J37" s="10">
+        <v>21.48</v>
+      </c>
+      <c r="K37" s="8">
+        <v>3708210</v>
+      </c>
+      <c r="L37" s="8">
+        <v>886330</v>
+      </c>
+      <c r="M37" s="8">
+        <v>19896</v>
+      </c>
+      <c r="N37" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="D38" s="8">
+        <v>20450</v>
+      </c>
+      <c r="E38" s="8">
+        <v>7001831149</v>
+      </c>
+      <c r="F38" s="13">
+        <v>42740</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H38" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="I38" s="11">
+        <v>0.878</v>
+      </c>
+      <c r="J38" s="10">
+        <v>12.61</v>
+      </c>
+      <c r="K38" s="8">
+        <v>18212754</v>
+      </c>
+      <c r="L38" s="8">
+        <v>5483397</v>
+      </c>
+      <c r="M38" s="8">
+        <v>761678</v>
+      </c>
+      <c r="N38" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A39" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>407</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="D39" s="8">
+        <v>20381</v>
+      </c>
+      <c r="E39" s="8">
+        <v>4587298919</v>
+      </c>
+      <c r="F39" s="13">
+        <v>44313</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="I39" s="11">
+        <v>0.90239999999999998</v>
+      </c>
+      <c r="J39" s="10">
+        <v>14.57</v>
+      </c>
+      <c r="K39" s="8">
+        <v>22361103</v>
+      </c>
+      <c r="L39" s="8">
+        <v>1237131</v>
+      </c>
+      <c r="M39" s="8">
+        <v>133780</v>
+      </c>
+      <c r="N39" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="D40" s="8">
+        <v>20191</v>
+      </c>
+      <c r="E40" s="8">
+        <v>709463954</v>
+      </c>
+      <c r="F40" s="13">
+        <v>43984</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H40" s="10" t="s">
+        <v>409</v>
+      </c>
+      <c r="I40" s="11">
+        <v>0.84850000000000003</v>
+      </c>
+      <c r="J40" s="10">
+        <v>26.5</v>
+      </c>
+      <c r="K40" s="8">
+        <v>1235600</v>
+      </c>
+      <c r="L40" s="8">
+        <v>725694</v>
+      </c>
+      <c r="M40" s="8">
+        <v>129618</v>
+      </c>
+      <c r="N40" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="D41" s="8">
+        <v>19653</v>
+      </c>
+      <c r="E41" s="8">
+        <v>5146301778</v>
+      </c>
+      <c r="F41" s="13">
+        <v>44268</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H41" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="I41" s="11">
+        <v>0.93369999999999997</v>
+      </c>
+      <c r="J41" s="10">
+        <v>7.78</v>
+      </c>
+      <c r="K41" s="8">
+        <v>6308714</v>
+      </c>
+      <c r="L41" s="8">
+        <v>3550706</v>
+      </c>
+      <c r="M41" s="8">
+        <v>252035</v>
+      </c>
+      <c r="N41" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A42" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="D42" s="8">
+        <v>19145</v>
+      </c>
+      <c r="E42" s="8">
+        <v>23590509797</v>
+      </c>
+      <c r="F42" s="13">
+        <v>43268</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="I42" s="11">
+        <v>0.7419</v>
+      </c>
+      <c r="J42" s="10">
+        <v>4.3099999999999996</v>
+      </c>
+      <c r="K42" s="8">
+        <v>11125392</v>
+      </c>
+      <c r="L42" s="8">
+        <v>3822797</v>
+      </c>
+      <c r="M42" s="8">
+        <v>1330192</v>
+      </c>
+      <c r="N42" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="D43" s="8">
+        <v>18158</v>
+      </c>
+      <c r="E43" s="8">
+        <v>895402335</v>
+      </c>
+      <c r="F43" s="13">
+        <v>44958</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H43" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="I43" s="11">
+        <v>0.84260000000000002</v>
+      </c>
+      <c r="J43" s="10">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="K43" s="8">
+        <v>598054</v>
+      </c>
+      <c r="L43" s="8">
+        <v>257808</v>
+      </c>
+      <c r="M43" s="8">
+        <v>48169</v>
+      </c>
+      <c r="N43" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A44" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>410</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>384</v>
+      </c>
+      <c r="D44" s="8">
+        <v>17370</v>
+      </c>
+      <c r="E44" s="8">
+        <v>935370141</v>
+      </c>
+      <c r="F44" s="13">
+        <v>43661</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H44" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="I44" s="11">
+        <v>0.91859999999999997</v>
+      </c>
+      <c r="J44" s="10">
+        <v>16.41</v>
+      </c>
+      <c r="K44" s="8">
+        <v>5348533</v>
+      </c>
+      <c r="L44" s="8">
+        <v>680091</v>
+      </c>
+      <c r="M44" s="8">
+        <v>60298</v>
+      </c>
+      <c r="N44" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="D45" s="8">
+        <v>16976</v>
+      </c>
+      <c r="E45" s="8">
+        <v>12938613960</v>
+      </c>
+      <c r="F45" s="13">
+        <v>43852</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="I45" s="11">
+        <v>0.89910000000000001</v>
+      </c>
+      <c r="J45" s="10">
+        <v>10.02</v>
+      </c>
+      <c r="K45" s="8">
+        <v>11608902</v>
+      </c>
+      <c r="L45" s="8">
+        <v>3563160</v>
+      </c>
+      <c r="M45" s="8">
+        <v>399818</v>
+      </c>
+      <c r="N45" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A46" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="D46" s="8">
+        <v>16745</v>
+      </c>
+      <c r="E46" s="8">
+        <v>695191851</v>
+      </c>
+      <c r="F46" s="13">
+        <v>45206</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="H46" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="I46" s="11">
+        <v>0.96550000000000002</v>
+      </c>
+      <c r="J46" s="10">
+        <v>12.93</v>
+      </c>
+      <c r="K46" s="8">
+        <v>965144</v>
+      </c>
+      <c r="L46" s="8">
+        <v>1963760</v>
+      </c>
+      <c r="M46" s="8">
+        <v>70150</v>
+      </c>
+      <c r="N46" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="D47" s="8">
+        <v>16378</v>
+      </c>
+      <c r="E47" s="8">
+        <v>562042977</v>
+      </c>
+      <c r="F47" s="13">
+        <v>45078</v>
+      </c>
+      <c r="G47" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H47" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="I47" s="11">
+        <v>0.85589999999999999</v>
+      </c>
+      <c r="J47" s="10">
+        <v>11.54</v>
+      </c>
+      <c r="K47" s="8">
+        <v>713958</v>
+      </c>
+      <c r="L47" s="8">
+        <v>632091</v>
+      </c>
+      <c r="M47" s="8">
+        <v>106416</v>
+      </c>
+      <c r="N47" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A48" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>382</v>
+      </c>
+      <c r="D48" s="8">
+        <v>16164</v>
+      </c>
+      <c r="E48" s="8">
+        <v>458308791</v>
+      </c>
+      <c r="F48" s="13">
+        <v>45253</v>
+      </c>
+      <c r="G48" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="H48" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="I48" s="11">
+        <v>0.93589999999999995</v>
+      </c>
+      <c r="J48" s="10">
+        <v>9.5299999999999994</v>
+      </c>
+      <c r="K48" s="8">
+        <v>1805821</v>
+      </c>
+      <c r="L48" s="8">
+        <v>383046</v>
+      </c>
+      <c r="M48" s="8">
+        <v>26229</v>
+      </c>
+      <c r="N48" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A49" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>366</v>
+      </c>
+      <c r="D49" s="8">
+        <v>15999</v>
+      </c>
+      <c r="E49" s="8">
+        <v>3067244417</v>
+      </c>
+      <c r="F49" s="13">
+        <v>43815</v>
+      </c>
+      <c r="G49" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H49" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="I49" s="11">
+        <v>0.90780000000000005</v>
+      </c>
+      <c r="J49" s="10">
+        <v>15.67</v>
+      </c>
+      <c r="K49" s="8">
+        <v>2252251</v>
+      </c>
+      <c r="L49" s="8">
+        <v>1301166</v>
+      </c>
+      <c r="M49" s="8">
+        <v>132209</v>
+      </c>
+      <c r="N49" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A50" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>413</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="D50" s="8">
+        <v>15893</v>
+      </c>
+      <c r="E50" s="8">
+        <v>2593917649</v>
+      </c>
+      <c r="F50" s="13">
+        <v>44593</v>
+      </c>
+      <c r="G50" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H50" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="I50" s="11">
+        <v>0.58179999999999998</v>
+      </c>
+      <c r="J50" s="10">
+        <v>6.73</v>
+      </c>
+      <c r="K50" s="8">
+        <v>1144381</v>
+      </c>
+      <c r="L50" s="8">
+        <v>264091</v>
+      </c>
+      <c r="M50" s="8">
+        <v>189839</v>
+      </c>
+      <c r="N50" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A51" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="D51" s="8">
+        <v>15826</v>
+      </c>
+      <c r="E51" s="8">
+        <v>1015792775</v>
+      </c>
+      <c r="F51" s="13">
+        <v>44362</v>
+      </c>
+      <c r="G51" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="H51" s="10" t="s">
+        <v>414</v>
+      </c>
+      <c r="I51" s="11">
+        <v>0.77239999999999998</v>
+      </c>
+      <c r="J51" s="10">
+        <v>12.15</v>
+      </c>
+      <c r="K51" s="8">
+        <v>1563576</v>
+      </c>
+      <c r="L51" s="8">
+        <v>483571</v>
+      </c>
+      <c r="M51" s="8">
+        <v>142484</v>
+      </c>
+      <c r="N51" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A52" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="D52" s="8">
+        <v>15762</v>
+      </c>
+      <c r="E52" s="8">
+        <v>3582992131</v>
+      </c>
+      <c r="F52" s="13">
+        <v>44513</v>
+      </c>
+      <c r="G52" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H52" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="I52" s="11">
+        <v>0.82399999999999995</v>
+      </c>
+      <c r="J52" s="10">
+        <v>6.86</v>
+      </c>
+      <c r="K52" s="8">
+        <v>3132724</v>
+      </c>
+      <c r="L52" s="8">
+        <v>1281154</v>
+      </c>
+      <c r="M52" s="8">
+        <v>273622</v>
+      </c>
+      <c r="N52" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:N1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B5663F-5CC2-A347-8216-F8FF4AE5954D}">
   <dimension ref="A1:N52"/>
   <sheetViews>
@@ -1634,22 +4005,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>287</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
@@ -3900,7 +6271,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99C60782-7F66-D04D-A716-667EE5D461B9}">
   <dimension ref="A1:N50"/>
   <sheetViews>
@@ -3924,22 +6295,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>286</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
@@ -6105,7 +8476,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B937581-5BFE-0C43-9A8A-CAE8581C0F34}">
   <dimension ref="A1:N51"/>
   <sheetViews>
@@ -6129,22 +8500,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>233</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
@@ -8354,11 +10725,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D4922F-A22D-1547-8F5C-336FD651258D}">
   <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -8378,22 +10749,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
@@ -10603,7 +12974,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N50"/>
   <sheetViews>
@@ -10630,22 +13001,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>209</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
@@ -12811,7 +15182,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CD5A4D4-8172-B14E-80EB-29CD406E771F}">
   <dimension ref="A1:N51"/>
   <sheetViews>

</xml_diff>

<commit_message>
aug 19 data push
</commit_message>
<xml_diff>
--- a/data/total_roblox_experiences.xlsx
+++ b/data/total_roblox_experiences.xlsx
@@ -1,32 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/helenwang/Desktop/Makers/Steam_Roblox_Streamlit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2681867F-FD93-484D-977F-0E3CE0EA4C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BB51F7-35D5-F04E-B511-9A9F70E6CA83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5840" yWindow="1100" windowWidth="23460" windowHeight="18020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2024-08-12" sheetId="7" r:id="rId1"/>
-    <sheet name="2024-08-05" sheetId="6" r:id="rId2"/>
-    <sheet name="2024-07-29" sheetId="5" r:id="rId3"/>
-    <sheet name="2024-07-22" sheetId="4" r:id="rId4"/>
-    <sheet name="2024-07-09" sheetId="3" r:id="rId5"/>
-    <sheet name="2024-07-01" sheetId="1" r:id="rId6"/>
-    <sheet name="2024-06-20" sheetId="2" r:id="rId7"/>
+    <sheet name="2024-08-19" sheetId="8" r:id="rId1"/>
+    <sheet name="2024-08-12" sheetId="7" r:id="rId2"/>
+    <sheet name="2024-08-05" sheetId="6" r:id="rId3"/>
+    <sheet name="2024-07-29" sheetId="5" r:id="rId4"/>
+    <sheet name="2024-07-22" sheetId="4" r:id="rId5"/>
+    <sheet name="2024-07-09" sheetId="3" r:id="rId6"/>
+    <sheet name="2024-07-01" sheetId="1" r:id="rId7"/>
+    <sheet name="2024-06-20" sheetId="2" r:id="rId8"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1820" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2085" uniqueCount="446">
   <si>
     <t>#1</t>
   </si>
@@ -1277,6 +1278,93 @@
   </si>
   <si>
     <t>/experience/5130598377/</t>
+  </si>
+  <si>
+    <t>Top Experiences 50 on Roblox (Data fetched from RoMonitor as of 12:21 PM EDT, 2024-08-19)</t>
+  </si>
+  <si>
+    <t>Dress To Impress 💚</t>
+  </si>
+  <si>
+    <t>Pet Simulator 99! 🔥🎲</t>
+  </si>
+  <si>
+    <t>[5 DAYS] Anime Defenders</t>
+  </si>
+  <si>
+    <t>LifeTogether 🏠 RP (UPDATE 24)</t>
+  </si>
+  <si>
+    <t>BedWars [🎭SEASON 11]</t>
+  </si>
+  <si>
+    <t>[📊 TRADE + JJK UPD] Anime Last Stand</t>
+  </si>
+  <si>
+    <t>[🍔FOOD CRATE] Toilet Tower Defense</t>
+  </si>
+  <si>
+    <t>@ItsMuneeeb</t>
+  </si>
+  <si>
+    <t>Five Nights TD [SEASON]</t>
+  </si>
+  <si>
+    <t>a dusty trip [🚚BOSS]</t>
+  </si>
+  <si>
+    <t>[FIXES] Realm Rampage</t>
+  </si>
+  <si>
+    <t>Gym League [UPD7 + 2x💰]</t>
+  </si>
+  <si>
+    <t>🍓Dandy's World [ALPHA]</t>
+  </si>
+  <si>
+    <t>[SUPPORT] Anime Card Battle</t>
+  </si>
+  <si>
+    <t>Kung Fu Cat Panda Pepper</t>
+  </si>
+  <si>
+    <t>🌊 Creatures of Sonaria 💀 Survive Kaiju Animals</t>
+  </si>
+  <si>
+    <t>@haz3mn</t>
+  </si>
+  <si>
+    <t>[💧UPDATE] Slap Battles👏</t>
+  </si>
+  <si>
+    <t>[LAMBORGHINI] Driving Empire 🏎️ Car Racing</t>
+  </si>
+  <si>
+    <t>Livetopia🏠 New house</t>
+  </si>
+  <si>
+    <t>[UPD🐰] Baddies 💅</t>
+  </si>
+  <si>
+    <t>Emergency Hamburg</t>
+  </si>
+  <si>
+    <t>[☢️AURAS UPDATE] Anime Simulator</t>
+  </si>
+  <si>
+    <t>Bick Boizz</t>
+  </si>
+  <si>
+    <t>/experience/18138547215/</t>
+  </si>
+  <si>
+    <t>/experience/6081130554/</t>
+  </si>
+  <si>
+    <t>/experience/7711635737/</t>
+  </si>
+  <si>
+    <t>/experience/17316900493/</t>
   </si>
 </sst>
 </file>
@@ -1700,10 +1788,2293 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD668D3A-F99A-DC40-BB77-DFA426FE76BE}">
+  <dimension ref="A1:N52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>417</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="D3" s="8">
+        <v>661255</v>
+      </c>
+      <c r="E3" s="8">
+        <v>38293132790</v>
+      </c>
+      <c r="F3" s="13">
+        <v>43480</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="I3" s="11">
+        <v>0.92849999999999999</v>
+      </c>
+      <c r="J3" s="10">
+        <v>15.87</v>
+      </c>
+      <c r="K3" s="8">
+        <v>13000225</v>
+      </c>
+      <c r="L3" s="8">
+        <v>8013446</v>
+      </c>
+      <c r="M3" s="8">
+        <v>616742</v>
+      </c>
+      <c r="N3" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="D4" s="8">
+        <v>572756</v>
+      </c>
+      <c r="E4" s="8">
+        <v>52762394400</v>
+      </c>
+      <c r="F4" s="13">
+        <v>43941</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="I4" s="11">
+        <v>0.86570000000000003</v>
+      </c>
+      <c r="J4" s="10">
+        <v>15.27</v>
+      </c>
+      <c r="K4" s="8">
+        <v>21624873</v>
+      </c>
+      <c r="L4" s="8">
+        <v>5863583</v>
+      </c>
+      <c r="M4" s="8">
+        <v>909868</v>
+      </c>
+      <c r="N4" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>418</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="D5" s="8">
+        <v>261761</v>
+      </c>
+      <c r="E5" s="8">
+        <v>2070336679</v>
+      </c>
+      <c r="F5" s="13">
+        <v>45216</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="I5" s="11">
+        <v>0.91669999999999996</v>
+      </c>
+      <c r="J5" s="10">
+        <v>14.13</v>
+      </c>
+      <c r="K5" s="8">
+        <v>2000462</v>
+      </c>
+      <c r="L5" s="8">
+        <v>1202768</v>
+      </c>
+      <c r="M5" s="8">
+        <v>109249</v>
+      </c>
+      <c r="N5" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>419</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="D6" s="8">
+        <v>243973</v>
+      </c>
+      <c r="E6" s="8">
+        <v>1366256320</v>
+      </c>
+      <c r="F6" s="13">
+        <v>44596</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="I6" s="11">
+        <v>0.96240000000000003</v>
+      </c>
+      <c r="J6" s="10">
+        <v>55.29</v>
+      </c>
+      <c r="K6" s="8">
+        <v>1388603</v>
+      </c>
+      <c r="L6" s="8">
+        <v>2452052</v>
+      </c>
+      <c r="M6" s="8">
+        <v>95928</v>
+      </c>
+      <c r="N6" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="D7" s="8">
+        <v>226860</v>
+      </c>
+      <c r="E7" s="8">
+        <v>16859862892</v>
+      </c>
+      <c r="F7" s="13">
+        <v>41656</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="I7" s="11">
+        <v>0.91149999999999998</v>
+      </c>
+      <c r="J7" s="10">
+        <v>11.92</v>
+      </c>
+      <c r="K7" s="8">
+        <v>18796395</v>
+      </c>
+      <c r="L7" s="8">
+        <v>7636009</v>
+      </c>
+      <c r="M7" s="8">
+        <v>741477</v>
+      </c>
+      <c r="N7" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>420</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="D8" s="8">
+        <v>209129</v>
+      </c>
+      <c r="E8" s="8">
+        <v>1844458201</v>
+      </c>
+      <c r="F8" s="13">
+        <v>45386</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="I8" s="11">
+        <v>0.97460000000000002</v>
+      </c>
+      <c r="J8" s="10">
+        <v>11.83</v>
+      </c>
+      <c r="K8" s="8">
+        <v>598990</v>
+      </c>
+      <c r="L8" s="8">
+        <v>1742181</v>
+      </c>
+      <c r="M8" s="8">
+        <v>45342</v>
+      </c>
+      <c r="N8" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="D9" s="8">
+        <v>164278</v>
+      </c>
+      <c r="E9" s="8">
+        <v>7202814833</v>
+      </c>
+      <c r="F9" s="13">
+        <v>44774</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="I9" s="11">
+        <v>0.84050000000000002</v>
+      </c>
+      <c r="J9" s="10">
+        <v>9.75</v>
+      </c>
+      <c r="K9" s="8">
+        <v>3659652</v>
+      </c>
+      <c r="L9" s="8">
+        <v>2529143</v>
+      </c>
+      <c r="M9" s="8">
+        <v>479980</v>
+      </c>
+      <c r="N9" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="D10" s="8">
+        <v>153028</v>
+      </c>
+      <c r="E10" s="8">
+        <v>138064914</v>
+      </c>
+      <c r="F10" s="13">
+        <v>44758</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="I10" s="11">
+        <v>0.93720000000000003</v>
+      </c>
+      <c r="J10" s="10">
+        <v>17.739999999999998</v>
+      </c>
+      <c r="K10" s="8">
+        <v>136709</v>
+      </c>
+      <c r="L10" s="8">
+        <v>134817</v>
+      </c>
+      <c r="M10" s="8">
+        <v>9035</v>
+      </c>
+      <c r="N10" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="D11" s="8">
+        <v>133093</v>
+      </c>
+      <c r="E11" s="8">
+        <v>37143435614</v>
+      </c>
+      <c r="F11" s="13">
+        <v>42929</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="I11" s="11">
+        <v>0.83509999999999995</v>
+      </c>
+      <c r="J11" s="10"/>
+      <c r="K11" s="8">
+        <v>26889321</v>
+      </c>
+      <c r="L11" s="8">
+        <v>7225962</v>
+      </c>
+      <c r="M11" s="8">
+        <v>1426402</v>
+      </c>
+      <c r="N11" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="D12" s="8">
+        <v>93683</v>
+      </c>
+      <c r="E12" s="8">
+        <v>3997714560</v>
+      </c>
+      <c r="F12" s="13">
+        <v>44567</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="I12" s="11">
+        <v>0.87160000000000004</v>
+      </c>
+      <c r="J12" s="10">
+        <v>14.55</v>
+      </c>
+      <c r="K12" s="8">
+        <v>2158447</v>
+      </c>
+      <c r="L12" s="8">
+        <v>618003</v>
+      </c>
+      <c r="M12" s="8">
+        <v>91038</v>
+      </c>
+      <c r="N12" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="D13" s="8">
+        <v>91421</v>
+      </c>
+      <c r="E13" s="8">
+        <v>2861403147</v>
+      </c>
+      <c r="F13" s="13">
+        <v>43179</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="I13" s="11">
+        <v>0.94930000000000003</v>
+      </c>
+      <c r="J13" s="10">
+        <v>40.479999999999997</v>
+      </c>
+      <c r="K13" s="8">
+        <v>5914721</v>
+      </c>
+      <c r="L13" s="8">
+        <v>2269368</v>
+      </c>
+      <c r="M13" s="8">
+        <v>121091</v>
+      </c>
+      <c r="N13" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="D14" s="8">
+        <v>73819</v>
+      </c>
+      <c r="E14" s="8">
+        <v>664850108</v>
+      </c>
+      <c r="F14" s="13">
+        <v>45262</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="I14" s="11">
+        <v>0.87929999999999997</v>
+      </c>
+      <c r="J14" s="10">
+        <v>38.159999999999997</v>
+      </c>
+      <c r="K14" s="8">
+        <v>590463</v>
+      </c>
+      <c r="L14" s="8">
+        <v>668958</v>
+      </c>
+      <c r="M14" s="8">
+        <v>91816</v>
+      </c>
+      <c r="N14" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="D15" s="8">
+        <v>66819</v>
+      </c>
+      <c r="E15" s="8">
+        <v>4723650841</v>
+      </c>
+      <c r="F15" s="13">
+        <v>44721</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="I15" s="11">
+        <v>0.9446</v>
+      </c>
+      <c r="J15" s="10">
+        <v>10.210000000000001</v>
+      </c>
+      <c r="K15" s="8">
+        <v>5059560</v>
+      </c>
+      <c r="L15" s="8">
+        <v>1969503</v>
+      </c>
+      <c r="M15" s="8">
+        <v>115441</v>
+      </c>
+      <c r="N15" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="D16" s="8">
+        <v>58177</v>
+      </c>
+      <c r="E16" s="8">
+        <v>4173499400</v>
+      </c>
+      <c r="F16" s="13">
+        <v>45093</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="I16" s="11">
+        <v>0.93620000000000003</v>
+      </c>
+      <c r="J16" s="10">
+        <v>12.63</v>
+      </c>
+      <c r="K16" s="8">
+        <v>9453307</v>
+      </c>
+      <c r="L16" s="8">
+        <v>6196910</v>
+      </c>
+      <c r="M16" s="8">
+        <v>422626</v>
+      </c>
+      <c r="N16" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="D17" s="8">
+        <v>50073</v>
+      </c>
+      <c r="E17" s="8">
+        <v>290279675</v>
+      </c>
+      <c r="F17" s="13">
+        <v>45437</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="I17" s="11">
+        <v>0.95840000000000003</v>
+      </c>
+      <c r="J17" s="10">
+        <v>5.68</v>
+      </c>
+      <c r="K17" s="8">
+        <v>4932859</v>
+      </c>
+      <c r="L17" s="8">
+        <v>1246216</v>
+      </c>
+      <c r="M17" s="8">
+        <v>54111</v>
+      </c>
+      <c r="N17" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>421</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="D18" s="8">
+        <v>50000</v>
+      </c>
+      <c r="E18" s="8">
+        <v>876734369</v>
+      </c>
+      <c r="F18" s="13">
+        <v>45111</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="I18" s="11">
+        <v>0.92869999999999997</v>
+      </c>
+      <c r="J18" s="10">
+        <v>17.12</v>
+      </c>
+      <c r="K18" s="8">
+        <v>1856474</v>
+      </c>
+      <c r="L18" s="8">
+        <v>354655</v>
+      </c>
+      <c r="M18" s="8">
+        <v>27242</v>
+      </c>
+      <c r="N18" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>422</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="D19" s="8">
+        <v>49613</v>
+      </c>
+      <c r="E19" s="8">
+        <v>9468468915</v>
+      </c>
+      <c r="F19" s="13">
+        <v>44342</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="I19" s="11">
+        <v>0.82550000000000001</v>
+      </c>
+      <c r="J19" s="10">
+        <v>12.89</v>
+      </c>
+      <c r="K19" s="8">
+        <v>4168742</v>
+      </c>
+      <c r="L19" s="8">
+        <v>2144075</v>
+      </c>
+      <c r="M19" s="8">
+        <v>453118</v>
+      </c>
+      <c r="N19" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="D20" s="8">
+        <v>47160</v>
+      </c>
+      <c r="E20" s="8">
+        <v>350096139</v>
+      </c>
+      <c r="F20" s="13">
+        <v>45008</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="I20" s="11">
+        <v>0.92410000000000003</v>
+      </c>
+      <c r="J20" s="10">
+        <v>20.59</v>
+      </c>
+      <c r="K20" s="8">
+        <v>226449</v>
+      </c>
+      <c r="L20" s="8">
+        <v>235261</v>
+      </c>
+      <c r="M20" s="8">
+        <v>19319</v>
+      </c>
+      <c r="N20" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="D21" s="8">
+        <v>45935</v>
+      </c>
+      <c r="E21" s="8">
+        <v>4658096321</v>
+      </c>
+      <c r="F21" s="13">
+        <v>45093</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="I21" s="11">
+        <v>0.877</v>
+      </c>
+      <c r="J21" s="10">
+        <v>11.39</v>
+      </c>
+      <c r="K21" s="8">
+        <v>1038256</v>
+      </c>
+      <c r="L21" s="8">
+        <v>1054065</v>
+      </c>
+      <c r="M21" s="8">
+        <v>147767</v>
+      </c>
+      <c r="N21" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="D22" s="8">
+        <v>40414</v>
+      </c>
+      <c r="E22" s="8">
+        <v>584883409</v>
+      </c>
+      <c r="F22" s="13">
+        <v>44667</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="I22" s="11">
+        <v>0.84899999999999998</v>
+      </c>
+      <c r="J22" s="10">
+        <v>12.61</v>
+      </c>
+      <c r="K22" s="8">
+        <v>740193</v>
+      </c>
+      <c r="L22" s="8">
+        <v>555322</v>
+      </c>
+      <c r="M22" s="8">
+        <v>98754</v>
+      </c>
+      <c r="N22" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="D23" s="8">
+        <v>39031</v>
+      </c>
+      <c r="E23" s="8">
+        <v>2608404176</v>
+      </c>
+      <c r="F23" s="13">
+        <v>44379</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>425</v>
+      </c>
+      <c r="I23" s="11">
+        <v>0.91559999999999997</v>
+      </c>
+      <c r="J23" s="10">
+        <v>12.48</v>
+      </c>
+      <c r="K23" s="8">
+        <v>3268484</v>
+      </c>
+      <c r="L23" s="8">
+        <v>1275682</v>
+      </c>
+      <c r="M23" s="8">
+        <v>117629</v>
+      </c>
+      <c r="N23" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="D24" s="8">
+        <v>34738</v>
+      </c>
+      <c r="E24" s="8">
+        <v>148169313</v>
+      </c>
+      <c r="F24" s="13">
+        <v>45292</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="I24" s="11">
+        <v>0.91620000000000001</v>
+      </c>
+      <c r="J24" s="10">
+        <v>11.13</v>
+      </c>
+      <c r="K24" s="8">
+        <v>146331</v>
+      </c>
+      <c r="L24" s="8">
+        <v>109990</v>
+      </c>
+      <c r="M24" s="8">
+        <v>10061</v>
+      </c>
+      <c r="N24" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="D25" s="8">
+        <v>32885</v>
+      </c>
+      <c r="E25" s="8">
+        <v>452516901</v>
+      </c>
+      <c r="F25" s="13">
+        <v>45121</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="I25" s="11">
+        <v>0.81340000000000001</v>
+      </c>
+      <c r="J25" s="10">
+        <v>30.51</v>
+      </c>
+      <c r="K25" s="8">
+        <v>318385</v>
+      </c>
+      <c r="L25" s="8">
+        <v>235786</v>
+      </c>
+      <c r="M25" s="8">
+        <v>54087</v>
+      </c>
+      <c r="N25" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="D26" s="8">
+        <v>32576</v>
+      </c>
+      <c r="E26" s="8">
+        <v>3970608387</v>
+      </c>
+      <c r="F26" s="13">
+        <v>42675</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="I26" s="11">
+        <v>0.93069999999999997</v>
+      </c>
+      <c r="J26" s="10">
+        <v>19.239999999999998</v>
+      </c>
+      <c r="K26" s="8">
+        <v>7560651</v>
+      </c>
+      <c r="L26" s="8">
+        <v>2989677</v>
+      </c>
+      <c r="M26" s="8">
+        <v>222762</v>
+      </c>
+      <c r="N26" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="D27" s="8">
+        <v>31504</v>
+      </c>
+      <c r="E27" s="8">
+        <v>8866452658</v>
+      </c>
+      <c r="F27" s="13">
+        <v>41946</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="I27" s="11">
+        <v>0.88090000000000002</v>
+      </c>
+      <c r="J27" s="10">
+        <v>20.61</v>
+      </c>
+      <c r="K27" s="8">
+        <v>13502818</v>
+      </c>
+      <c r="L27" s="8">
+        <v>5256500</v>
+      </c>
+      <c r="M27" s="8">
+        <v>710418</v>
+      </c>
+      <c r="N27" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="D28" s="8">
+        <v>31472</v>
+      </c>
+      <c r="E28" s="8">
+        <v>2257165859</v>
+      </c>
+      <c r="F28" s="13">
+        <v>43484</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="I28" s="11">
+        <v>0.91549999999999998</v>
+      </c>
+      <c r="J28" s="10">
+        <v>20.12</v>
+      </c>
+      <c r="K28" s="8">
+        <v>4741103</v>
+      </c>
+      <c r="L28" s="8">
+        <v>1609164</v>
+      </c>
+      <c r="M28" s="8">
+        <v>148571</v>
+      </c>
+      <c r="N28" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>427</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="D29" s="8">
+        <v>30912</v>
+      </c>
+      <c r="E29" s="8">
+        <v>940722006</v>
+      </c>
+      <c r="F29" s="13">
+        <v>45337</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="I29" s="11">
+        <v>0.91800000000000004</v>
+      </c>
+      <c r="J29" s="10">
+        <v>10.46</v>
+      </c>
+      <c r="K29" s="8">
+        <v>1117372</v>
+      </c>
+      <c r="L29" s="8">
+        <v>1378419</v>
+      </c>
+      <c r="M29" s="8">
+        <v>123059</v>
+      </c>
+      <c r="N29" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>428</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="D30" s="8">
+        <v>28483</v>
+      </c>
+      <c r="E30" s="8">
+        <v>36772145</v>
+      </c>
+      <c r="F30" s="13">
+        <v>45394</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H30" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="I30" s="11">
+        <v>0.88319999999999999</v>
+      </c>
+      <c r="J30" s="10">
+        <v>13.22</v>
+      </c>
+      <c r="K30" s="8">
+        <v>361310</v>
+      </c>
+      <c r="L30" s="8">
+        <v>165726</v>
+      </c>
+      <c r="M30" s="8">
+        <v>21916</v>
+      </c>
+      <c r="N30" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="D31" s="8">
+        <v>28250</v>
+      </c>
+      <c r="E31" s="8">
+        <v>873565151</v>
+      </c>
+      <c r="F31" s="13">
+        <v>45018</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="I31" s="11">
+        <v>0.87109999999999999</v>
+      </c>
+      <c r="J31" s="10">
+        <v>17.36</v>
+      </c>
+      <c r="K31" s="8">
+        <v>18809771</v>
+      </c>
+      <c r="L31" s="8">
+        <v>152796</v>
+      </c>
+      <c r="M31" s="8">
+        <v>22616</v>
+      </c>
+      <c r="N31" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="D32" s="8">
+        <v>28182</v>
+      </c>
+      <c r="E32" s="8">
+        <v>88426330</v>
+      </c>
+      <c r="F32" s="13">
+        <v>44963</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="I32" s="11">
+        <v>0.95240000000000002</v>
+      </c>
+      <c r="J32" s="10">
+        <v>14.27</v>
+      </c>
+      <c r="K32" s="8">
+        <v>713133</v>
+      </c>
+      <c r="L32" s="8">
+        <v>270789</v>
+      </c>
+      <c r="M32" s="8">
+        <v>13539</v>
+      </c>
+      <c r="N32" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>429</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="D33" s="8">
+        <v>28174</v>
+      </c>
+      <c r="E33" s="8">
+        <v>264251878</v>
+      </c>
+      <c r="F33" s="13">
+        <v>45421</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I33" s="11">
+        <v>0.97770000000000001</v>
+      </c>
+      <c r="J33" s="10">
+        <v>17.98</v>
+      </c>
+      <c r="K33" s="8">
+        <v>3715277</v>
+      </c>
+      <c r="L33" s="8">
+        <v>895681</v>
+      </c>
+      <c r="M33" s="8">
+        <v>20467</v>
+      </c>
+      <c r="N33" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>430</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="D34" s="8">
+        <v>26461</v>
+      </c>
+      <c r="E34" s="8">
+        <v>93757882</v>
+      </c>
+      <c r="F34" s="13">
+        <v>45316</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="I34" s="11">
+        <v>0.92879999999999996</v>
+      </c>
+      <c r="J34" s="10">
+        <v>12.27</v>
+      </c>
+      <c r="K34" s="8">
+        <v>158953</v>
+      </c>
+      <c r="L34" s="8">
+        <v>79176</v>
+      </c>
+      <c r="M34" s="8">
+        <v>6071</v>
+      </c>
+      <c r="N34" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>431</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>442</v>
+      </c>
+      <c r="D35" s="8">
+        <v>26346</v>
+      </c>
+      <c r="E35" s="8">
+        <v>8159509</v>
+      </c>
+      <c r="F35" s="13">
+        <v>45463</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="H35" s="10" t="s">
+        <v>432</v>
+      </c>
+      <c r="I35" s="11">
+        <v>0.8861</v>
+      </c>
+      <c r="J35" s="10">
+        <v>32.049999999999997</v>
+      </c>
+      <c r="K35" s="8">
+        <v>24880</v>
+      </c>
+      <c r="L35" s="8">
+        <v>12457</v>
+      </c>
+      <c r="M35" s="8">
+        <v>1602</v>
+      </c>
+      <c r="N35" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="D36" s="8">
+        <v>26178</v>
+      </c>
+      <c r="E36" s="8">
+        <v>875557799</v>
+      </c>
+      <c r="F36" s="13">
+        <v>44006</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="H36" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="I36" s="11">
+        <v>0.89610000000000001</v>
+      </c>
+      <c r="J36" s="10">
+        <v>22.65</v>
+      </c>
+      <c r="K36" s="8">
+        <v>2736652</v>
+      </c>
+      <c r="L36" s="8">
+        <v>588628</v>
+      </c>
+      <c r="M36" s="8">
+        <v>68219</v>
+      </c>
+      <c r="N36" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="D37" s="8">
+        <v>25433</v>
+      </c>
+      <c r="E37" s="8">
+        <v>2628170130</v>
+      </c>
+      <c r="F37" s="13">
+        <v>44596</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="H37" s="10" t="s">
+        <v>434</v>
+      </c>
+      <c r="I37" s="11">
+        <v>0.92910000000000004</v>
+      </c>
+      <c r="J37" s="10">
+        <v>8.83</v>
+      </c>
+      <c r="K37" s="8">
+        <v>2939169</v>
+      </c>
+      <c r="L37" s="8">
+        <v>2136675</v>
+      </c>
+      <c r="M37" s="8">
+        <v>163031</v>
+      </c>
+      <c r="N37" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A38" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>342</v>
+      </c>
+      <c r="D38" s="8">
+        <v>23386</v>
+      </c>
+      <c r="E38" s="8">
+        <v>2233092158</v>
+      </c>
+      <c r="F38" s="13">
+        <v>44242</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H38" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="I38" s="11">
+        <v>0.85429999999999995</v>
+      </c>
+      <c r="J38" s="10">
+        <v>11.1</v>
+      </c>
+      <c r="K38" s="8">
+        <v>2078462</v>
+      </c>
+      <c r="L38" s="8">
+        <v>1371960</v>
+      </c>
+      <c r="M38" s="8">
+        <v>234023</v>
+      </c>
+      <c r="N38" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A39" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="D39" s="8">
+        <v>22850</v>
+      </c>
+      <c r="E39" s="8">
+        <v>7017720476</v>
+      </c>
+      <c r="F39" s="13">
+        <v>42740</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="I39" s="11">
+        <v>0.87809999999999999</v>
+      </c>
+      <c r="J39" s="10">
+        <v>13.94</v>
+      </c>
+      <c r="K39" s="8">
+        <v>18220741</v>
+      </c>
+      <c r="L39" s="8">
+        <v>5492648</v>
+      </c>
+      <c r="M39" s="8">
+        <v>762733</v>
+      </c>
+      <c r="N39" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A40" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>335</v>
+      </c>
+      <c r="D40" s="8">
+        <v>22719</v>
+      </c>
+      <c r="E40" s="8">
+        <v>1449308804</v>
+      </c>
+      <c r="F40" s="13">
+        <v>43638</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H40" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="I40" s="11">
+        <v>0.93140000000000001</v>
+      </c>
+      <c r="J40" s="10">
+        <v>11.63</v>
+      </c>
+      <c r="K40" s="8">
+        <v>11066817</v>
+      </c>
+      <c r="L40" s="8">
+        <v>1429235</v>
+      </c>
+      <c r="M40" s="8">
+        <v>105245</v>
+      </c>
+      <c r="N40" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="D41" s="8">
+        <v>22634</v>
+      </c>
+      <c r="E41" s="8">
+        <v>5170799691</v>
+      </c>
+      <c r="F41" s="13">
+        <v>44268</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H41" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="I41" s="11">
+        <v>0.93359999999999999</v>
+      </c>
+      <c r="J41" s="10">
+        <v>8.44</v>
+      </c>
+      <c r="K41" s="8">
+        <v>6328411</v>
+      </c>
+      <c r="L41" s="8">
+        <v>3563537</v>
+      </c>
+      <c r="M41" s="8">
+        <v>253289</v>
+      </c>
+      <c r="N41" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A42" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="D42" s="8">
+        <v>22383</v>
+      </c>
+      <c r="E42" s="8">
+        <v>12962773179</v>
+      </c>
+      <c r="F42" s="13">
+        <v>43852</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="I42" s="11">
+        <v>0.89910000000000001</v>
+      </c>
+      <c r="J42" s="10">
+        <v>10.130000000000001</v>
+      </c>
+      <c r="K42" s="8">
+        <v>11618249</v>
+      </c>
+      <c r="L42" s="8">
+        <v>3571158</v>
+      </c>
+      <c r="M42" s="8">
+        <v>400741</v>
+      </c>
+      <c r="N42" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>357</v>
+      </c>
+      <c r="D43" s="8">
+        <v>22348</v>
+      </c>
+      <c r="E43" s="8">
+        <v>916483913</v>
+      </c>
+      <c r="F43" s="13">
+        <v>44958</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H43" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="I43" s="11">
+        <v>0.84260000000000002</v>
+      </c>
+      <c r="J43" s="10">
+        <v>10.9</v>
+      </c>
+      <c r="K43" s="8">
+        <v>608298</v>
+      </c>
+      <c r="L43" s="8">
+        <v>263905</v>
+      </c>
+      <c r="M43" s="8">
+        <v>49298</v>
+      </c>
+      <c r="N43" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A44" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>437</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="D44" s="8">
+        <v>21998</v>
+      </c>
+      <c r="E44" s="8">
+        <v>4599922848</v>
+      </c>
+      <c r="F44" s="13">
+        <v>44313</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H44" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="I44" s="11">
+        <v>0.91269999999999996</v>
+      </c>
+      <c r="J44" s="10">
+        <v>13.81</v>
+      </c>
+      <c r="K44" s="8">
+        <v>22997282</v>
+      </c>
+      <c r="L44" s="8">
+        <v>1071735</v>
+      </c>
+      <c r="M44" s="8">
+        <v>102487</v>
+      </c>
+      <c r="N44" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="D45" s="8">
+        <v>21767</v>
+      </c>
+      <c r="E45" s="8">
+        <v>23638603845</v>
+      </c>
+      <c r="F45" s="13">
+        <v>43268</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="I45" s="11">
+        <v>0.74180000000000001</v>
+      </c>
+      <c r="J45" s="10">
+        <v>4.0599999999999996</v>
+      </c>
+      <c r="K45" s="8">
+        <v>11130990</v>
+      </c>
+      <c r="L45" s="8">
+        <v>3828190</v>
+      </c>
+      <c r="M45" s="8">
+        <v>1332831</v>
+      </c>
+      <c r="N45" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A46" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>438</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="D46" s="8">
+        <v>21311</v>
+      </c>
+      <c r="E46" s="8">
+        <v>158154455</v>
+      </c>
+      <c r="F46" s="13">
+        <v>44836</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H46" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="I46" s="11">
+        <v>0.74170000000000003</v>
+      </c>
+      <c r="J46" s="10">
+        <v>10.82</v>
+      </c>
+      <c r="K46" s="8">
+        <v>3576088</v>
+      </c>
+      <c r="L46" s="8">
+        <v>53075</v>
+      </c>
+      <c r="M46" s="8">
+        <v>18480</v>
+      </c>
+      <c r="N46" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>408</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>416</v>
+      </c>
+      <c r="D47" s="8">
+        <v>20531</v>
+      </c>
+      <c r="E47" s="8">
+        <v>718853979</v>
+      </c>
+      <c r="F47" s="13">
+        <v>43984</v>
+      </c>
+      <c r="G47" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="H47" s="10" t="s">
+        <v>409</v>
+      </c>
+      <c r="I47" s="11">
+        <v>0.85050000000000003</v>
+      </c>
+      <c r="J47" s="10">
+        <v>25.08</v>
+      </c>
+      <c r="K47" s="8">
+        <v>1245419</v>
+      </c>
+      <c r="L47" s="8">
+        <v>741345</v>
+      </c>
+      <c r="M47" s="8">
+        <v>130276</v>
+      </c>
+      <c r="N47" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A48" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="D48" s="8">
+        <v>19006</v>
+      </c>
+      <c r="E48" s="8">
+        <v>362430891</v>
+      </c>
+      <c r="F48" s="13">
+        <v>44480</v>
+      </c>
+      <c r="G48" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H48" s="10" t="s">
+        <v>439</v>
+      </c>
+      <c r="I48" s="11">
+        <v>0.84040000000000004</v>
+      </c>
+      <c r="J48" s="10">
+        <v>15.45</v>
+      </c>
+      <c r="K48" s="8">
+        <v>454134</v>
+      </c>
+      <c r="L48" s="8">
+        <v>177724</v>
+      </c>
+      <c r="M48" s="8">
+        <v>33764</v>
+      </c>
+      <c r="N48" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A49" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="D49" s="8">
+        <v>18986</v>
+      </c>
+      <c r="E49" s="8">
+        <v>3605567879</v>
+      </c>
+      <c r="F49" s="13">
+        <v>44513</v>
+      </c>
+      <c r="G49" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="H49" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="I49" s="11">
+        <v>0.82420000000000004</v>
+      </c>
+      <c r="J49" s="10">
+        <v>7.66</v>
+      </c>
+      <c r="K49" s="8">
+        <v>3140130</v>
+      </c>
+      <c r="L49" s="8">
+        <v>1285246</v>
+      </c>
+      <c r="M49" s="8">
+        <v>274132</v>
+      </c>
+      <c r="N49" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A50" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="D50" s="8">
+        <v>18434</v>
+      </c>
+      <c r="E50" s="8">
+        <v>2431995391</v>
+      </c>
+      <c r="F50" s="13">
+        <v>44016</v>
+      </c>
+      <c r="G50" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="H50" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="I50" s="11">
+        <v>0.75360000000000005</v>
+      </c>
+      <c r="J50" s="10">
+        <v>21.99</v>
+      </c>
+      <c r="K50" s="8">
+        <v>2410843</v>
+      </c>
+      <c r="L50" s="8">
+        <v>560123</v>
+      </c>
+      <c r="M50" s="8">
+        <v>183135</v>
+      </c>
+      <c r="N50" s="10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A51" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>440</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="D51" s="8">
+        <v>17804</v>
+      </c>
+      <c r="E51" s="8">
+        <v>4775842</v>
+      </c>
+      <c r="F51" s="13">
+        <v>45409</v>
+      </c>
+      <c r="G51" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="H51" s="10" t="s">
+        <v>441</v>
+      </c>
+      <c r="I51" s="11">
+        <v>0.97399999999999998</v>
+      </c>
+      <c r="J51" s="10">
+        <v>41.9</v>
+      </c>
+      <c r="K51" s="8">
+        <v>48878</v>
+      </c>
+      <c r="L51" s="8">
+        <v>42998</v>
+      </c>
+      <c r="M51" s="8">
+        <v>1147</v>
+      </c>
+      <c r="N51" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A52" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="D52" s="8">
+        <v>17340</v>
+      </c>
+      <c r="E52" s="8">
+        <v>707610288</v>
+      </c>
+      <c r="F52" s="13">
+        <v>45206</v>
+      </c>
+      <c r="G52" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="H52" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="I52" s="11">
+        <v>0.96550000000000002</v>
+      </c>
+      <c r="J52" s="10">
+        <v>12.84</v>
+      </c>
+      <c r="K52" s="8">
+        <v>976325</v>
+      </c>
+      <c r="L52" s="8">
+        <v>1982788</v>
+      </c>
+      <c r="M52" s="8">
+        <v>70866</v>
+      </c>
+      <c r="N52" s="10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:N1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09C3FBEA-4DAA-4D4C-B801-8F0A46D4D9A9}">
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+    <sheetView topLeftCell="A32" workbookViewId="0">
       <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
@@ -3981,7 +6352,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B5663F-5CC2-A347-8216-F8FF4AE5954D}">
   <dimension ref="A1:N52"/>
   <sheetViews>
@@ -6271,7 +8642,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99C60782-7F66-D04D-A716-667EE5D461B9}">
   <dimension ref="A1:N50"/>
   <sheetViews>
@@ -8476,7 +10847,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B937581-5BFE-0C43-9A8A-CAE8581C0F34}">
   <dimension ref="A1:N51"/>
   <sheetViews>
@@ -10725,7 +13096,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D4922F-A22D-1547-8F5C-336FD651258D}">
   <dimension ref="A1:N51"/>
   <sheetViews>
@@ -12974,7 +15345,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N50"/>
   <sheetViews>
@@ -15182,7 +17553,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CD5A4D4-8172-B14E-80EB-29CD406E771F}">
   <dimension ref="A1:N51"/>
   <sheetViews>

</xml_diff>